<commit_message>
Remoção de linhas inutilizadas
</commit_message>
<xml_diff>
--- a/prototipos/DataInput/Relatório.xlsx
+++ b/prototipos/DataInput/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E144"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Dados Brutos</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Dividas:</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -483,10 +488,15 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:
-TOTAL ORIGEM: 2.327,45 14,19 18,89 2.360,53</t>
+2.327,45 14,19 18,89 2.360,53 
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -513,10 +523,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:
-TOTAL ORIGEM: 2.327,45 14,19 18,89 2.360,53</t>
+2.327,45 14,19 18,89 2.360,53 
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -543,10 +558,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:
-TOTAL ORIGEM: 2.327,45 14,19 18,89 2.360,53</t>
+2.327,45 14,19 18,89 2.360,53 
+</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -573,10 +593,15 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:
-TOTAL ORIGEM: 2.327,45 14,19 18,89 2.360,53</t>
+2.327,45 14,19 18,89 2.360,53 
+</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -603,10 +628,15 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:
-TOTAL ORIGEM: 2.327,45 14,19 18,89 2.360,53</t>
+2.327,45 14,19 18,89 2.360,53 
+</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -633,10 +663,15 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:
-TOTAL ORIGEM: 3.109,60 4,63 18,44 3.132,67</t>
+3.109,60 4,63 18,44 3.132,67 
+</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -663,10 +698,15 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:
-TOTAL ORIGEM: 3.109,60 4,63 18,44 3.132,67</t>
+3.109,60 4,63 18,44 3.132,67 
+</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -693,10 +733,15 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:
-TOTAL ORIGEM: 3.109,60 4,63 18,44 3.132,67</t>
+3.109,60 4,63 18,44 3.132,67 
+</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -723,10 +768,15 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:
-TOTAL ORIGEM: 3.109,60 4,63 18,44 3.132,67</t>
+3.109,60 4,63 18,44 3.132,67 
+</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -753,10 +803,15 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:
-TOTAL ORIGEM: 3.109,60 4,63 18,44 3.132,67</t>
+3.109,60 4,63 18,44 3.132,67 
+</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -783,10 +838,15 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:
-TOTAL ORIGEM: 3.109,60 4,63 18,44 3.132,67</t>
+3.109,60 4,63 18,44 3.132,67 
+</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -813,11 +873,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -844,11 +909,16 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -875,11 +945,16 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -906,11 +981,16 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -937,10 +1017,15 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:
-TOTAL ORIGEM: 320,88 4,81 16,05 341,74</t>
+320,88 4,81 16,05 341,74 
+</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -967,10 +1052,15 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:
-TOTAL ORIGEM: 320,88 4,81 16,05 341,74</t>
+320,88 4,81 16,05 341,74 
+</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -997,10 +1087,15 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:
-TOTAL ORIGEM: 320,88 4,81 16,05 341,74</t>
+320,88 4,81 16,05 341,74 
+</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1027,10 +1122,15 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:
-TOTAL ORIGEM: 320,88 4,81 16,05 341,74</t>
+320,88 4,81 16,05 341,74 
+</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1057,10 +1157,15 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:
-TOTAL ORIGEM: 320,88 4,81 16,05 341,74</t>
+320,88 4,81 16,05 341,74 
+</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1087,10 +1192,15 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:
-TOTAL ORIGEM: 320,88 4,81 16,05 341,74</t>
+320,88 4,81 16,05 341,74 
+</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1117,11 +1227,16 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:
-TOTAL ORIGEM: 1.315,32 60,30 157,20 1.532,82</t>
+1.315,32 60,30 157,20 1.532,82 
+</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1148,11 +1263,16 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:
-TOTAL ORIGEM: 1.315,32 60,30 157,20 1.532,82</t>
+1.315,32 60,30 157,20 1.532,82 
+</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1179,11 +1299,16 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:
-TOTAL ORIGEM: 1.315,32 60,30 157,20 1.532,82</t>
+1.315,32 60,30 157,20 1.532,82 
+</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1210,11 +1335,16 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:
-TOTAL ORIGEM: 1.315,32 60,30 157,20 1.532,82</t>
+1.315,32 60,30 157,20 1.532,82 
+</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1241,11 +1371,16 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:
-TOTAL ORIGEM: 1.315,32 60,30 157,20 1.532,82</t>
+1.315,32 60,30 157,20 1.532,82 
+</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1272,11 +1407,16 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:
-TOTAL ORIGEM: 1.315,32 60,30 157,20 1.532,82</t>
+1.315,32 60,30 157,20 1.532,82 
+</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1303,11 +1443,16 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:
-TOTAL ORIGEM: 1.316,44 60,16 156,87 1.533,47</t>
+1.316,44 60,16 156,87 1.533,47 
+</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1334,11 +1479,16 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:
-TOTAL ORIGEM: 1.316,44 60,16 156,87 1.533,47</t>
+1.316,44 60,16 156,87 1.533,47 
+</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1365,11 +1515,16 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:
-TOTAL ORIGEM: 1.316,44 60,16 156,87 1.533,47</t>
+1.316,44 60,16 156,87 1.533,47 
+</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1396,11 +1551,16 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:
-TOTAL ORIGEM: 1.316,44 60,16 156,87 1.533,47</t>
+1.316,44 60,16 156,87 1.533,47 
+</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1427,11 +1587,16 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:
-TOTAL ORIGEM: 1.316,44 60,16 156,87 1.533,47</t>
+1.316,44 60,16 156,87 1.533,47 
+</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1458,11 +1623,16 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1489,11 +1659,16 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1520,11 +1695,16 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1551,11 +1731,16 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1582,11 +1767,16 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1613,11 +1803,16 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1644,11 +1839,16 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1675,11 +1875,16 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1706,11 +1911,16 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1737,11 +1947,16 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1768,11 +1983,16 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1799,11 +2019,16 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1830,11 +2055,16 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1861,11 +2091,16 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:
-TOTAL ORIGEM: 1.310,04 59,88 156,14 1.526,06</t>
+1.310,04 59,88 156,14 1.526,06 
+</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1892,11 +2127,16 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:
-TOTAL ORIGEM: 1.737,88 79,14 206,36 2.023,38</t>
+1.737,88 79,14 206,36 2.023,38 
+</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1923,11 +2163,16 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:
-TOTAL ORIGEM: 1.737,88 79,14 206,36 2.023,38</t>
+1.737,88 79,14 206,36 2.023,38 
+</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1954,11 +2199,16 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:
-TOTAL ORIGEM: 1.737,88 79,14 206,36 2.023,38</t>
+1.737,88 79,14 206,36 2.023,38 
+</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -1985,11 +2235,16 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:
-TOTAL ORIGEM: 1.737,88 79,14 206,36 2.023,38</t>
+1.737,88 79,14 206,36 2.023,38 
+</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -2016,11 +2271,16 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:
-TOTAL ORIGEM: 1.737,88 79,14 206,36 2.023,38</t>
+1.737,88 79,14 206,36 2.023,38 
+</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -2047,15 +2307,20 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
+35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:
-TOTAL ORIGEM: 70.402,49 7.217,06 11.178,50 88.798,05</t>
+35.200,13 5.632,02 7.040,02 47.872,17 
+</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2082,15 +2347,20 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
+35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:
-TOTAL ORIGEM: 70.402,49 7.217,06 11.178,50 88.798,05</t>
+35.200,13 5.632,02 7.040,02 47.872,17 
+</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2117,15 +2387,20 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
+35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:
-TOTAL ORIGEM: 70.402,49 7.217,06 11.178,50 88.798,05</t>
+35.200,13 5.632,02 7.040,02 47.872,17 
+</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2152,15 +2427,20 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
+35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:
-TOTAL ORIGEM: 70.402,49 7.217,06 11.178,50 88.798,05</t>
+35.200,13 5.632,02 7.040,02 47.872,17 
+</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2187,15 +2467,20 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
+10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:
-TOTAL ORIGEM: 20.762,49 2.128,94 3.298,15 26.189,58</t>
+10.380,13 1.660,82 2.076,02 14.116,97 
+</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2222,15 +2507,20 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
+10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:
-TOTAL ORIGEM: 20.762,49 2.128,94 3.298,15 26.189,58</t>
+10.380,13 1.660,82 2.076,02 14.116,97 
+</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2257,15 +2547,20 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
+10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:
-TOTAL ORIGEM: 20.762,49 2.128,94 3.298,15 26.189,58</t>
+10.380,13 1.660,82 2.076,02 14.116,97 
+</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2292,15 +2587,20 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
+10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:
-TOTAL ORIGEM: 20.762,49 2.128,94 3.298,15 26.189,58</t>
+10.380,13 1.660,82 2.076,02 14.116,97 
+</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2327,14 +2627,19 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
+588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:
-TOTAL ORIGEM: 866,09 62,88 137,88 1.066,85</t>
+277,15 30,49 55,43 363,07 
+</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2361,14 +2666,19 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
+588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:
-TOTAL ORIGEM: 866,09 62,88 137,88 1.066,85</t>
+277,15 30,49 55,43 363,07 
+</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2395,14 +2705,19 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
+588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:
-TOTAL ORIGEM: 866,09 62,88 137,88 1.066,85</t>
+277,15 30,49 55,43 363,07 
+</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2429,14 +2744,19 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
+588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:
-TOTAL ORIGEM: 866,09 62,88 137,88 1.066,85</t>
+277,15 30,49 55,43 363,07 
+</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2463,10 +2783,10 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
+1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2474,8 +2794,13 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:
-TOTAL ORIGEM: 6.841,85 1.697,90 1.182,35 9.722,10</t>
+5.023,57 1.615,14 966,52 7.605,23 
+</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2502,10 +2827,10 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
+1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2513,8 +2838,13 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:
-TOTAL ORIGEM: 6.841,85 1.697,90 1.182,35 9.722,10</t>
+5.023,57 1.615,14 966,52 7.605,23 
+</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2541,10 +2871,10 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
+1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2552,8 +2882,13 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:
-TOTAL ORIGEM: 6.841,85 1.697,90 1.182,35 9.722,10</t>
+5.023,57 1.615,14 966,52 7.605,23 
+</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2580,10 +2915,10 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
+1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2591,8 +2926,13 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:
-TOTAL ORIGEM: 6.841,85 1.697,90 1.182,35 9.722,10</t>
+5.023,57 1.615,14 966,52 7.605,23 
+</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2619,11 +2959,16 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
+          <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:
-TOTAL ORIGEM: 255,67 51,14 51,14 357,95</t>
+255,67 51,14 51,14 357,95 
+</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2650,11 +2995,16 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
+          <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:
-TOTAL ORIGEM: 255,67 51,14 51,14 357,95</t>
+255,67 51,14 51,14 357,95 
+</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2681,11 +3031,16 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
+          <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:
-TOTAL ORIGEM: 255,67 51,14 51,14 357,95</t>
+255,67 51,14 51,14 357,95 
+</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2712,11 +3067,16 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
+          <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:
-TOTAL ORIGEM: 255,67 51,14 51,14 357,95</t>
+255,67 51,14 51,14 357,95 
+</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2743,10 +3103,10 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
+324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -2754,8 +3114,13 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:
-TOTAL ORIGEM: 1.864,33 721,98 340,53 2.926,84</t>
+1.539,77 697,38 275,61 2.512,76 
+</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2782,10 +3147,10 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
+324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -2793,8 +3158,13 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:
-TOTAL ORIGEM: 1.864,33 721,98 340,53 2.926,84</t>
+1.539,77 697,38 275,61 2.512,76 
+</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2821,10 +3191,10 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
+324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -2832,8 +3202,13 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:
-TOTAL ORIGEM: 1.864,33 721,98 340,53 2.926,84</t>
+1.539,77 697,38 275,61 2.512,76 
+</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2860,10 +3235,10 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
+324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -2871,8 +3246,13 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:
-TOTAL ORIGEM: 1.864,33 721,98 340,53 2.926,84</t>
+1.539,77 697,38 275,61 2.512,76 
+</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2899,16 +3279,21 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
+718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:
-TOTAL ORIGEM: 2.085,77 566,17 381,25 3.033,19</t>
+1.367,23 517,37 254,89 2.139,49 
+</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2935,16 +3320,21 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
+718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:
-TOTAL ORIGEM: 2.085,77 566,17 381,25 3.033,19</t>
+1.367,23 517,37 254,89 2.139,49 
+</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2971,16 +3361,21 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
+718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:
-TOTAL ORIGEM: 2.085,77 566,17 381,25 3.033,19</t>
+1.367,23 517,37 254,89 2.139,49 
+</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3007,16 +3402,21 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
+718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:
-TOTAL ORIGEM: 2.085,77 566,17 381,25 3.033,19</t>
+1.367,23 517,37 254,89 2.139,49 
+</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3043,21 +3443,26 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 TOTAL:
+1.383,40 63,18 164,73 1.611,31 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 TOTAL:
+2.633,14 664,34 526,62 3.824,10 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 TOTAL:
-TOTAL ORIGEM: 5.271,42 1.279,67 942,32 7.493,41</t>
+1.254,88 552,15 250,97 2.058,00 
+</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -3084,21 +3489,26 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 TOTAL:
+1.383,40 63,18 164,73 1.611,31 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 TOTAL:
+2.633,14 664,34 526,62 3.824,10 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 TOTAL:
-TOTAL ORIGEM: 5.271,42 1.279,67 942,32 7.493,41</t>
+1.254,88 552,15 250,97 2.058,00 
+</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -3125,21 +3535,26 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 TOTAL:
+1.383,40 63,18 164,73 1.611,31 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 TOTAL:
+2.633,14 664,34 526,62 3.824,10 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 TOTAL:
-TOTAL ORIGEM: 5.271,42 1.279,67 942,32 7.493,41</t>
+1.254,88 552,15 250,97 2.058,00 
+</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -3166,11 +3581,16 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:
-TOTAL ORIGEM: 508,64 27,97 71,21 607,82</t>
+508,64 27,97 71,21 607,82 
+</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3197,11 +3617,16 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:
-TOTAL ORIGEM: 508,64 27,97 71,21 607,82</t>
+508,64 27,97 71,21 607,82 
+</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3228,11 +3653,16 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:
-TOTAL ORIGEM: 508,64 27,97 71,21 607,82</t>
+508,64 27,97 71,21 607,82 
+</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3259,11 +3689,16 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:
-TOTAL ORIGEM: 508,64 27,97 71,21 607,82</t>
+508,64 27,97 71,21 607,82 
+</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3290,11 +3725,16 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:
-TOTAL ORIGEM: 508,64 27,97 71,21 607,82</t>
+508,64 27,97 71,21 607,82 
+</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3321,10 +3761,15 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:
-TOTAL ORIGEM: 170,92 0,00 0,00 170,92</t>
+170,92 0,00 0,00 170,92 
+</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -3351,10 +3796,15 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:
-TOTAL ORIGEM: 170,92 0,00 0,00 170,92</t>
+170,92 0,00 0,00 170,92 
+</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -3381,10 +3831,15 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:
-TOTAL ORIGEM: 170,92 0,00 0,00 170,92</t>
+170,92 0,00 0,00 170,92 
+</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -3411,10 +3866,15 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:
-TOTAL ORIGEM: 170,92 0,00 0,00 170,92</t>
+170,92 0,00 0,00 170,92 
+</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -3441,10 +3901,15 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:
-TOTAL ORIGEM: 170,92 0,00 0,00 170,92</t>
+170,92 0,00 0,00 170,92 
+</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -3471,10 +3936,15 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
+          <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:
-TOTAL ORIGEM: 170,92 0,00 0,00 170,92</t>
+170,92 0,00 0,00 170,92 
+</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>[['Dívida Parcelada']]</t>
         </is>
       </c>
     </row>
@@ -3501,16 +3971,21 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
 2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 TOTAL:
+1.105,34 59,55 155,06 1.319,95 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
 2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
 2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 TOTAL:
-TOTAL ORIGEM: 2.611,26 394,71 401,19 3.407,16</t>
+1.505,92 335,16 246,13 2.087,21 
+</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3537,16 +4012,21 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
 2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 TOTAL:
+1.105,34 59,55 155,06 1.319,95 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
 2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
 2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 TOTAL:
-TOTAL ORIGEM: 2.611,26 394,71 401,19 3.407,16</t>
+1.505,92 335,16 246,13 2.087,21 
+</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3573,16 +4053,21 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
 2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 TOTAL:
+1.105,34 59,55 155,06 1.319,95 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
 2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
 2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 TOTAL:
-TOTAL ORIGEM: 2.611,26 394,71 401,19 3.407,16</t>
+1.505,92 335,16 246,13 2.087,21 
+</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3609,11 +4094,16 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:
-TOTAL ORIGEM: 879,90 49,06 124,79 1.053,75</t>
+879,90 49,06 124,79 1.053,75 
+</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3640,11 +4130,16 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:
-TOTAL ORIGEM: 879,90 49,06 124,79 1.053,75</t>
+879,90 49,06 124,79 1.053,75 
+</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3671,11 +4166,16 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:
-TOTAL ORIGEM: 879,90 49,06 124,79 1.053,75</t>
+879,90 49,06 124,79 1.053,75 
+</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3702,11 +4202,16 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:
-TOTAL ORIGEM: 879,90 49,06 124,79 1.053,75</t>
+879,90 49,06 124,79 1.053,75 
+</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3733,10 +4238,15 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:
-TOTAL ORIGEM: 204,00 8,16 16,32 228,48</t>
+204,00 8,16 16,32 228,48 
+</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3763,10 +4273,15 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:
-TOTAL ORIGEM: 204,00 8,16 16,32 228,48</t>
+204,00 8,16 16,32 228,48 
+</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3793,10 +4308,15 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:
-TOTAL ORIGEM: 204,00 8,16 16,32 228,48</t>
+204,00 8,16 16,32 228,48 
+</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3823,10 +4343,15 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:
-TOTAL ORIGEM: 204,00 8,16 16,32 228,48</t>
+204,00 8,16 16,32 228,48 
+</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -3853,16 +4378,21 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
+792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:
-TOTAL ORIGEM: 2.716,57 793,94 477,72 3.988,23</t>
+1.924,32 744,30 352,24 3.020,86 
+</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3889,16 +4419,21 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
+792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:
-TOTAL ORIGEM: 2.716,57 793,94 477,72 3.988,23</t>
+1.924,32 744,30 352,24 3.020,86 
+</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3925,16 +4460,21 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
+792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:
-TOTAL ORIGEM: 2.716,57 793,94 477,72 3.988,23</t>
+1.924,32 744,30 352,24 3.020,86 
+</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3961,16 +4501,21 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
+792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:
-TOTAL ORIGEM: 2.716,57 793,94 477,72 3.988,23</t>
+1.924,32 744,30 352,24 3.020,86 
+</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3997,15 +4542,20 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
+942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:
-TOTAL ORIGEM: 1.670,69 199,61 282,68 2.152,98</t>
+728,25 145,65 145,65 1.019,55 
+</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4032,15 +4582,20 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
+942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:
-TOTAL ORIGEM: 1.670,69 199,61 282,68 2.152,98</t>
+728,25 145,65 145,65 1.019,55 
+</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4067,15 +4622,20 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
+942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:
-TOTAL ORIGEM: 1.670,69 199,61 282,68 2.152,98</t>
+728,25 145,65 145,65 1.019,55 
+</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4102,15 +4662,20 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
+942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:
-TOTAL ORIGEM: 1.670,69 199,61 282,68 2.152,98</t>
+728,25 145,65 145,65 1.019,55 
+</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4137,10 +4702,10 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
+1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4154,8 +4719,13 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:
-TOTAL ORIGEM: 4.207,95 1.370,38 773,85 6.352,18</t>
+3.047,35 1.307,18 609,49 4.964,02 
+</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4182,10 +4752,10 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
+1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4199,8 +4769,13 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:
-TOTAL ORIGEM: 4.207,95 1.370,38 773,85 6.352,18</t>
+3.047,35 1.307,18 609,49 4.964,02 
+</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4227,10 +4802,10 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
+1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4244,8 +4819,13 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:
-TOTAL ORIGEM: 4.207,95 1.370,38 773,85 6.352,18</t>
+3.047,35 1.307,18 609,49 4.964,02 
+</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4272,10 +4852,10 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
+1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4289,8 +4869,13 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:
-TOTAL ORIGEM: 4.207,95 1.370,38 773,85 6.352,18</t>
+3.047,35 1.307,18 609,49 4.964,02 
+</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4317,24 +4902,29 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
 2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 TOTAL:
+862,55 53,88 136,23 1.052,66 
 Dívida Ativa Situação:
 2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
 2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
 2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
 2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
 2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 TOTAL:
+2.069,09 674,06 400,17 3.143,32 
 Ajuizada Situação:
 2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
 2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
 2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
 2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 TOTAL:
-TOTAL ORIGEM: 4.696,97 1.610,58 889,47 7.197,02</t>
+1.765,33 882,64 353,07 3.001,04 
+</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -4361,24 +4951,29 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
 2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 TOTAL:
+862,55 53,88 136,23 1.052,66 
 Dívida Ativa Situação:
 2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
 2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
 2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
 2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
 2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 TOTAL:
+2.069,09 674,06 400,17 3.143,32 
 Ajuizada Situação:
 2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
 2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
 2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
 2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 TOTAL:
-TOTAL ORIGEM: 4.696,97 1.610,58 889,47 7.197,02</t>
+1.765,33 882,64 353,07 3.001,04 
+</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -4405,24 +5000,29 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
 2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 TOTAL:
+862,55 53,88 136,23 1.052,66 
 Dívida Ativa Situação:
 2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
 2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
 2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
 2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
 2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 TOTAL:
+2.069,09 674,06 400,17 3.143,32 
 Ajuizada Situação:
 2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
 2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
 2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
 2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 TOTAL:
-TOTAL ORIGEM: 4.696,97 1.610,58 889,47 7.197,02</t>
+1.765,33 882,64 353,07 3.001,04 
+</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -4449,11 +5049,11 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 TOTAL:
+909,77 57,15 149,35 1.116,27 
 Dívida Ativa Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
@@ -4462,8 +5062,13 @@
 2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 TOTAL:
-TOTAL ORIGEM: 3.102,52 706,69 587,89 4.397,10</t>
+2.192,75 649,54 438,54 3.280,83 
+</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4490,11 +5095,11 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 TOTAL:
+909,77 57,15 149,35 1.116,27 
 Dívida Ativa Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
@@ -4503,8 +5108,13 @@
 2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 TOTAL:
-TOTAL ORIGEM: 3.102,52 706,69 587,89 4.397,10</t>
+2.192,75 649,54 438,54 3.280,83 
+</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4531,11 +5141,11 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 TOTAL:
+909,77 57,15 149,35 1.116,27 
 Dívida Ativa Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
@@ -4544,8 +5154,13 @@
 2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 TOTAL:
-TOTAL ORIGEM: 3.102,52 706,69 587,89 4.397,10</t>
+2.192,75 649,54 438,54 3.280,83 
+</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4572,17 +5187,22 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
 2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 TOTAL:
+366,61 27,88 73,32 467,81 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
 2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
 2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
 2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 TOTAL:
-TOTAL ORIGEM: 1.115,16 219,10 223,03 1.557,29</t>
+748,55 191,22 149,71 1.089,48 
+</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4609,17 +5229,22 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
 2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 TOTAL:
+366,61 27,88 73,32 467,81 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
 2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
 2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
 2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 TOTAL:
-TOTAL ORIGEM: 1.115,16 219,10 223,03 1.557,29</t>
+748,55 191,22 149,71 1.089,48 
+</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4646,17 +5271,22 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
 2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 TOTAL:
+366,61 27,88 73,32 467,81 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
 2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
 2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
 2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 TOTAL:
-TOTAL ORIGEM: 1.115,16 219,10 223,03 1.557,29</t>
+748,55 191,22 149,71 1.089,48 
+</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4683,17 +5313,22 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
+1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:
-TOTAL ORIGEM: 2.500,87 305,07 430,12 3.236,06</t>
+1.248,98 237,60 249,80 1.736,38 
+</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4720,17 +5355,22 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
+1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:
-TOTAL ORIGEM: 2.500,87 305,07 430,12 3.236,06</t>
+1.248,98 237,60 249,80 1.736,38 
+</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4757,17 +5397,22 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
+1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:
-TOTAL ORIGEM: 2.500,87 305,07 430,12 3.236,06</t>
+1.248,98 237,60 249,80 1.736,38 
+</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4794,17 +5439,22 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
+1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:
-TOTAL ORIGEM: 2.500,87 305,07 430,12 3.236,06</t>
+1.248,98 237,60 249,80 1.736,38 
+</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4831,17 +5481,22 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
+1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:
-TOTAL ORIGEM: 2.500,87 305,07 430,12 3.236,06</t>
+1.248,98 237,60 249,80 1.736,38 
+</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4868,14 +5523,19 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 TOTAL:
+925,32 51,55 131,12 1.107,99 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 TOTAL:
-TOTAL ORIGEM: 1.128,65 80,02 171,79 1.380,46</t>
+203,33 28,47 40,67 272,47 
+</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4902,14 +5562,19 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 TOTAL:
+925,32 51,55 131,12 1.107,99 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 TOTAL:
-TOTAL ORIGEM: 1.128,65 80,02 171,79 1.380,46</t>
+203,33 28,47 40,67 272,47 
+</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4936,14 +5601,19 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 TOTAL:
+925,32 51,55 131,12 1.107,99 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 TOTAL:
-TOTAL ORIGEM: 1.128,65 80,02 171,79 1.380,46</t>
+203,33 28,47 40,67 272,47 
+</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4970,12 +5640,17 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:
-TOTAL ORIGEM: 1.944,91 53,19 139,52 2.137,62</t>
+1.944,91 53,19 139,52 2.137,62 
+</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -5002,12 +5677,17 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:
-TOTAL ORIGEM: 1.944,91 53,19 139,52 2.137,62</t>
+1.944,91 53,19 139,52 2.137,62 
+</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -5034,12 +5714,17 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:
-TOTAL ORIGEM: 1.944,91 53,19 139,52 2.137,62</t>
+1.944,91 53,19 139,52 2.137,62 
+</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -5066,12 +5751,17 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:
-TOTAL ORIGEM: 1.944,91 53,19 139,52 2.137,62</t>
+1.944,91 53,19 139,52 2.137,62 
+</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>[['Dívida Corrente']]</t>
         </is>
       </c>
     </row>
@@ -5098,17 +5788,22 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
+1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:
-TOTAL ORIGEM: 1.909,72 131,41 286,72 2.327,85</t>
+439,18 57,09 87,84 584,11 
+</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5135,17 +5830,22 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
+1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:
-TOTAL ORIGEM: 1.909,72 131,41 286,72 2.327,85</t>
+439,18 57,09 87,84 584,11 
+</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5172,17 +5872,22 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
+1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:
-TOTAL ORIGEM: 1.909,72 131,41 286,72 2.327,85</t>
+439,18 57,09 87,84 584,11 
+</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5209,17 +5914,22 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
+1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:
-TOTAL ORIGEM: 1.909,72 131,41 286,72 2.327,85</t>
+439,18 57,09 87,84 584,11 
+</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5246,17 +5956,22 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
+1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:
-TOTAL ORIGEM: 1.909,72 131,41 286,72 2.327,85</t>
+439,18 57,09 87,84 584,11 
+</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>[['Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5283,22 +5998,27 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
+          <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.683,92 75,76 197,87 1.957,55 8 0
-1.710,44 77,88 203,17 1.991,49 TOTAL:
+1.710,44 77,88 203,17 1.991,49 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.517,01 470,27 303,40 2.290,68 1 0
 2022 07 Capin. RoçaD.A 216,32 23,80 43,26 283,38 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.683,88 336,78 336,78 2.357,44 1 0
-3.471,09 844,88 694,21 5.010,18 TOTAL:
+3.471,09 844,88 694,21 5.010,18 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.517,01 667,48 303,40 2.487,89 1 0
-1.549,48 681,77 309,89 2.541,14 TOTAL:
-TOTAL ORIGEM: 6.731,01 1.604,53 1.207,27 9.542,81</t>
+1.549,48 681,77 309,89 2.541,14 
+</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>[['Ajuizada']]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
extração de dados completa
</commit_message>
<xml_diff>
--- a/prototipos/DataInput/Relatório.xlsx
+++ b/prototipos/DataInput/Relatório.xlsx
@@ -490,7 +490,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 
 </t>
         </is>
       </c>
@@ -525,7 +524,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 
 </t>
         </is>
       </c>
@@ -560,7 +558,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 
 </t>
         </is>
       </c>
@@ -595,7 +592,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 
 </t>
         </is>
       </c>
@@ -630,7 +626,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 
 </t>
         </is>
       </c>
@@ -665,7 +660,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 
 </t>
         </is>
       </c>
@@ -700,7 +694,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 
 </t>
         </is>
       </c>
@@ -735,7 +728,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 
 </t>
         </is>
       </c>
@@ -770,7 +762,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 
 </t>
         </is>
       </c>
@@ -805,7 +796,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 
 </t>
         </is>
       </c>
@@ -840,7 +830,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 
 </t>
         </is>
       </c>
@@ -876,7 +865,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -912,7 +900,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -948,7 +935,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -984,7 +970,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1019,7 +1004,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 
 </t>
         </is>
       </c>
@@ -1054,7 +1038,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 
 </t>
         </is>
       </c>
@@ -1089,7 +1072,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 
 </t>
         </is>
       </c>
@@ -1124,7 +1106,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 
 </t>
         </is>
       </c>
@@ -1159,7 +1140,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 
 </t>
         </is>
       </c>
@@ -1194,7 +1174,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 
 </t>
         </is>
       </c>
@@ -1230,7 +1209,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 
 </t>
         </is>
       </c>
@@ -1266,7 +1244,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 
 </t>
         </is>
       </c>
@@ -1302,7 +1279,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 
 </t>
         </is>
       </c>
@@ -1338,7 +1314,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 
 </t>
         </is>
       </c>
@@ -1374,7 +1349,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 
 </t>
         </is>
       </c>
@@ -1410,7 +1384,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 31,80 2,54 6,36 40,70 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 
 </t>
         </is>
       </c>
@@ -1446,7 +1419,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 
 </t>
         </is>
       </c>
@@ -1482,7 +1454,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 
 </t>
         </is>
       </c>
@@ -1518,7 +1489,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 
 </t>
         </is>
       </c>
@@ -1554,7 +1524,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 
 </t>
         </is>
       </c>
@@ -1590,7 +1559,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 
 </t>
         </is>
       </c>
@@ -1626,7 +1594,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1662,7 +1629,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1698,7 +1664,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1734,7 +1699,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1770,7 +1734,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1806,7 +1769,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1842,7 +1804,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1878,7 +1839,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1914,7 +1874,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1950,7 +1909,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -1986,7 +1944,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -2022,7 +1979,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -2058,7 +2014,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -2094,7 +2049,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 
 </t>
         </is>
       </c>
@@ -2130,7 +2084,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 
 </t>
         </is>
       </c>
@@ -2166,7 +2119,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 
 </t>
         </is>
       </c>
@@ -2202,7 +2154,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 
 </t>
         </is>
       </c>
@@ -2238,7 +2189,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 
 </t>
         </is>
       </c>
@@ -2274,7 +2224,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 
 </t>
         </is>
       </c>
@@ -2310,17 +2259,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 
 </t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2350,17 +2297,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 
 </t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2390,17 +2335,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 
 </t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2430,17 +2373,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 
 </t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2470,17 +2411,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 
 </t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2510,17 +2449,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 
 </t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2550,17 +2487,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 
 </t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2590,17 +2525,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 
 Dívida Ativa Situação:
 2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
 2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 
 </t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2630,10 +2563,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 
 </t>
         </is>
       </c>
@@ -2669,10 +2600,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 
 </t>
         </is>
       </c>
@@ -2708,10 +2637,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 
 </t>
         </is>
       </c>
@@ -2747,10 +2674,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
 2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 
 Dívida Ativa Situação:
 2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 
 </t>
         </is>
       </c>
@@ -2786,7 +2711,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2794,13 +2718,12 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 
 </t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2830,7 +2753,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2838,13 +2760,12 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 
 </t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2874,7 +2795,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2882,13 +2802,12 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 
 </t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2918,7 +2837,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 
 Dívida Ativa Situação:
 2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
@@ -2926,13 +2844,12 @@
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
 2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 
 </t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2962,13 +2879,12 @@
           <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 
 </t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -2998,13 +2914,12 @@
           <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 
 </t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3034,13 +2949,12 @@
           <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 
 </t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3070,13 +2984,12 @@
           <t xml:space="preserve">Dívida Ativa Situação:
 2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
 2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 
 </t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3019,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -3114,13 +3026,12 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 
 </t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3150,7 +3061,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -3158,13 +3068,12 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 
 </t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3103,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -3202,13 +3110,12 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 
 </t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3145,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
 2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
 2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
@@ -3246,13 +3152,12 @@
 2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
 2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
 2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 
 </t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3282,18 +3187,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 
 </t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3323,18 +3226,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 
 </t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3364,18 +3265,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 
 </t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3405,18 +3304,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
 2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
 2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
 2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 
 </t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -3446,23 +3343,20 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 
 </t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -3492,23 +3386,20 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 
 </t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -3538,23 +3429,20 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 
 </t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -3584,7 +3472,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 
 </t>
         </is>
       </c>
@@ -3620,7 +3507,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 
 </t>
         </is>
       </c>
@@ -3656,7 +3542,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 
 </t>
         </is>
       </c>
@@ -3692,7 +3577,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 
 </t>
         </is>
       </c>
@@ -3728,7 +3612,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
 2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 
 </t>
         </is>
       </c>
@@ -3763,7 +3646,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 
 </t>
         </is>
       </c>
@@ -3798,7 +3680,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 
 </t>
         </is>
       </c>
@@ -3833,7 +3714,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 
 </t>
         </is>
       </c>
@@ -3868,7 +3748,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 
 </t>
         </is>
       </c>
@@ -3903,7 +3782,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 
 </t>
         </is>
       </c>
@@ -3938,7 +3816,6 @@
         <is>
           <t xml:space="preserve">Dívida Parcelada Situação:
 2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 
 </t>
         </is>
       </c>
@@ -3974,18 +3851,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
 2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
 2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
 2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 
 </t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'TSU - DA', 151.04, 30.21, 30.21, 211.46, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4015,18 +3890,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
 2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
 2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
 2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 
 </t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'TSU - DA', 151.04, 30.21, 30.21, 211.46, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4056,18 +3929,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
 2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
 2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
 2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 
 </t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'TSU - DA', 151.04, 30.21, 30.21, 211.46, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4097,7 +3968,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 
 </t>
         </is>
       </c>
@@ -4133,7 +4003,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 
 </t>
         </is>
       </c>
@@ -4169,7 +4038,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 
 </t>
         </is>
       </c>
@@ -4205,7 +4073,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 
 </t>
         </is>
       </c>
@@ -4240,7 +4107,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 
 </t>
         </is>
       </c>
@@ -4275,7 +4141,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 
 </t>
         </is>
       </c>
@@ -4310,7 +4175,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 
 </t>
         </is>
       </c>
@@ -4345,7 +4209,6 @@
         <is>
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 
 </t>
         </is>
       </c>
@@ -4381,18 +4244,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 
 </t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4422,18 +4283,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 
 </t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4463,18 +4322,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 
 </t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4504,18 +4361,16 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
 2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
 2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
 2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 
 </t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4545,17 +4400,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 
 </t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4585,17 +4438,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 
 </t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4625,17 +4476,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 
 </t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4665,17 +4514,15 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
 2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 
 Dívida Ativa Situação:
 2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
 2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 
 </t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4705,7 +4552,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4719,13 +4565,12 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 
 </t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4755,7 +4600,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4769,13 +4613,12 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 
 </t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4805,7 +4648,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4819,13 +4661,12 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 
 </t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4855,7 +4696,6 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
 2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 
 Dívida Ativa Situação:
 2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
 2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
@@ -4869,13 +4709,12 @@
 2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
 2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
 2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 
 </t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -4905,26 +4744,23 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
 2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 
 Dívida Ativa Situação:
 2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
 2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
 2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
 2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
 2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 
 Ajuizada Situação:
 2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
 2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
 2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
 2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 
 </t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'TSU - DA', 124.42, 38.57, 24.88, 187.87, 1, 0], ['2022', '01', 'TSU - DA', 112.68, 22.54, 22.54, 157.76, 1, 0], ['2019', '01', 'TSU - DA', 130.9, 73.31, 26.18, 230.39, 1, 0], ['2020', '01', 'TSU - DA', 131.53, 57.88, 26.31, 215.72, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -4954,26 +4790,23 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
 2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 
 Dívida Ativa Situação:
 2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
 2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
 2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
 2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
 2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 
 Ajuizada Situação:
 2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
 2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
 2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
 2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 
 </t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'TSU - DA', 124.42, 38.57, 24.88, 187.87, 1, 0], ['2022', '01', 'TSU - DA', 112.68, 22.54, 22.54, 157.76, 1, 0], ['2019', '01', 'TSU - DA', 130.9, 73.31, 26.18, 230.39, 1, 0], ['2020', '01', 'TSU - DA', 131.53, 57.88, 26.31, 215.72, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -5003,26 +4836,23 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
 2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 
 Dívida Ativa Situação:
 2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
 2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
 2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
 2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
 2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 
 Ajuizada Situação:
 2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
 2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
 2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
 2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 
 </t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'TSU - DA', 124.42, 38.57, 24.88, 187.87, 1, 0], ['2022', '01', 'TSU - DA', 112.68, 22.54, 22.54, 157.76, 1, 0], ['2019', '01', 'TSU - DA', 130.9, 73.31, 26.18, 230.39, 1, 0], ['2020', '01', 'TSU - DA', 131.53, 57.88, 26.31, 215.72, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>
@@ -5053,7 +4883,6 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 
 Dívida Ativa Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
@@ -5062,13 +4891,12 @@
 2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 
 </t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], ['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2021', '01', 'ITU - DA', 611.92, 189.7, 122.38, 924.0, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2022', '01', 'ITU - DA', 679.23, 135.85, 135.85, 950.93, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5099,7 +4927,6 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 
 Dívida Ativa Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
@@ -5108,13 +4935,12 @@
 2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 
 </t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], ['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2021', '01', 'ITU - DA', 611.92, 189.7, 122.38, 924.0, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2022', '01', 'ITU - DA', 679.23, 135.85, 135.85, 950.93, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5145,7 +4971,6 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 
 Dívida Ativa Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
@@ -5154,13 +4979,12 @@
 2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 
 </t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], ['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2021', '01', 'ITU - DA', 611.92, 189.7, 122.38, 924.0, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2022', '01', 'ITU - DA', 679.23, 135.85, 135.85, 950.93, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5190,19 +5014,17 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
 2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
 2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
 2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
 2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 
 </t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 288.47, 89.42, 57.69, 435.58, 1, 0], ['2021', '01', 'TSU - DA', 88.98, 27.58, 17.8, 134.36, 1, 0], ['2022', '01', 'IPTU - DA', 290.52, 58.1, 58.1, 406.72, 1, 0], ['2022', '01', 'TSU - DA', 80.58, 16.12, 16.12, 112.82, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5232,19 +5054,17 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
 2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
 2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
 2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
 2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 
 </t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 288.47, 89.42, 57.69, 435.58, 1, 0], ['2021', '01', 'TSU - DA', 88.98, 27.58, 17.8, 134.36, 1, 0], ['2022', '01', 'IPTU - DA', 290.52, 58.1, 58.1, 406.72, 1, 0], ['2022', '01', 'TSU - DA', 80.58, 16.12, 16.12, 112.82, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5274,19 +5094,17 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
 2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 
 Dívida Ativa Situação:
 2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
 2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
 2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
 2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 
 </t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2021', '01', 'IPTU - DA', 288.47, 89.42, 57.69, 435.58, 1, 0], ['2021', '01', 'TSU - DA', 88.98, 27.58, 17.8, 134.36, 1, 0], ['2022', '01', 'IPTU - DA', 290.52, 58.1, 58.1, 406.72, 1, 0], ['2022', '01', 'TSU - DA', 80.58, 16.12, 16.12, 112.82, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5317,18 +5135,16 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 
 </t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5359,18 +5175,16 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 
 </t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5401,18 +5215,16 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 
 </t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5443,18 +5255,16 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 
 </t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5485,18 +5295,16 @@
 2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 
 </t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
         </is>
       </c>
     </row>
@@ -5526,10 +5334,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 
 </t>
         </is>
       </c>
@@ -5565,10 +5371,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 
 </t>
         </is>
       </c>
@@ -5604,10 +5408,8 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 
 Dívida Ativa Situação:
 2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 
 </t>
         </is>
       </c>
@@ -5644,7 +5446,6 @@
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 
 </t>
         </is>
       </c>
@@ -5681,7 +5482,6 @@
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 
 </t>
         </is>
       </c>
@@ -5718,7 +5518,6 @@
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 
 </t>
         </is>
       </c>
@@ -5755,7 +5554,6 @@
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
 2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 
 </t>
         </is>
       </c>
@@ -5793,11 +5591,9 @@
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 
 </t>
         </is>
       </c>
@@ -5835,11 +5631,9 @@
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 
 </t>
         </is>
       </c>
@@ -5877,11 +5671,9 @@
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 
 </t>
         </is>
       </c>
@@ -5919,11 +5711,9 @@
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 
 </t>
         </is>
       </c>
@@ -5961,11 +5751,9 @@
 2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 
 Dívida Ativa Situação:
 2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
 2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 
 </t>
         </is>
       </c>
@@ -6001,24 +5789,21 @@
           <t xml:space="preserve">Dívida Corrente Situação:
 2023 01 CIP 26,52 2,12 5,30 33,94 1 0
 2023 01 ITU 1.683,92 75,76 197,87 1.957,55 8 0
-1.710,44 77,88 203,17 1.991,49 
 Dívida Ativa Situação:
 2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
 2021 01 ITU - DA 1.517,01 470,27 303,40 2.290,68 1 0
 2022 07 Capin. RoçaD.A 216,32 23,80 43,26 283,38 1 0
 2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
 2022 01 ITU - DA 1.683,88 336,78 336,78 2.357,44 1 0
-3.471,09 844,88 694,21 5.010,18 
 Ajuizada Situação:
 2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
 2020 01 ITU - DA 1.517,01 667,48 303,40 2.487,89 1 0
-1.549,48 681,77 309,89 2.541,14 
 </t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>[['Ajuizada']]</t>
+          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
extração de dados em testes
</commit_message>
<xml_diff>
--- a/prototipos/DataInput/Relatório.xlsx
+++ b/prototipos/DataInput/Relatório.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Origem:</t>
+          <t>Origem</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Inscrição:</t>
+          <t>Inscrição</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Matrícula:</t>
+          <t>Matrícula</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Endereço:</t>
+          <t>Endereço</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Dados Brutos</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Dividas:</t>
+          <t>Dívidas</t>
         </is>
       </c>
     </row>
@@ -488,14 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': '2.327,45', 'Juros': '14,19', 'Multa': '18,89', 'Total': '2.360,53', 'Vencidas': '2', 'A Vencer': '3'}]}]</t>
         </is>
       </c>
     </row>
@@ -522,14 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': '2.327,45', 'Juros': '14,19', 'Multa': '18,89', 'Total': '2.360,53', 'Vencidas': '2', 'A Vencer': '3'}]}]</t>
         </is>
       </c>
     </row>
@@ -556,14 +537,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': '2.327,45', 'Juros': '14,19', 'Multa': '18,89', 'Total': '2.360,53', 'Vencidas': '2', 'A Vencer': '3'}]}]</t>
         </is>
       </c>
     </row>
@@ -590,14 +564,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': '2.327,45', 'Juros': '14,19', 'Multa': '18,89', 'Total': '2.360,53', 'Vencidas': '2', 'A Vencer': '3'}]}]</t>
         </is>
       </c>
     </row>
@@ -624,14 +591,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': '2.327,45', 'Juros': '14,19', 'Multa': '18,89', 'Total': '2.360,53', 'Vencidas': '2', 'A Vencer': '3'}]}]</t>
         </is>
       </c>
     </row>
@@ -658,14 +618,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '3.109,60', 'Juros': '4,63', 'Multa': '18,44', 'Total': '3.132,67', 'Vencidas': '2', 'A Vencer': '5'}]}]</t>
         </is>
       </c>
     </row>
@@ -692,14 +645,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '3.109,60', 'Juros': '4,63', 'Multa': '18,44', 'Total': '3.132,67', 'Vencidas': '2', 'A Vencer': '5'}]}]</t>
         </is>
       </c>
     </row>
@@ -726,14 +672,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '3.109,60', 'Juros': '4,63', 'Multa': '18,44', 'Total': '3.132,67', 'Vencidas': '2', 'A Vencer': '5'}]}]</t>
         </is>
       </c>
     </row>
@@ -760,14 +699,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '3.109,60', 'Juros': '4,63', 'Multa': '18,44', 'Total': '3.132,67', 'Vencidas': '2', 'A Vencer': '5'}]}]</t>
         </is>
       </c>
     </row>
@@ -794,14 +726,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '3.109,60', 'Juros': '4,63', 'Multa': '18,44', 'Total': '3.132,67', 'Vencidas': '2', 'A Vencer': '5'}]}]</t>
         </is>
       </c>
     </row>
@@ -828,14 +753,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '3.109,60', 'Juros': '4,63', 'Multa': '18,44', 'Total': '3.132,67', 'Vencidas': '2', 'A Vencer': '5'}]}]</t>
         </is>
       </c>
     </row>
@@ -862,15 +780,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -897,15 +807,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -932,15 +834,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -967,15 +861,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1002,14 +888,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '320,88', 'Juros': '4,81', 'Multa': '16,05', 'Total': '341,74', 'Vencidas': '2', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1036,14 +915,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '320,88', 'Juros': '4,81', 'Multa': '16,05', 'Total': '341,74', 'Vencidas': '2', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1070,14 +942,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '320,88', 'Juros': '4,81', 'Multa': '16,05', 'Total': '341,74', 'Vencidas': '2', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1104,14 +969,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '320,88', 'Juros': '4,81', 'Multa': '16,05', 'Total': '341,74', 'Vencidas': '2', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1138,14 +996,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '320,88', 'Juros': '4,81', 'Multa': '16,05', 'Total': '341,74', 'Vencidas': '2', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1172,14 +1023,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '320,88', 'Juros': '4,81', 'Multa': '16,05', 'Total': '341,74', 'Vencidas': '2', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1206,15 +1050,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '31,80', 'Juros': '2,54', 'Multa': '6,36', 'Total': '40,70', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1241,15 +1077,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '31,80', 'Juros': '2,54', 'Multa': '6,36', 'Total': '40,70', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1276,15 +1104,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '31,80', 'Juros': '2,54', 'Multa': '6,36', 'Total': '40,70', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1311,15 +1131,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '31,80', 'Juros': '2,54', 'Multa': '6,36', 'Total': '40,70', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1346,15 +1158,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '31,80', 'Juros': '2,54', 'Multa': '6,36', 'Total': '40,70', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1381,15 +1185,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '31,80', 'Juros': '2,54', 'Multa': '6,36', 'Total': '40,70', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1416,15 +1212,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.289,92', 'Juros': '58,04', 'Multa': '151,57', 'Total': '1.499,53', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1451,15 +1239,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.289,92', 'Juros': '58,04', 'Multa': '151,57', 'Total': '1.499,53', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1486,15 +1266,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.289,92', 'Juros': '58,04', 'Multa': '151,57', 'Total': '1.499,53', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1521,15 +1293,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.289,92', 'Juros': '58,04', 'Multa': '151,57', 'Total': '1.499,53', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1556,15 +1320,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.289,92', 'Juros': '58,04', 'Multa': '151,57', 'Total': '1.499,53', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1591,15 +1347,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1626,15 +1374,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1661,15 +1401,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1696,15 +1428,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1731,15 +1455,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1766,15 +1482,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1801,15 +1509,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1836,15 +1536,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1871,15 +1563,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1906,15 +1590,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1941,15 +1617,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -1976,15 +1644,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2011,15 +1671,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2046,15 +1698,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.283,52', 'Juros': '57,76', 'Multa': '150,84', 'Total': '1.492,12', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2081,15 +1725,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.711,36', 'Juros': '77,02', 'Multa': '201,06', 'Total': '1.989,44', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2116,15 +1752,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.711,36', 'Juros': '77,02', 'Multa': '201,06', 'Total': '1.989,44', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2151,15 +1779,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.711,36', 'Juros': '77,02', 'Multa': '201,06', 'Total': '1.989,44', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2186,15 +1806,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.711,36', 'Juros': '77,02', 'Multa': '201,06', 'Total': '1.989,44', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2221,15 +1833,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.711,36', 'Juros': '77,02', 'Multa': '201,06', 'Total': '1.989,44', 'Vencidas': '8', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2256,18 +1860,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '35.175,84', 'Juros': '1.582,92', 'Multa': '4.133,18', 'Total': '40.891,94', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '35.175,86', 'Juros': '5.628,14', 'Multa': '7.035,17', 'Total': '47.839,17', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2294,18 +1887,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '35.175,84', 'Juros': '1.582,92', 'Multa': '4.133,18', 'Total': '40.891,94', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '35.175,86', 'Juros': '5.628,14', 'Multa': '7.035,17', 'Total': '47.839,17', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2332,18 +1914,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '35.175,84', 'Juros': '1.582,92', 'Multa': '4.133,18', 'Total': '40.891,94', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '35.175,86', 'Juros': '5.628,14', 'Multa': '7.035,17', 'Total': '47.839,17', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2370,18 +1941,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '35.175,84', 'Juros': '1.582,92', 'Multa': '4.133,18', 'Total': '40.891,94', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '35.175,86', 'Juros': '5.628,14', 'Multa': '7.035,17', 'Total': '47.839,17', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2408,18 +1968,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '10.355,84', 'Juros': '466,00', 'Multa': '1.216,83', 'Total': '12.038,67', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '10.355,86', 'Juros': '1.656,94', 'Multa': '2.071,17', 'Total': '14.083,97', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2446,18 +1995,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '10.355,84', 'Juros': '466,00', 'Multa': '1.216,83', 'Total': '12.038,67', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '10.355,86', 'Juros': '1.656,94', 'Multa': '2.071,17', 'Total': '14.083,97', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2484,18 +2022,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '10.355,84', 'Juros': '466,00', 'Multa': '1.216,83', 'Total': '12.038,67', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '10.355,86', 'Juros': '1.656,94', 'Multa': '2.071,17', 'Total': '14.083,97', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2522,18 +2049,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 3.88, 4.85, 33.0, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '10.355,84', 'Juros': '466,00', 'Multa': '1.216,83', 'Total': '12.038,67', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '3,88', 'Multa': '4,85', 'Total': '33,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '10.355,86', 'Juros': '1.656,94', 'Multa': '2.071,17', 'Total': '14.083,97', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2560,17 +2076,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '14,72', 'Multa': '23,56', 'Total': '332,75', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '17,67', 'Multa': '58,89', 'Total': '371,03', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '277,15', 'Juros': '30,49', 'Multa': '55,43', 'Total': '363,07', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2597,17 +2103,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '14,72', 'Multa': '23,56', 'Total': '332,75', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '17,67', 'Multa': '58,89', 'Total': '371,03', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '277,15', 'Juros': '30,49', 'Multa': '55,43', 'Total': '363,07', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2634,17 +2130,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '14,72', 'Multa': '23,56', 'Total': '332,75', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '17,67', 'Multa': '58,89', 'Total': '371,03', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '277,15', 'Juros': '30,49', 'Multa': '55,43', 'Total': '363,07', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2671,17 +2157,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '14,72', 'Multa': '23,56', 'Total': '332,75', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '294,47', 'Juros': '17,67', 'Multa': '58,89', 'Total': '371,03', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '277,15', 'Juros': '30,49', 'Multa': '55,43', 'Total': '363,07', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2708,22 +2184,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.791,76', 'Juros': '80,64', 'Multa': '210,53', 'Total': '2.082,93', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '244,95', 'Juros': '124,92', 'Multa': '48,99', 'Total': '418,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.614,20', 'Juros': '500,40', 'Multa': '322,84', 'Total': '2.437,44', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.791,78', 'Juros': '358,36', 'Multa': '358,36', 'Total': '2.508,50', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.318,76', 'Juros': '617,43', 'Multa': '225,56', 'Total': '2.161,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2750,22 +2211,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.791,76', 'Juros': '80,64', 'Multa': '210,53', 'Total': '2.082,93', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '244,95', 'Juros': '124,92', 'Multa': '48,99', 'Total': '418,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.614,20', 'Juros': '500,40', 'Multa': '322,84', 'Total': '2.437,44', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.791,78', 'Juros': '358,36', 'Multa': '358,36', 'Total': '2.508,50', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.318,76', 'Juros': '617,43', 'Multa': '225,56', 'Total': '2.161,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2792,22 +2238,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.791,76', 'Juros': '80,64', 'Multa': '210,53', 'Total': '2.082,93', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '244,95', 'Juros': '124,92', 'Multa': '48,99', 'Total': '418,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.614,20', 'Juros': '500,40', 'Multa': '322,84', 'Total': '2.437,44', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.791,78', 'Juros': '358,36', 'Multa': '358,36', 'Total': '2.508,50', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.318,76', 'Juros': '617,43', 'Multa': '225,56', 'Total': '2.161,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2834,22 +2265,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.791,76', 'Juros': '80,64', 'Multa': '210,53', 'Total': '2.082,93', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '244,95', 'Juros': '124,92', 'Multa': '48,99', 'Total': '418,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.614,20', 'Juros': '500,40', 'Multa': '322,84', 'Total': '2.437,44', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.791,78', 'Juros': '358,36', 'Multa': '358,36', 'Total': '2.508,50', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.318,76', 'Juros': '617,43', 'Multa': '225,56', 'Total': '2.161,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2876,15 +2292,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '205,00', 'Juros': '41,00', 'Multa': '41,00', 'Total': '287,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '50,67', 'Juros': '10,14', 'Multa': '10,14', 'Total': '70,95', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2911,15 +2319,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '205,00', 'Juros': '41,00', 'Multa': '41,00', 'Total': '287,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '50,67', 'Juros': '10,14', 'Multa': '10,14', 'Total': '70,95', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2946,15 +2346,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '205,00', 'Juros': '41,00', 'Multa': '41,00', 'Total': '287,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '50,67', 'Juros': '10,14', 'Multa': '10,14', 'Total': '70,95', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -2981,15 +2373,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 205.0, 41.0, 41.0, 287.0, 1, 0], ['2022', '01', 'TSU - DA', 50.67, 10.14, 10.14, 70.95, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '205,00', 'Juros': '41,00', 'Multa': '41,00', 'Total': '287,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '50,67', 'Juros': '10,14', 'Multa': '10,14', 'Total': '70,95', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3016,22 +2400,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '273,46', 'Juros': '20,51', 'Multa': '54,70', 'Total': '348,67', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '51,10', 'Juros': '4,09', 'Multa': '10,22', 'Total': '65,41', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '262,32', 'Juros': '81,32', 'Multa': '52,46', 'Total': '396,10', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,75', 'Juros': '18,52', 'Multa': '11,95', 'Total': '90,22', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '273,45', 'Juros': '54,69', 'Multa': '54,69', 'Total': '382,83', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '499,73', 'Juros': '350,98', 'Multa': '78,92', 'Total': '929,63', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '390,41', 'Juros': '181,05', 'Multa': '66,77', 'Total': '638,23', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '54,11', 'Juros': '10,82', 'Multa': '10,82', 'Total': '75,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3058,22 +2427,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '273,46', 'Juros': '20,51', 'Multa': '54,70', 'Total': '348,67', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '51,10', 'Juros': '4,09', 'Multa': '10,22', 'Total': '65,41', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '262,32', 'Juros': '81,32', 'Multa': '52,46', 'Total': '396,10', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,75', 'Juros': '18,52', 'Multa': '11,95', 'Total': '90,22', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '273,45', 'Juros': '54,69', 'Multa': '54,69', 'Total': '382,83', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '499,73', 'Juros': '350,98', 'Multa': '78,92', 'Total': '929,63', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '390,41', 'Juros': '181,05', 'Multa': '66,77', 'Total': '638,23', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '54,11', 'Juros': '10,82', 'Multa': '10,82', 'Total': '75,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3100,22 +2454,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '273,46', 'Juros': '20,51', 'Multa': '54,70', 'Total': '348,67', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '51,10', 'Juros': '4,09', 'Multa': '10,22', 'Total': '65,41', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '262,32', 'Juros': '81,32', 'Multa': '52,46', 'Total': '396,10', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,75', 'Juros': '18,52', 'Multa': '11,95', 'Total': '90,22', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '273,45', 'Juros': '54,69', 'Multa': '54,69', 'Total': '382,83', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '499,73', 'Juros': '350,98', 'Multa': '78,92', 'Total': '929,63', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '390,41', 'Juros': '181,05', 'Multa': '66,77', 'Total': '638,23', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '54,11', 'Juros': '10,82', 'Multa': '10,82', 'Total': '75,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3142,22 +2481,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 262.32, 81.32, 52.46, 396.1, 1, 0], ['2021', '01', 'TSU - DA', 59.75, 18.52, 11.95, 90.22, 1, 0], ['2022', '01', 'IPTU - DA', 273.45, 54.69, 54.69, 382.83, 1, 0], ['2022', '01', 'TSU - DA', 54.11, 10.82, 10.82, 75.75, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '273,46', 'Juros': '20,51', 'Multa': '54,70', 'Total': '348,67', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '51,10', 'Juros': '4,09', 'Multa': '10,22', 'Total': '65,41', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '262,32', 'Juros': '81,32', 'Multa': '52,46', 'Total': '396,10', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,75', 'Juros': '18,52', 'Multa': '11,95', 'Total': '90,22', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '273,45', 'Juros': '54,69', 'Multa': '54,69', 'Total': '382,83', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '499,73', 'Juros': '350,98', 'Multa': '78,92', 'Total': '929,63', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '390,41', 'Juros': '181,05', 'Multa': '66,77', 'Total': '638,23', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '54,11', 'Juros': '10,82', 'Multa': '10,82', 'Total': '75,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3184,19 +2508,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '578,72', 'Juros': '37,61', 'Multa': '98,39', 'Total': '714,72', 'Vencidas': '4', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '139,82', 'Juros': '11,19', 'Multa': '27,97', 'Total': '178,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '578,72', 'Juros': '115,74', 'Multa': '115,74', 'Total': '810,20', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '640,44', 'Juros': '372,02', 'Multa': '109,54', 'Total': '1.122,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '148,07', 'Juros': '29,61', 'Multa': '29,61', 'Total': '207,29', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3223,19 +2535,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '578,72', 'Juros': '37,61', 'Multa': '98,39', 'Total': '714,72', 'Vencidas': '4', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '139,82', 'Juros': '11,19', 'Multa': '27,97', 'Total': '178,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '578,72', 'Juros': '115,74', 'Multa': '115,74', 'Total': '810,20', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '640,44', 'Juros': '372,02', 'Multa': '109,54', 'Total': '1.122,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '148,07', 'Juros': '29,61', 'Multa': '29,61', 'Total': '207,29', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3262,19 +2562,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '578,72', 'Juros': '37,61', 'Multa': '98,39', 'Total': '714,72', 'Vencidas': '4', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '139,82', 'Juros': '11,19', 'Multa': '27,97', 'Total': '178,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '578,72', 'Juros': '115,74', 'Multa': '115,74', 'Total': '810,20', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '640,44', 'Juros': '372,02', 'Multa': '109,54', 'Total': '1.122,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '148,07', 'Juros': '29,61', 'Multa': '29,61', 'Total': '207,29', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3301,19 +2589,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 578.72, 115.74, 115.74, 810.2, 1, 0], ['2022', '01', 'TSU - DA', 148.07, 29.61, 29.61, 207.29, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '578,72', 'Juros': '37,61', 'Multa': '98,39', 'Total': '714,72', 'Vencidas': '4', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '139,82', 'Juros': '11,19', 'Multa': '27,97', 'Total': '178,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '578,72', 'Juros': '115,74', 'Multa': '115,74', 'Total': '810,20', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '640,44', 'Juros': '372,02', 'Multa': '109,54', 'Total': '1.122,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '148,07', 'Juros': '29,61', 'Multa': '29,61', 'Total': '207,29', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3340,23 +2616,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.356,88', 'Juros': '61,06', 'Multa': '159,43', 'Total': '1.577,37', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.222,40', 'Juros': '378,94', 'Multa': '244,48', 'Total': '1.845,82', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.356,86', 'Juros': '271,37', 'Multa': '271,37', 'Total': '1.899,60', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.222,41', 'Juros': '537,86', 'Multa': '244,48', 'Total': '2.004,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3383,23 +2643,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.356,88', 'Juros': '61,06', 'Multa': '159,43', 'Total': '1.577,37', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.222,40', 'Juros': '378,94', 'Multa': '244,48', 'Total': '1.845,82', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.356,86', 'Juros': '271,37', 'Multa': '271,37', 'Total': '1.899,60', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.222,41', 'Juros': '537,86', 'Multa': '244,48', 'Total': '2.004,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3426,23 +2670,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.356,88', 'Juros': '61,06', 'Multa': '159,43', 'Total': '1.577,37', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.222,40', 'Juros': '378,94', 'Multa': '244,48', 'Total': '1.845,82', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.356,86', 'Juros': '271,37', 'Multa': '271,37', 'Total': '1.899,60', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.222,41', 'Juros': '537,86', 'Multa': '244,48', 'Total': '2.004,75', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3469,15 +2697,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '10,17', 'Multa': '20,35', 'Total': '284,84', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '17,80', 'Multa': '50,86', 'Total': '322,98', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3504,15 +2724,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '10,17', 'Multa': '20,35', 'Total': '284,84', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '17,80', 'Multa': '50,86', 'Total': '322,98', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3539,15 +2751,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '10,17', 'Multa': '20,35', 'Total': '284,84', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '17,80', 'Multa': '50,86', 'Total': '322,98', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3574,15 +2778,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '10,17', 'Multa': '20,35', 'Total': '284,84', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '17,80', 'Multa': '50,86', 'Total': '322,98', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3609,15 +2805,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '10,17', 'Multa': '20,35', 'Total': '284,84', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': '254,32', 'Juros': '17,80', 'Multa': '50,86', 'Total': '322,98', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3644,14 +2832,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '170,92', 'Juros': '0,00', 'Multa': '0,00', 'Total': '170,92', 'Vencidas': '0', 'A Vencer': '1'}]}]</t>
         </is>
       </c>
     </row>
@@ -3678,14 +2859,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '170,92', 'Juros': '0,00', 'Multa': '0,00', 'Total': '170,92', 'Vencidas': '0', 'A Vencer': '1'}]}]</t>
         </is>
       </c>
     </row>
@@ -3712,14 +2886,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '170,92', 'Juros': '0,00', 'Multa': '0,00', 'Total': '170,92', 'Vencidas': '0', 'A Vencer': '1'}]}]</t>
         </is>
       </c>
     </row>
@@ -3746,14 +2913,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '170,92', 'Juros': '0,00', 'Multa': '0,00', 'Total': '170,92', 'Vencidas': '0', 'A Vencer': '1'}]}]</t>
         </is>
       </c>
     </row>
@@ -3780,14 +2940,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '170,92', 'Juros': '0,00', 'Multa': '0,00', 'Total': '170,92', 'Vencidas': '0', 'A Vencer': '1'}]}]</t>
         </is>
       </c>
     </row>
@@ -3814,14 +2967,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>[['Dívida Parcelada']]</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Detalhes': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': '170,92', 'Juros': '0,00', 'Multa': '0,00', 'Total': '170,92', 'Vencidas': '0', 'A Vencer': '1'}]}]</t>
         </is>
       </c>
     </row>
@@ -3848,19 +2994,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
-2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
-2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
-2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'TSU - DA', 151.04, 30.21, 30.21, 211.46, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '962,71', 'Juros': '48,14', 'Multa': '126,53', 'Total': '1.137,38', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '142,63', 'Juros': '11,41', 'Multa': '28,53', 'Total': '182,57', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '962,68', 'Juros': '192,54', 'Multa': '192,54', 'Total': '1.347,76', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '392,20', 'Juros': '112,41', 'Multa': '23,38', 'Total': '527,99', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '151,04', 'Juros': '30,21', 'Multa': '30,21', 'Total': '211,46', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3887,19 +3021,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
-2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
-2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
-2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'TSU - DA', 151.04, 30.21, 30.21, 211.46, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '962,71', 'Juros': '48,14', 'Multa': '126,53', 'Total': '1.137,38', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '142,63', 'Juros': '11,41', 'Multa': '28,53', 'Total': '182,57', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '962,68', 'Juros': '192,54', 'Multa': '192,54', 'Total': '1.347,76', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '392,20', 'Juros': '112,41', 'Multa': '23,38', 'Total': '527,99', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '151,04', 'Juros': '30,21', 'Multa': '30,21', 'Total': '211,46', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3926,19 +3048,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
-2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
-2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
-2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'TSU - DA', 151.04, 30.21, 30.21, 211.46, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '962,71', 'Juros': '48,14', 'Multa': '126,53', 'Total': '1.137,38', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '142,63', 'Juros': '11,41', 'Multa': '28,53', 'Total': '182,57', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '962,68', 'Juros': '192,54', 'Multa': '192,54', 'Total': '1.347,76', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '392,20', 'Juros': '112,41', 'Multa': '23,38', 'Total': '527,99', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '151,04', 'Juros': '30,21', 'Multa': '30,21', 'Total': '211,46', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -3965,15 +3075,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '853,38', 'Juros': '46,94', 'Multa': '119,49', 'Total': '1.019,81', 'Vencidas': '6', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4000,15 +3102,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '853,38', 'Juros': '46,94', 'Multa': '119,49', 'Total': '1.019,81', 'Vencidas': '6', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4035,15 +3129,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '853,38', 'Juros': '46,94', 'Multa': '119,49', 'Total': '1.019,81', 'Vencidas': '6', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4070,15 +3156,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '853,38', 'Juros': '46,94', 'Multa': '119,49', 'Total': '1.019,81', 'Vencidas': '6', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4105,14 +3183,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '8,16', 'Multa': '16,32', 'Total': '228,48', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4139,14 +3210,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '8,16', 'Multa': '16,32', 'Total': '228,48', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4173,14 +3237,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '8,16', 'Multa': '16,32', 'Total': '228,48', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4207,14 +3264,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '8,16', 'Multa': '16,32', 'Total': '228,48', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4241,19 +3291,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '686,80', 'Juros': '41,20', 'Multa': '104,39', 'Total': '832,39', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '105,45', 'Juros': '8,44', 'Multa': '21,09', 'Total': '134,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '686,77', 'Juros': '137,35', 'Multa': '137,35', 'Total': '961,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.125,88', 'Juros': '584,62', 'Multa': '192,56', 'Total': '1.903,06', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '111,67', 'Juros': '22,33', 'Multa': '22,33', 'Total': '156,33', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4280,19 +3318,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '686,80', 'Juros': '41,20', 'Multa': '104,39', 'Total': '832,39', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '105,45', 'Juros': '8,44', 'Multa': '21,09', 'Total': '134,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '686,77', 'Juros': '137,35', 'Multa': '137,35', 'Total': '961,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.125,88', 'Juros': '584,62', 'Multa': '192,56', 'Total': '1.903,06', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '111,67', 'Juros': '22,33', 'Multa': '22,33', 'Total': '156,33', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4319,19 +3345,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '686,80', 'Juros': '41,20', 'Multa': '104,39', 'Total': '832,39', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '105,45', 'Juros': '8,44', 'Multa': '21,09', 'Total': '134,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '686,77', 'Juros': '137,35', 'Multa': '137,35', 'Total': '961,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.125,88', 'Juros': '584,62', 'Multa': '192,56', 'Total': '1.903,06', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '111,67', 'Juros': '22,33', 'Multa': '22,33', 'Total': '156,33', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4358,19 +3372,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 686.77, 137.35, 137.35, 961.47, 1, 0], ['2022', '01', 'TSU - DA', 111.67, 22.33, 22.33, 156.33, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '686,80', 'Juros': '41,20', 'Multa': '104,39', 'Total': '832,39', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '105,45', 'Juros': '8,44', 'Multa': '21,09', 'Total': '134,98', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '686,77', 'Juros': '137,35', 'Multa': '137,35', 'Total': '961,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '1.125,88', 'Juros': '584,62', 'Multa': '192,56', 'Total': '1.903,06', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '111,67', 'Juros': '22,33', 'Multa': '22,33', 'Total': '156,33', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4397,18 +3399,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '857,58', 'Juros': '47,17', 'Multa': '120,06', 'Total': '1.024,81', 'Vencidas': '6', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '84,86', 'Juros': '6,79', 'Multa': '16,97', 'Total': '108,62', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '599,87', 'Juros': '119,97', 'Multa': '119,97', 'Total': '839,81', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '128,38', 'Juros': '25,68', 'Multa': '25,68', 'Total': '179,74', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4435,18 +3426,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '857,58', 'Juros': '47,17', 'Multa': '120,06', 'Total': '1.024,81', 'Vencidas': '6', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '84,86', 'Juros': '6,79', 'Multa': '16,97', 'Total': '108,62', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '599,87', 'Juros': '119,97', 'Multa': '119,97', 'Total': '839,81', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '128,38', 'Juros': '25,68', 'Multa': '25,68', 'Total': '179,74', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4473,18 +3453,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '857,58', 'Juros': '47,17', 'Multa': '120,06', 'Total': '1.024,81', 'Vencidas': '6', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '84,86', 'Juros': '6,79', 'Multa': '16,97', 'Total': '108,62', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '599,87', 'Juros': '119,97', 'Multa': '119,97', 'Total': '839,81', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '128,38', 'Juros': '25,68', 'Multa': '25,68', 'Total': '179,74', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4511,18 +3480,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'IPTU - DA', 599.87, 119.97, 119.97, 839.81, 1, 0], ['2022', '01', 'TSU - DA', 128.38, 25.68, 25.68, 179.74, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '857,58', 'Juros': '47,17', 'Multa': '120,06', 'Total': '1.024,81', 'Vencidas': '6', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '84,86', 'Juros': '6,79', 'Multa': '16,97', 'Total': '108,62', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '599,87', 'Juros': '119,97', 'Multa': '119,97', 'Total': '839,81', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '128,38', 'Juros': '25,68', 'Multa': '25,68', 'Total': '179,74', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4549,28 +3507,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '988,05', 'Juros': '49,40', 'Multa': '129,85', 'Total': '1.167,30', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '172,55', 'Juros': '13,80', 'Multa': '34,51', 'Total': '220,86', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '235,14', 'Multa': '58,79', 'Total': '587,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '155,07', 'Juros': '124,06', 'Multa': '31,01', 'Total': '310,14', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '199,87', 'Multa': '58,79', 'Total': '552,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '76,24', 'Juros': '51,84', 'Multa': '15,25', 'Total': '143,33', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '164,60', 'Multa': '58,79', 'Total': '517,32', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,42', 'Juros': '33,28', 'Multa': '11,88', 'Total': '104,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '129,33', 'Multa': '58,79', 'Total': '482,05', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,71', 'Juros': '26,27', 'Multa': '11,94', 'Total': '97,92', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,94', 'Juros': '91,12', 'Multa': '58,79', 'Total': '443,85', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '56,48', 'Juros': '17,51', 'Multa': '11,30', 'Total': '85,29', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '988,04', 'Juros': '197,61', 'Multa': '197,61', 'Total': '1.383,26', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '182,73', 'Juros': '36,55', 'Multa': '36,55', 'Total': '255,83', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4597,28 +3534,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '988,05', 'Juros': '49,40', 'Multa': '129,85', 'Total': '1.167,30', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '172,55', 'Juros': '13,80', 'Multa': '34,51', 'Total': '220,86', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '235,14', 'Multa': '58,79', 'Total': '587,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '155,07', 'Juros': '124,06', 'Multa': '31,01', 'Total': '310,14', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '199,87', 'Multa': '58,79', 'Total': '552,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '76,24', 'Juros': '51,84', 'Multa': '15,25', 'Total': '143,33', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '164,60', 'Multa': '58,79', 'Total': '517,32', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,42', 'Juros': '33,28', 'Multa': '11,88', 'Total': '104,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '129,33', 'Multa': '58,79', 'Total': '482,05', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,71', 'Juros': '26,27', 'Multa': '11,94', 'Total': '97,92', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,94', 'Juros': '91,12', 'Multa': '58,79', 'Total': '443,85', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '56,48', 'Juros': '17,51', 'Multa': '11,30', 'Total': '85,29', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '988,04', 'Juros': '197,61', 'Multa': '197,61', 'Total': '1.383,26', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '182,73', 'Juros': '36,55', 'Multa': '36,55', 'Total': '255,83', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4645,28 +3561,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '988,05', 'Juros': '49,40', 'Multa': '129,85', 'Total': '1.167,30', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '172,55', 'Juros': '13,80', 'Multa': '34,51', 'Total': '220,86', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '235,14', 'Multa': '58,79', 'Total': '587,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '155,07', 'Juros': '124,06', 'Multa': '31,01', 'Total': '310,14', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '199,87', 'Multa': '58,79', 'Total': '552,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '76,24', 'Juros': '51,84', 'Multa': '15,25', 'Total': '143,33', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '164,60', 'Multa': '58,79', 'Total': '517,32', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,42', 'Juros': '33,28', 'Multa': '11,88', 'Total': '104,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '129,33', 'Multa': '58,79', 'Total': '482,05', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,71', 'Juros': '26,27', 'Multa': '11,94', 'Total': '97,92', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,94', 'Juros': '91,12', 'Multa': '58,79', 'Total': '443,85', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '56,48', 'Juros': '17,51', 'Multa': '11,30', 'Total': '85,29', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '988,04', 'Juros': '197,61', 'Multa': '197,61', 'Total': '1.383,26', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '182,73', 'Juros': '36,55', 'Multa': '36,55', 'Total': '255,83', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4693,28 +3588,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>[[['2017', '01', 'IPTU - DA', 293.93, 235.14, 58.79, 587.86, 1, 0], ['2017', '01', 'TSU - DA', 155.07, 124.06, 31.01, 310.14, 1, 0], ['2018', '01', 'IPTU - DA', 293.93, 199.87, 58.79, 552.59, 1, 0], ['2018', '01', 'TSU - DA', 76.24, 51.84, 15.25, 143.33, 1, 0], ['2019', '01', 'IPTU - DA', 293.93, 164.6, 58.79, 517.32, 1, 0], ['2019', '01', 'TSU - DA', 59.42, 33.28, 11.88, 104.58, 1, 0], ['2020', '01', 'IPTU - DA', 293.93, 129.33, 58.79, 482.05, 1, 0], ['2020', '01', 'TSU - DA', 59.71, 26.27, 11.94, 97.92, 1, 0], ['2021', '01', 'IPTU - DA', 293.94, 91.12, 58.79, 443.85, 1, 0], ['2021', '01', 'TSU - DA', 56.48, 17.51, 11.3, 85.29, 1, 0], ['2022', '01', 'TSU - DA', 182.73, 36.55, 36.55, 255.83, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '988,05', 'Juros': '49,40', 'Multa': '129,85', 'Total': '1.167,30', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '172,55', 'Juros': '13,80', 'Multa': '34,51', 'Total': '220,86', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '235,14', 'Multa': '58,79', 'Total': '587,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '155,07', 'Juros': '124,06', 'Multa': '31,01', 'Total': '310,14', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '199,87', 'Multa': '58,79', 'Total': '552,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '76,24', 'Juros': '51,84', 'Multa': '15,25', 'Total': '143,33', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '164,60', 'Multa': '58,79', 'Total': '517,32', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,42', 'Juros': '33,28', 'Multa': '11,88', 'Total': '104,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,93', 'Juros': '129,33', 'Multa': '58,79', 'Total': '482,05', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '59,71', 'Juros': '26,27', 'Multa': '11,94', 'Total': '97,92', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '293,94', 'Juros': '91,12', 'Multa': '58,79', 'Total': '443,85', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '56,48', 'Juros': '17,51', 'Multa': '11,30', 'Total': '85,29', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '988,04', 'Juros': '197,61', 'Multa': '197,61', 'Total': '1.383,26', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '182,73', 'Juros': '36,55', 'Multa': '36,55', 'Total': '255,83', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4741,26 +3615,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
-2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-Dívida Ativa Situação:
-2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
-2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
-2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
-2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
-2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-Ajuizada Situação:
-2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
-2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
-2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
-2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'TSU - DA', 124.42, 38.57, 24.88, 187.87, 1, 0], ['2022', '01', 'TSU - DA', 112.68, 22.54, 22.54, 157.76, 1, 0], ['2019', '01', 'TSU - DA', 130.9, 73.31, 26.18, 230.39, 1, 0], ['2020', '01', 'TSU - DA', 131.53, 57.88, 26.31, 215.72, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '756,15', 'Juros': '45,37', 'Multa': '114,95', 'Total': '916,47', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '106,40', 'Juros': '8,51', 'Multa': '21,28', 'Total': '136,19', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '324,41', 'Juros': '228,77', 'Multa': '51,23', 'Total': '604,41', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '232,95', 'Multa': '150,29', 'Total': '1.134,69', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '124,42', 'Juros': '38,57', 'Multa': '24,88', 'Total': '187,87', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '756,13', 'Juros': '151,23', 'Multa': '151,23', 'Total': '1.058,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '112,68', 'Juros': '22,54', 'Multa': '22,54', 'Total': '157,76', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '420,81', 'Multa': '150,29', 'Total': '1.322,55', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '130,90', 'Juros': '73,31', 'Multa': '26,18', 'Total': '230,39', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '330,64', 'Multa': '150,29', 'Total': '1.232,38', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '131,53', 'Juros': '57,88', 'Multa': '26,31', 'Total': '215,72', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4787,26 +3642,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
-2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-Dívida Ativa Situação:
-2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
-2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
-2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
-2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
-2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-Ajuizada Situação:
-2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
-2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
-2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
-2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'TSU - DA', 124.42, 38.57, 24.88, 187.87, 1, 0], ['2022', '01', 'TSU - DA', 112.68, 22.54, 22.54, 157.76, 1, 0], ['2019', '01', 'TSU - DA', 130.9, 73.31, 26.18, 230.39, 1, 0], ['2020', '01', 'TSU - DA', 131.53, 57.88, 26.31, 215.72, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '756,15', 'Juros': '45,37', 'Multa': '114,95', 'Total': '916,47', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '106,40', 'Juros': '8,51', 'Multa': '21,28', 'Total': '136,19', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '324,41', 'Juros': '228,77', 'Multa': '51,23', 'Total': '604,41', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '232,95', 'Multa': '150,29', 'Total': '1.134,69', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '124,42', 'Juros': '38,57', 'Multa': '24,88', 'Total': '187,87', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '756,13', 'Juros': '151,23', 'Multa': '151,23', 'Total': '1.058,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '112,68', 'Juros': '22,54', 'Multa': '22,54', 'Total': '157,76', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '420,81', 'Multa': '150,29', 'Total': '1.322,55', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '130,90', 'Juros': '73,31', 'Multa': '26,18', 'Total': '230,39', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '330,64', 'Multa': '150,29', 'Total': '1.232,38', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '131,53', 'Juros': '57,88', 'Multa': '26,31', 'Total': '215,72', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4833,26 +3669,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
-2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-Dívida Ativa Situação:
-2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
-2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
-2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
-2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
-2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-Ajuizada Situação:
-2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
-2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
-2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
-2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'TSU - DA', 124.42, 38.57, 24.88, 187.87, 1, 0], ['2022', '01', 'TSU - DA', 112.68, 22.54, 22.54, 157.76, 1, 0], ['2019', '01', 'TSU - DA', 130.9, 73.31, 26.18, 230.39, 1, 0], ['2020', '01', 'TSU - DA', 131.53, 57.88, 26.31, 215.72, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '756,15', 'Juros': '45,37', 'Multa': '114,95', 'Total': '916,47', 'Vencidas': '5', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '106,40', 'Juros': '8,51', 'Multa': '21,28', 'Total': '136,19', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': '324,41', 'Juros': '228,77', 'Multa': '51,23', 'Total': '604,41', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '232,95', 'Multa': '150,29', 'Total': '1.134,69', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '124,42', 'Juros': '38,57', 'Multa': '24,88', 'Total': '187,87', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '756,13', 'Juros': '151,23', 'Multa': '151,23', 'Total': '1.058,59', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '112,68', 'Juros': '22,54', 'Multa': '22,54', 'Total': '157,76', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '420,81', 'Multa': '150,29', 'Total': '1.322,55', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '130,90', 'Juros': '73,31', 'Multa': '26,18', 'Total': '230,39', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '751,45', 'Juros': '330,64', 'Multa': '150,29', 'Total': '1.232,38', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '131,53', 'Juros': '57,88', 'Multa': '26,31', 'Total': '215,72', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4879,24 +3696,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-Dívida Ativa Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 611,92 189,70 122,38 924,00 1 0
-2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>[[['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], ['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2021', '01', 'ITU - DA', 611.92, 189.7, 122.38, 924.0, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2022', '01', 'ITU - DA', 679.23, 135.85, 135.85, 950.93, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '679,25', 'Juros': '40,75', 'Multa': '103,25', 'Total': '823,25', 'Vencidas': '5', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '611,92', 'Juros': '269,24', 'Multa': '122,38', 'Total': '1.003,54', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '611,92', 'Juros': '189,70', 'Multa': '122,38', 'Total': '924,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '26,43', 'Multa': '40,67', 'Total': '270,43', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '679,23', 'Juros': '135,85', 'Multa': '135,85', 'Total': '950,93', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4923,24 +3723,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-Dívida Ativa Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 611,92 189,70 122,38 924,00 1 0
-2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>[[['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], ['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2021', '01', 'ITU - DA', 611.92, 189.7, 122.38, 924.0, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2022', '01', 'ITU - DA', 679.23, 135.85, 135.85, 950.93, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '679,25', 'Juros': '40,75', 'Multa': '103,25', 'Total': '823,25', 'Vencidas': '5', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '611,92', 'Juros': '269,24', 'Multa': '122,38', 'Total': '1.003,54', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '611,92', 'Juros': '189,70', 'Multa': '122,38', 'Total': '924,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '26,43', 'Multa': '40,67', 'Total': '270,43', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '679,23', 'Juros': '135,85', 'Multa': '135,85', 'Total': '950,93', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -4967,24 +3750,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-Dívida Ativa Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 611,92 189,70 122,38 924,00 1 0
-2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>[[['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], ['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2021', '01', 'ITU - DA', 611.92, 189.7, 122.38, 924.0, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2022', '01', 'ITU - DA', 679.23, 135.85, 135.85, 950.93, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '679,25', 'Juros': '40,75', 'Multa': '103,25', 'Total': '823,25', 'Vencidas': '5', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '611,92', 'Juros': '269,24', 'Multa': '122,38', 'Total': '1.003,54', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '611,92', 'Juros': '189,70', 'Multa': '122,38', 'Total': '924,00', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '26,43', 'Multa': '40,67', 'Total': '270,43', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '679,23', 'Juros': '135,85', 'Multa': '135,85', 'Total': '950,93', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5011,20 +3777,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
-2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
-2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
-2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
-2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 288.47, 89.42, 57.69, 435.58, 1, 0], ['2021', '01', 'TSU - DA', 88.98, 27.58, 17.8, 134.36, 1, 0], ['2022', '01', 'IPTU - DA', 290.52, 58.1, 58.1, 406.72, 1, 0], ['2022', '01', 'TSU - DA', 80.58, 16.12, 16.12, 112.82, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '290,52', 'Juros': '21,79', 'Multa': '58,10', 'Total': '370,41', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '76,09', 'Juros': '6,09', 'Multa': '15,22', 'Total': '97,40', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '288,47', 'Juros': '89,42', 'Multa': '57,69', 'Total': '435,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '88,98', 'Juros': '27,58', 'Multa': '17,80', 'Total': '134,36', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '290,52', 'Juros': '58,10', 'Multa': '58,10', 'Total': '406,72', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '80,58', 'Juros': '16,12', 'Multa': '16,12', 'Total': '112,82', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5051,20 +3804,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
-2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
-2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
-2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
-2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 288.47, 89.42, 57.69, 435.58, 1, 0], ['2021', '01', 'TSU - DA', 88.98, 27.58, 17.8, 134.36, 1, 0], ['2022', '01', 'IPTU - DA', 290.52, 58.1, 58.1, 406.72, 1, 0], ['2022', '01', 'TSU - DA', 80.58, 16.12, 16.12, 112.82, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '290,52', 'Juros': '21,79', 'Multa': '58,10', 'Total': '370,41', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '76,09', 'Juros': '6,09', 'Multa': '15,22', 'Total': '97,40', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '288,47', 'Juros': '89,42', 'Multa': '57,69', 'Total': '435,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '88,98', 'Juros': '27,58', 'Multa': '17,80', 'Total': '134,36', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '290,52', 'Juros': '58,10', 'Multa': '58,10', 'Total': '406,72', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '80,58', 'Juros': '16,12', 'Multa': '16,12', 'Total': '112,82', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5091,20 +3831,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
-2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-Dívida Ativa Situação:
-2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
-2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
-2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
-2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'IPTU - DA', 288.47, 89.42, 57.69, 435.58, 1, 0], ['2021', '01', 'TSU - DA', 88.98, 27.58, 17.8, 134.36, 1, 0], ['2022', '01', 'IPTU - DA', 290.52, 58.1, 58.1, 406.72, 1, 0], ['2022', '01', 'TSU - DA', 80.58, 16.12, 16.12, 112.82, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': '290,52', 'Juros': '21,79', 'Multa': '58,10', 'Total': '370,41', 'Vencidas': '2', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': '76,09', 'Juros': '6,09', 'Multa': '15,22', 'Total': '97,40', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '288,47', 'Juros': '89,42', 'Multa': '57,69', 'Total': '435,58', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '88,98', 'Juros': '27,58', 'Multa': '17,80', 'Total': '134,36', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': '290,52', 'Juros': '58,10', 'Multa': '58,10', 'Total': '406,72', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': '80,58', 'Juros': '16,12', 'Multa': '16,12', 'Total': '112,82', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5131,20 +3858,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.021,38', 'Juros': '204,28', 'Multa': '204,28', 'Total': '1.429,94', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5171,20 +3885,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-</t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.021,38', 'Juros': '204,28', 'Multa': '204,28', 'Total': '1.429,94', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5211,20 +3912,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.021,38', 'Juros': '204,28', 'Multa': '204,28', 'Total': '1.429,94', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5251,20 +3939,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.021,38', 'Juros': '204,28', 'Multa': '204,28', 'Total': '1.429,94', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5291,20 +3966,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>[[['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], 'Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '204,00', 'Juros': '14,28', 'Multa': '40,80', 'Total': '259,08', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.021,38', 'Juros': '204,28', 'Multa': '204,28', 'Total': '1.429,94', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5331,17 +3993,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-</t>
-        </is>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '898,80', 'Juros': '49,43', 'Multa': '125,82', 'Total': '1.074,05', 'Vencidas': '6', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5368,17 +4020,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '898,80', 'Juros': '49,43', 'Multa': '125,82', 'Total': '1.074,05', 'Vencidas': '6', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5405,17 +4047,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-</t>
-        </is>
-      </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '898,80', 'Juros': '49,43', 'Multa': '125,82', 'Total': '1.074,05', 'Vencidas': '6', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '203,33', 'Juros': '28,47', 'Multa': '40,67', 'Total': '272,47', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5442,16 +4074,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': '897,02', 'Juros': '0,00', 'Multa': '0,00', 'Total': '897,02', 'Vencidas': '0', 'A Vencer': '2'}]}]</t>
         </is>
       </c>
     </row>
@@ -5478,16 +4101,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': '897,02', 'Juros': '0,00', 'Multa': '0,00', 'Total': '897,02', 'Vencidas': '0', 'A Vencer': '2'}]}]</t>
         </is>
       </c>
     </row>
@@ -5514,16 +4128,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-</t>
-        </is>
-      </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': '897,02', 'Juros': '0,00', 'Multa': '0,00', 'Total': '897,02', 'Vencidas': '0', 'A Vencer': '2'}]}]</t>
         </is>
       </c>
     </row>
@@ -5550,16 +4155,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-</t>
-        </is>
-      </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>[['Dívida Corrente']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.021,37', 'Juros': '51,07', 'Multa': '134,22', 'Total': '1.206,66', 'Vencidas': '7', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': '897,02', 'Juros': '0,00', 'Multa': '0,00', 'Total': '897,02', 'Vencidas': '0', 'A Vencer': '2'}]}]</t>
         </is>
       </c>
     </row>
@@ -5586,20 +4182,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-</t>
-        </is>
-      </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '15,42', 'Multa': '44,06', 'Total': '279,80', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '6,61', 'Multa': '17,63', 'Total': '244,56', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.003,38', 'Juros': '50,17', 'Multa': '131,89', 'Total': '1.185,44', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '08', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '26,35', 'Multa': '43,92', 'Total': '289,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '30,74', 'Multa': '43,92', 'Total': '294,25', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5626,20 +4209,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-</t>
-        </is>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '15,42', 'Multa': '44,06', 'Total': '279,80', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '6,61', 'Multa': '17,63', 'Total': '244,56', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.003,38', 'Juros': '50,17', 'Multa': '131,89', 'Total': '1.185,44', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '08', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '26,35', 'Multa': '43,92', 'Total': '289,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '30,74', 'Multa': '43,92', 'Total': '294,25', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5666,20 +4236,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-</t>
-        </is>
-      </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '15,42', 'Multa': '44,06', 'Total': '279,80', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '6,61', 'Multa': '17,63', 'Total': '244,56', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.003,38', 'Juros': '50,17', 'Multa': '131,89', 'Total': '1.185,44', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '08', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '26,35', 'Multa': '43,92', 'Total': '289,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '30,74', 'Multa': '43,92', 'Total': '294,25', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5706,20 +4263,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-</t>
-        </is>
-      </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '15,42', 'Multa': '44,06', 'Total': '279,80', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '6,61', 'Multa': '17,63', 'Total': '244,56', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.003,38', 'Juros': '50,17', 'Multa': '131,89', 'Total': '1.185,44', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '08', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '26,35', 'Multa': '43,92', 'Total': '289,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '30,74', 'Multa': '43,92', 'Total': '294,25', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5746,20 +4290,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-</t>
-        </is>
-      </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>[['Dívida Ativa']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '15,42', 'Multa': '44,06', 'Total': '279,80', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': '220,32', 'Juros': '6,61', 'Multa': '17,63', 'Total': '244,56', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.003,38', 'Juros': '50,17', 'Multa': '131,89', 'Total': '1.185,44', 'Vencidas': '7', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2022', 'Mês': '08', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '26,35', 'Multa': '43,92', 'Total': '289,86', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '219,59', 'Juros': '30,74', 'Multa': '43,92', 'Total': '294,25', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>
@@ -5786,24 +4317,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.683,92 75,76 197,87 1.957,55 8 0
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.517,01 470,27 303,40 2.290,68 1 0
-2022 07 Capin. RoçaD.A 216,32 23,80 43,26 283,38 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.683,88 336,78 336,78 2.357,44 1 0
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.517,01 667,48 303,40 2.487,89 1 0
-</t>
-        </is>
-      </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>[[['2021', '01', 'CIP - DA', 29.61, 9.18, 5.92, 44.71, 1, 0], ['2022', '01', 'CIP - DA', 24.27, 4.85, 4.85, 33.97, 1, 0], ['2020', '01', 'CIP - DA', 32.47, 14.29, 6.49, 53.25, 1, 0], 'Ajuizada']]</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': '26,52', 'Juros': '2,12', 'Multa': '5,30', 'Total': '33,94', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': '1.683,92', 'Juros': '75,76', 'Multa': '197,87', 'Total': '1.957,55', 'Vencidas': '8', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '29,61', 'Juros': '9,18', 'Multa': '5,92', 'Total': '44,71', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.517,01', 'Juros': '470,27', 'Multa': '303,40', 'Total': '2.290,68', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': '216,32', 'Juros': '23,80', 'Multa': '43,26', 'Total': '283,38', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '24,27', 'Juros': '4,85', 'Multa': '4,85', 'Total': '33,97', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.683,88', 'Juros': '336,78', 'Multa': '336,78', 'Total': '2.357,44', 'Vencidas': '1', 'A Vencer': '0'}]}, {'Situação': 'Dívida Corrente', 'Detalhes': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': '32,47', 'Juros': '14,29', 'Multa': '6,49', 'Total': '53,25', 'Vencidas': '1', 'A Vencer': '0'}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': '1.517,01', 'Juros': '667,48', 'Multa': '303,40', 'Total': '2.487,89', 'Vencidas': '1', 'A Vencer': '0'}]}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
extração e atribuição de dados completa
</commit_message>
<xml_diff>
--- a/prototipos/DataInput/Relatório.xlsx
+++ b/prototipos/DataInput/Relatório.xlsx
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Origem:</t>
+          <t>Origem</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Inscrição:</t>
+          <t>Inscrição</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Matrícula:</t>
+          <t>Endereço</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Endereço:</t>
+          <t>Matrícula</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Dados Brutos</t>
+          <t>Dívidas</t>
         </is>
       </c>
     </row>
@@ -473,19 +473,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JOSE NETO PARANHOS         0 QD. 41 LT. 62 BAIRRO JUNDIAI, Qt.Qd.Lt.SubLt. 41 62101.165.0706.000 </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>101.165.0706.000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Rua JOSE NETO PARANHOS         0 QD. 41 LT. 62 BAIRRO JUNDIAI, Qt.Qd.Lt.SubLt. 41 62</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Divida': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': 2327.45, 'Juros': 14.19, 'Multa': 18.89, 'Total': '2360.53', 'Vencidas': 2, 'A Vencer': 3}], 'Total Origem': 2360.53}]</t>
         </is>
       </c>
     </row>
@@ -502,19 +500,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida PB 1          S/N QD: 30 LT: 14 PARQUE BRASILIA I E II ETAPA, Qt.Qd.Lt.SubLt. 30 14104.063.0283.001 </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>104.063.0283.001</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Avenida PB 1          S/N QD: 30 LT: 14 PARQUE BRASILIA I E II ETAPA, Qt.Qd.Lt.SubLt. 30 14</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 581.84, 'Juros': 37.82, 'Multa': 98.91, 'Total': '718.57', 'Vencidas': 4, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 81.06, 'Juros': 6.48, 'Multa': 16.21, 'Total': '103.75', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 577.69, 'Juros': 179.08, 'Multa': 115.54, 'Total': '872.31', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 94.79, 'Juros': 29.38, 'Multa': 18.96, 'Total': '143.13', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 581.83, 'Juros': 116.37, 'Multa': 116.37, 'Total': '814.57', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 85.84, 'Juros': 17.17, 'Multa': 17.17, 'Total': '120.18', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2772.51}]</t>
         </is>
       </c>
     </row>
@@ -531,19 +527,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CEREJEIRAS         0 QD- 19 LT- 13 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 13104.433.0025.000 </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>104.433.0025.000</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Avenida CEREJEIRAS         0 QD- 19 LT- 13 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 13</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': 590.62, 'Juros': 29.53, 'Multa': 47.25, 'Total': '667.40', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '11', 'Tributo': 'Capinação e Roç', 'Valor Atual': 590.62, 'Juros': 0.0, 'Multa': 0.0, 'Total': '590.62', 'Vencidas': 0, 'A Vencer': 1}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 555.88, 'Juros': 61.15, 'Multa': 111.18, 'Total': '728.21', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1986.23}]</t>
         </is>
       </c>
     </row>
@@ -560,19 +554,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CEREJEIRAS         0 QD- 19 LT- 12 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 12104.433.0041.000 </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>104.433.0041.000</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Avenida CEREJEIRAS         0 QD- 19 LT- 12 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 12</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '11', 'Tributo': 'Capinação e Roç', 'Valor Atual': 424.95, 'Juros': 0.0, 'Multa': 0.0, 'Total': '424.95', 'Vencidas': 0, 'A Vencer': 1}, {'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': 424.95, 'Juros': 21.25, 'Multa': 34.0, 'Total': '480.20', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 399.96, 'Juros': 44.0, 'Multa': 79.99, 'Total': '523.95', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1429.1}]</t>
         </is>
       </c>
     </row>
@@ -589,19 +581,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CEREJEIRAS         0 QD- 19 LT- 11 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 11104.433.0057.000 </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>104.433.0057.000</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Avenida CEREJEIRAS         0 QD- 19 LT- 11 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 11</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelam/Div/Aj 2.327,45 14,19 18,89 2.360,53 2 3
-2.327,45 14,19 18,89 2.360,53 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': 431.12, 'Juros': 21.56, 'Multa': 34.49, 'Total': '487.17', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '11', 'Tributo': 'Capinação e Roç', 'Valor Atual': 431.12, 'Juros': 0.0, 'Multa': 0.0, 'Total': '431.12', 'Vencidas': 0, 'A Vencer': 1}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 405.76, 'Juros': 44.63, 'Multa': 81.15, 'Total': '531.54', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1449.83}]</t>
         </is>
       </c>
     </row>
@@ -618,19 +608,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida UNIVERSITARIA      2045 SALA: 02 RESIDENCIAL ARAUJOVILLE, Qt.Qd.Lt.SubLt. 01 14/17105.279.0351.002 </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>105.279.0351.002</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Avenida UNIVERSITARIA      2045 SALA: 02 RESIDENCIAL ARAUJOVILLE, Qt.Qd.Lt.SubLt. 01 14/17</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Divida': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': 3109.6, 'Juros': 4.63, 'Multa': 18.44, 'Total': '3132.67', 'Vencidas': 2, 'A Vencer': 5}], 'Total Origem': 3132.67}]</t>
         </is>
       </c>
     </row>
@@ -647,19 +635,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua TARSILA DO AMARAL         0 QD.13  LT.17 CONDOMÍNO RESIDENCIAL  BELAS ARTES, Qt.Qd.Lt.SubLt. 13 17105.322.0262.000 </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>105.322.0262.000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Rua TARSILA DO AMARAL         0 QD.13  LT.17 CONDOMÍNO RESIDENCIAL  BELAS ARTES, Qt.Qd.Lt.SubLt. 13 17</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 3498.6, 'Juros': 699.72, 'Multa': 699.72, 'Total': '4898.04', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4932.01}]</t>
         </is>
       </c>
     </row>
@@ -676,19 +662,17 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua GT 16         0 QD. 23 LT. 19 CONDOMÍNIO RESIDENCIAL GRAND TRIANON, Qt.Qd.Lt.SubLt. 23 19105.350.0307.000 </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>105.350.0307.000</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Rua GT 16         0 QD. 23 LT. 19 CONDOMÍNIO RESIDENCIAL GRAND TRIANON, Qt.Qd.Lt.SubLt. 23 19</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 2044.64, 'Juros': 92.01, 'Multa': 240.27, 'Total': '2376.92', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 2410.86}]</t>
         </is>
       </c>
     </row>
@@ -705,19 +689,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.02 LT. 14 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 14105.373.0166.000 </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>105.373.0166.000</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.02 LT. 14 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 14</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -734,19 +716,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-18         0 QD.02 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 23105.373.0334.000 </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>105.373.0334.000</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Rua CJ-18         0 QD.02 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 23</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1778.57}]</t>
         </is>
       </c>
     </row>
@@ -763,19 +743,17 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-18         0 QD.02 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 25105.373.0358.000 </t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>105.373.0358.000</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Rua CJ-18         0 QD.02 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 25</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 3.109,60 4,63 18,44 3.132,67 2 5
-3.109,60 4,63 18,44 3.132,67 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -792,20 +770,17 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CJ-02         0 QD.03 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 07105.374.0090.000 </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>105.374.0090.000</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Avenida CJ-02         0 QD.03 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 07</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -822,20 +797,17 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-18         0 QD.03 LT. 24 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 24105.374.0330.000 </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>105.374.0330.000</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Rua CJ-18         0 QD.03 LT. 24 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 24</t>
-        </is>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -852,20 +824,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida AV. CJ-01         0 QD.06 LT. 13 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 13105.377.0199.000 </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>105.377.0199.000</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Avenida AV. CJ-01         0 QD.06 LT. 13 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 13</t>
-        </is>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 2346.96, 'Juros': 105.61, 'Multa': 275.76, 'Total': '2728.33', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 2346.91, 'Juros': 375.51, 'Multa': 469.38, 'Total': '3191.80', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 5987.07}]</t>
         </is>
       </c>
     </row>
@@ -882,20 +851,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida AV. CJ-01         0 QD.06 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 16105.377.0235.000 </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>105.377.0235.000</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Avenida AV. CJ-01         0 QD.06 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 16</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -912,19 +878,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-06         0 QD.11 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 04105.382.0049.000 </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>105.382.0049.000</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Rua CJ-06         0 QD.11 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 04</t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 320.88, 'Juros': 4.81, 'Multa': 16.05, 'Total': '341.74', 'Vencidas': 2, 'A Vencer': 0}], 'Total Origem': 341.74}]</t>
         </is>
       </c>
     </row>
@@ -941,19 +905,17 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-06         0 QD.11 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 09105.382.0109.000 </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>105.382.0109.000</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Rua CJ-06         0 QD.11 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 09</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -970,19 +932,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-05         0 QD.11 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 16105.382.0235.000 </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>105.382.0235.000</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Rua CJ-05         0 QD.11 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 16</t>
-        </is>
-      </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -999,19 +959,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-05         0 QD.11 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 17105.382.0247.000 </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>105.382.0247.000</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Rua CJ-05         0 QD.11 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 17</t>
-        </is>
-      </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -1028,19 +986,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-06         0 QD.12 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 12 18105.383.0259.000 </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>105.383.0259.000</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Rua CJ-06         0 QD.12 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 12 18</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -1057,19 +1013,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-11         0 QD.13 LT. 11 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 13 11105.384.0133.000 </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>105.384.0133.000</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Rua CJ-11         0 QD.13 LT. 11 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 13 11</t>
-        </is>
-      </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 ITU 320,88 4,81 16,05 341,74 2 0
-320,88 4,81 16,05 341,74 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.23, 'Juros': 4.68, 'Multa': 5.85, 'Total': '39.76', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1785.33}]</t>
         </is>
       </c>
     </row>
@@ -1086,20 +1040,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-14         0 QD.16 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 16 05105.387.0061.000 </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>105.387.0061.000</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Rua CJ-14         0 QD.16 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 16 05</t>
-        </is>
-      </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 31.8, 'Juros': 2.54, 'Multa': 6.36, 'Total': '40.70', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1532.82}]</t>
         </is>
       </c>
     </row>
@@ -1116,20 +1067,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-15         0 QD.17 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 17 04105.388.0049.000 </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>105.388.0049.000</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Rua CJ-15         0 QD.17 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 17 04</t>
-        </is>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -1146,20 +1094,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-15         0 QD.18 LT. 21 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 18 21105.389.0295.000 </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>105.389.0295.000</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Rua CJ-15         0 QD.18 LT. 21 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 18 21</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -1176,20 +1121,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-17         0 QD.20 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 20 23105.391.0328.000 </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>105.391.0328.000</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Rua CJ-17         0 QD.20 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 20 23</t>
-        </is>
-      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -1206,20 +1148,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-22         0 QD.21 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 04105.392.0209.000 </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>105.392.0209.000</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Rua CJ-22         0 QD.21 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 04</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1289.92, 'Juros': 58.04, 'Multa': 151.57, 'Total': '1499.53', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1533.47}]</t>
         </is>
       </c>
     </row>
@@ -1236,20 +1175,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-22         0 QD.21 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 05105.392.0222.000 </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>105.392.0222.000</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Rua CJ-22         0 QD.21 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 05</t>
-        </is>
-      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 31,80 2,54 6,36 40,70 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.315,32 60,30 157,20 1.532,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1289.92, 'Juros': 58.04, 'Multa': 151.57, 'Total': '1499.53', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1533.47}]</t>
         </is>
       </c>
     </row>
@@ -1266,20 +1202,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-22         0 QD.21 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 06105.392.0235.000 </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>105.392.0235.000</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Rua CJ-22         0 QD.21 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 06</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1289.92, 'Juros': 58.04, 'Multa': 151.57, 'Total': '1499.53', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1533.47}]</t>
         </is>
       </c>
     </row>
@@ -1296,20 +1229,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-24         0 QD.22 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 22 17105.393.0274.000 </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>105.393.0274.000</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Rua CJ-24         0 QD.22 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 22 17</t>
-        </is>
-      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1289.52, 'Juros': 58.02, 'Multa': 151.5, 'Total': '1499.04', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1289.49, 'Juros': 206.32, 'Multa': 257.9, 'Total': '1753.71', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3319.69}]</t>
         </is>
       </c>
     </row>
@@ -1326,20 +1256,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-24         0 QD.23 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 01105.394.0013.000 </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
           <t>105.394.0013.000</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Rua CJ-24         0 QD.23 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 01</t>
-        </is>
-      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Divida': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': 838.09, 'Juros': 0.0, 'Multa': 0.0, 'Total': '838.09', 'Vencidas': 0, 'A Vencer': 2}], 'Total Origem': 838.09}]</t>
         </is>
       </c>
     </row>
@@ -1356,20 +1283,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-25         0 QD.23 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 19105.394.0306.000 </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
           <t>105.394.0306.000</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Rua CJ-25         0 QD.23 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 19</t>
-        </is>
-      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1289.52, 'Juros': 58.02, 'Multa': 151.5, 'Total': '1499.04', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1532.98}]</t>
         </is>
       </c>
     </row>
@@ -1386,20 +1310,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-14         0 QD. 25 LT. 15 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 25 15105.396.0223.000 </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
           <t>105.396.0223.000</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Rua CJ-14         0 QD. 25 LT. 15 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 25 15</t>
-        </is>
-      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.289,92 58,04 151,57 1.499,53 8 0
-1.316,44 60,16 156,87 1.533,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -1416,20 +1337,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-13         0 QD.27 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 27 03105.398.0066.000 </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>105.398.0066.000</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Rua CJ-13         0 QD.27 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 27 03</t>
-        </is>
-      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -1446,20 +1364,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CJ-02         0 QD.34 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 34 09105.405.0165.000 </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>105.405.0165.000</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Avenida CJ-02         0 QD.34 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 34 09</t>
-        </is>
-      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1325.6, 'Juros': 59.66, 'Multa': 155.77, 'Total': '1541.03', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1325.6, 'Juros': 212.1, 'Multa': 265.12, 'Total': '1802.82', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3410.79}]</t>
         </is>
       </c>
     </row>
@@ -1476,20 +1391,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 18105.407.0274.000 </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>105.407.0274.000</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 18</t>
-        </is>
-      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1540.24, 'Juros': 69.32, 'Multa': 180.98, 'Total': '1790.54', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1540.21, 'Juros': 246.43, 'Multa': 308.04, 'Total': '2094.68', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3952.16}]</t>
         </is>
       </c>
     </row>
@@ -1506,20 +1418,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 19105.407.0289.000 </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>105.407.0289.000</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 19</t>
-        </is>
-      </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1540.24, 'Juros': 69.32, 'Multa': 180.98, 'Total': '1790.54', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1540.21, 'Juros': 246.43, 'Multa': 308.04, 'Total': '2094.68', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3952.16}]</t>
         </is>
       </c>
     </row>
@@ -1536,20 +1445,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-25         0 QD.37 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 37 09105.408.0116.000 </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t>105.408.0116.000</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Rua CJ-25         0 QD.37 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 37 09</t>
-        </is>
-      </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -1566,20 +1472,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-25         0 QD.38 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 07105.409.0090.000 </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t>105.409.0090.000</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Rua CJ-25         0 QD.38 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 07</t>
-        </is>
-      </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -1596,20 +1499,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.38 LT. 33 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 33105.409.0458.000 </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>105.409.0458.000</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.38 LT. 33 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 33</t>
-        </is>
-      </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1283.51, 'Juros': 205.36, 'Multa': 256.7, 'Total': '1745.57', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3304.63}]</t>
         </is>
       </c>
     </row>
@@ -1626,20 +1526,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.40 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 40 25105.411.0358.000 </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>105.411.0358.000</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.40 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 40 25</t>
-        </is>
-      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 2246.14, 'Juros': 359.38, 'Multa': 449.23, 'Total': '3054.75', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4613.8099999999995}]</t>
         </is>
       </c>
     </row>
@@ -1656,20 +1553,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-25         0 QD.41 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 41 09105.412.0117.000 </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
           <t>105.412.0117.000</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Rua CJ-25         0 QD.41 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 41 09</t>
-        </is>
-      </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -1686,20 +1580,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-26         0 QD.43 LT. 20 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 43 20105.414.0298.000 </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>105.414.0298.000</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Rua CJ-26         0 QD.43 LT. 20 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 43 20</t>
-        </is>
-      </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1283.52, 'Juros': 57.76, 'Multa': 150.84, 'Total': '1492.12', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1526.06}]</t>
         </is>
       </c>
     </row>
@@ -1716,20 +1607,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.47 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 47 01105.418.0015.000 </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>105.418.0015.000</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.47 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 47 01</t>
-        </is>
-      </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 2246.16, 'Juros': 101.08, 'Multa': 263.91, 'Total': '2611.15', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 2246.14, 'Juros': 359.38, 'Multa': 449.23, 'Total': '3054.75', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 5732.84}]</t>
         </is>
       </c>
     </row>
@@ -1746,20 +1634,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.48 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 48 01105.419.0025.000 </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>105.419.0025.000</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 QD.48 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 48 01</t>
-        </is>
-      </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 2246.16, 'Juros': 101.08, 'Multa': 263.91, 'Total': '2611.15', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 2246.14, 'Juros': 359.38, 'Multa': 449.23, 'Total': '3054.75', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 5732.84}]</t>
         </is>
       </c>
     </row>
@@ -1776,20 +1661,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-29         0 QD.49 LT. 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 49 02105.420.0059.000 </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>105.420.0059.000</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Rua CJ-29         0 QD.49 LT. 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 49 02</t>
-        </is>
-      </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1711.36, 'Juros': 77.02, 'Multa': 201.06, 'Total': '1989.44', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 2023.38}]</t>
         </is>
       </c>
     </row>
@@ -1806,20 +1688,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-30         0 QD.50 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 50 06105.421.0148.000 </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
           <t>105.421.0148.000</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Rua CJ-30         0 QD.50 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 50 06</t>
-        </is>
-      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.283,52 57,76 150,84 1.492,12 8 0
-1.310,04 59,88 156,14 1.526,06 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 235.31, 'Juros': 30.59, 'Multa': 47.06, 'Total': '312.96', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 312.96}]</t>
         </is>
       </c>
     </row>
@@ -1836,20 +1715,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-35         0 QD.55 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 55 03105.426.0070.000 </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
           <t>105.426.0070.000</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Rua CJ-35         0 QD.55 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 55 03</t>
-        </is>
-      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1711.36, 'Juros': 77.02, 'Multa': 201.06, 'Total': '1989.44', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 2023.38}]</t>
         </is>
       </c>
     </row>
@@ -1866,20 +1742,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 APM 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 01105.427.0077.000 </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
           <t>105.427.0077.000</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 APM 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 01</t>
-        </is>
-      </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 65351.52, 'Juros': 2940.84, 'Multa': 7678.83, 'Total': '75971.19', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 65351.54, 'Juros': 10456.25, 'Multa': 13070.31, 'Total': '88878.10', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 164916.23}]</t>
         </is>
       </c>
     </row>
@@ -1896,20 +1769,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ - 08         0 APM 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 02105.428.0040.000 </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
           <t>105.428.0040.000</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Rua CJ - 08         0 APM 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 02</t>
-        </is>
-      </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 35175.84, 'Juros': 1582.92, 'Multa': 4133.18, 'Total': '40891.94', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 35175.86, 'Juros': 5628.14, 'Multa': 7035.17, 'Total': '47839.17', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 88798.05}]</t>
         </is>
       </c>
     </row>
@@ -1926,20 +1796,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ- 07         0 APM 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 03105.429.0040.000 </t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>105.429.0040.000</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Rua CJ- 07         0 APM 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 03</t>
-        </is>
-      </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 25125.6, 'Juros': 1130.66, 'Multa': 2952.27, 'Total': '29208.53', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 25125.61, 'Juros': 4020.1, 'Multa': 5025.12, 'Total': '34170.83', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 63446.3}]</t>
         </is>
       </c>
     </row>
@@ -1956,20 +1823,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ - 08         0 APM 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 04105.430.0040.000 </t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>105.430.0040.000</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Rua CJ - 08         0 APM 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 04</t>
-        </is>
-      </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.711,36 77,02 201,06 1.989,44 8 0
-1.737,88 79,14 206,36 2.023,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 35175.84, 'Juros': 1582.92, 'Multa': 4133.18, 'Total': '40891.94', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 35175.86, 'Juros': 5628.14, 'Multa': 7035.17, 'Total': '47839.17', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 88798.05}]</t>
         </is>
       </c>
     </row>
@@ -1986,24 +1850,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ- 07         0 AREA APM 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 05105.431.0040.000 </t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>105.431.0040.000</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Rua CJ- 07         0 AREA APM 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 05</t>
-        </is>
-      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 35175.84, 'Juros': 1582.92, 'Multa': 4133.18, 'Total': '40891.94', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 35175.86, 'Juros': 5628.14, 'Multa': 7035.17, 'Total': '47839.17', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 88798.05}]</t>
         </is>
       </c>
     </row>
@@ -2020,24 +1877,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ-16         0 APM 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 06105.432.0109.000 </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
           <t>105.432.0109.000</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Rua CJ-16         0 APM 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 06</t>
-        </is>
-      </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 84342.64, 'Juros': 3795.42, 'Multa': 9910.29, 'Total': '98048.35', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 84342.61, 'Juros': 13494.82, 'Multa': 16868.52, 'Total': '114705.95', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 212821.24}]</t>
         </is>
       </c>
     </row>
@@ -2054,24 +1904,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ- 28         0 APM 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 07105.433.0073.000 </t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
           <t>105.433.0073.000</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Rua CJ- 28         0 APM 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 07</t>
-        </is>
-      </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 131651.04, 'Juros': 5924.3, 'Multa': 15469.01, 'Total': '153044.35', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 131651.04, 'Juros': 21064.17, 'Multa': 26330.21, 'Total': '179045.42', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 332156.71}]</t>
         </is>
       </c>
     </row>
@@ -2088,24 +1931,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CJ- 20         0 AREA APM 08 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM08105.434.0030.000 </t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
           <t>105.434.0030.000</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Rua CJ- 20         0 AREA APM 08 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM08</t>
-        </is>
-      </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 35.175,84 1.582,92 4.133,18 40.891,94 8 0
-35.202,36 1.585,04 4.138,48 40.925,88 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 35.175,86 5.628,14 7.035,17 47.839,17 1 0
-35.200,13 5.632,02 7.040,02 47.872,17 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 26132.64, 'Juros': 1175.97, 'Multa': 3070.61, 'Total': '30379.22', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 26132.66, 'Juros': 4181.23, 'Multa': 5226.53, 'Total': '35540.42', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 65986.58}]</t>
         </is>
       </c>
     </row>
@@ -2122,24 +1958,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 AREA APM 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 09105.435.0040.000 </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
           <t>105.435.0040.000</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 01         0 AREA APM 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 09</t>
-        </is>
-      </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 10355.84, 'Juros': 466.0, 'Multa': 1216.83, 'Total': '12038.67', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 10355.86, 'Juros': 1656.94, 'Multa': 2071.17, 'Total': '14083.97', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 26189.58}]</t>
         </is>
       </c>
     </row>
@@ -2156,24 +1985,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 02         0 APP 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 AREA APP01105.435.0205.000 </t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
           <t>105.435.0205.000</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 02         0 APP 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 AREA APP01</t>
-        </is>
-      </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 57764.8, 'Juros': 2599.42, 'Multa': 6787.37, 'Total': '67151.59', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 57764.79, 'Juros': 9242.37, 'Multa': 11552.96, 'Total': '78560.12', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 145778.65}]</t>
         </is>
       </c>
     </row>
@@ -2190,24 +2012,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 02         0 APM 10 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 10105.435.0399.000 </t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
           <t>105.435.0399.000</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Avenida CAMPOS DO JORDAO 02         0 APM 10 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 10</t>
-        </is>
-      </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 35508.8, 'Juros': 1597.9, 'Multa': 4172.29, 'Total': '41278.99', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 3.88, 'Multa': 4.85, 'Total': '33.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 35508.79, 'Juros': 5681.41, 'Multa': 7101.76, 'Total': '48291.96', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 89637.89}]</t>
         </is>
       </c>
     </row>
@@ -2224,24 +2039,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 01 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 01106.027.0012.000 </t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>106.027.0012.000</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 01 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 01</t>
-        </is>
-      </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 10.355,84 466,00 1.216,83 12.038,67 8 0
-10.382,36 468,12 1.222,13 12.072,61 TOTAL:
-Dívida Ativa Situação:
-2022 01 CIP - DA 24,27 3,88 4,85 33,00 1 0
-2022 01 ITU - DA 10.355,86 1.656,94 2.071,17 14.083,97 1 0
-10.380,13 1.660,82 2.076,02 14.116,97 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 286.24, 'Juros': 17.17, 'Multa': 57.25, 'Total': '360.66', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': 286.24, 'Juros': 14.31, 'Multa': 22.9, 'Total': '323.45', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 269.4, 'Juros': 29.63, 'Multa': 53.88, 'Total': '352.91', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1037.02}]</t>
         </is>
       </c>
     </row>
@@ -2258,23 +2066,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 27 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 27106.027.0407.000 </t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
           <t>106.027.0407.000</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 27 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 27</t>
-        </is>
-      </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '05', 'Tributo': 'Capinação e Roç', 'Valor Atual': 294.47, 'Juros': 14.72, 'Multa': 23.56, 'Total': '332.75', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 294.47, 'Juros': 17.67, 'Multa': 58.89, 'Total': '371.03', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 277.15, 'Juros': 30.49, 'Multa': 55.43, 'Total': '363.07', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1066.85}]</t>
         </is>
       </c>
     </row>
@@ -2291,23 +2093,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida AGLAIA DE ARAUJO         0 QD.04  LT.25 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 25106.029.0109.000 </t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
           <t>106.029.0109.000</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Avenida AGLAIA DE ARAUJO         0 QD.04  LT.25 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 25</t>
-        </is>
-      </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 12.24, 'Multa': 40.8, 'Total': '257.04', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.0, 'Juros': 21.12, 'Multa': 38.4, 'Total': '251.52', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.0, 'Juros': 21.12, 'Multa': 38.4, 'Total': '251.52', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 760.08}]</t>
         </is>
       </c>
     </row>
@@ -2324,23 +2120,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FC-07         0 QD.04  LT.03 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 03106.029.0244.000 </t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
           <t>106.029.0244.000</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Rua FC-07         0 QD.04  LT.03 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 03</t>
-        </is>
-      </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 273.36, 'Juros': 16.4, 'Multa': 54.67, 'Total': '344.43', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '08', 'Tributo': 'Capinação e Roç', 'Valor Atual': 273.36, 'Juros': 8.2, 'Multa': 21.87, 'Total': '303.43', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 257.28, 'Juros': 28.3, 'Multa': 51.46, 'Total': '337.04', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 257.28, 'Juros': 28.3, 'Multa': 51.46, 'Total': '337.04', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1321.94}]</t>
         </is>
       </c>
     </row>
@@ -2357,23 +2147,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FC-07         0 QD.04  LT.04 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 04106.029.0256.000 </t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
           <t>106.029.0256.000</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Rua FC-07         0 QD.04  LT.04 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 04</t>
-        </is>
-      </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 05 Capinação e Roç 294,47 14,72 23,56 332,75 1 0
-2023 02 Capinação e Roç 294,47 17,67 58,89 371,03 1 0
-588,94 32,39 82,45 703,78 TOTAL:
-Dívida Ativa Situação:
-2022 07 Capin. RoçaD.A 277,15 30,49 55,43 363,07 1 0
-277,15 30,49 55,43 363,07 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.68, 'Juros': 12.28, 'Multa': 40.94, 'Total': '257.90', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '08', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.68, 'Juros': 6.14, 'Multa': 16.37, 'Total': '227.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.64, 'Juros': 21.19, 'Multa': 38.53, 'Total': '252.36', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 737.45}]</t>
         </is>
       </c>
     </row>
@@ -2390,28 +2174,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FC-07         0 QD.05 LT. 26 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 05 26106.030.0393.000 </t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
           <t>106.030.0393.000</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Rua FC-07         0 QD.05 LT. 26 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 05 26</t>
-        </is>
-      </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1791.76, 'Juros': 80.64, 'Multa': 210.53, 'Total': '2082.93', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 244.95, 'Juros': 124.92, 'Multa': 48.99, 'Total': '418.86', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1614.2, 'Juros': 500.4, 'Multa': 322.84, 'Total': '2437.44', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1791.78, 'Juros': 358.36, 'Multa': 358.36, 'Total': '2508.50', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '10', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 1318.76, 'Juros': 617.43, 'Multa': 225.56, 'Total': '2161.75', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 9722.1}]</t>
         </is>
       </c>
     </row>
@@ -2428,28 +2201,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FC-15          S/N QD: 29 LT: 24 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 29 24106.054.0334.000 </t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
           <t>106.054.0334.000</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Rua FC-15          S/N QD: 29 LT: 24 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 29 24</t>
-        </is>
-      </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 622.2, 'Juros': 40.44, 'Multa': 105.77, 'Total': '768.41', 'Vencidas': 4, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 65.23, 'Juros': 5.22, 'Multa': 13.05, 'Total': '83.50', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 603.59, 'Juros': 187.11, 'Multa': 120.72, 'Total': '911.42', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 76.28, 'Juros': 23.64, 'Multa': 15.25, 'Total': '115.17', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 622.18, 'Juros': 124.44, 'Multa': 124.44, 'Total': '871.06', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 69.08, 'Juros': 13.81, 'Multa': 13.81, 'Total': '96.70', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2846.2599999999998}]</t>
         </is>
       </c>
     </row>
@@ -2466,28 +2228,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RA 02         0 QD. 04 LT. 21A RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21A107.488.0366.000 </t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
           <t>107.488.0366.000</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Rua RA 02         0 QD. 04 LT. 21A RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21A</t>
-        </is>
-      </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 178.88, 'Juros': 14.31, 'Multa': 35.78, 'Total': '228.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': 156.16, 'Juros': 0.0, 'Multa': 0.0, 'Total': '156.16', 'Vencidas': 0, 'A Vencer': 1}, {'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': 134.77, 'Juros': 0.0, 'Multa': 0.0, 'Total': '134.77', 'Vencidas': 0, 'A Vencer': 1}], 'Total Origem': 519.9}]</t>
         </is>
       </c>
     </row>
@@ -2504,28 +2255,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RA 02          -777 QD. 04 LT. 21C RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21C107.488.0390.002 </t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
           <t>107.488.0390.002</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Rua RA 02          -777 QD. 04 LT. 21C RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21C</t>
-        </is>
-      </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.791,76 80,64 210,53 2.082,93 8 0
-1.818,28 82,76 215,83 2.116,87 TOTAL:
-Dívida Ativa Situação:
-2019 02 Capin. RoçaD.A 244,95 124,92 48,99 418,86 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.614,20 500,40 322,84 2.437,44 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.791,78 358,36 358,36 2.508,50 1 0
-2022 10 Saldo Parc. D.A 1.318,76 617,43 225,56 2.161,75 1 0
-5.023,57 1.615,14 966,52 7.605,23 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 253.46, 'Juros': 20.28, 'Multa': 50.69, 'Total': '324.43', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 40.32, 'Juros': 3.23, 'Multa': 8.06, 'Total': '51.61', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 376.04}]</t>
         </is>
       </c>
     </row>
@@ -2542,20 +2282,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30107.533.0338.001 </t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
           <t>107.533.0338.001</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30</t>
-        </is>
-      </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 205.0, 'Juros': 41.0, 'Multa': 41.0, 'Total': '287.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 50.67, 'Juros': 10.14, 'Multa': 10.14, 'Total': '70.95', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 357.95}]</t>
         </is>
       </c>
     </row>
@@ -2572,20 +2309,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30107.533.0338.002 </t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
           <t>107.533.0338.002</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30</t>
-        </is>
-      </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 233.09, 'Juros': 46.62, 'Multa': 46.62, 'Total': '326.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 54.31, 'Juros': 10.86, 'Multa': 10.86, 'Total': '76.03', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 402.36}]</t>
         </is>
       </c>
     </row>
@@ -2602,20 +2336,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua ACACIA          S/N QD: 37 LT: 5-C JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 5-C107.539.0331.000 </t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
           <t>107.539.0331.000</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Rua ACACIA          S/N QD: 37 LT: 5-C JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 5-C</t>
-        </is>
-      </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 259.19, 'Juros': 20.74, 'Multa': 51.84, 'Total': '331.77', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 61.6, 'Juros': 4.93, 'Multa': 12.32, 'Total': '78.85', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2016', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 111.74, 'Juros': 102.8, 'Multa': 22.35, 'Total': '236.89', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 249.83, 'Juros': 199.87, 'Multa': 49.97, 'Total': '499.67', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 197.78, 'Juros': 158.22, 'Multa': 39.56, 'Total': '395.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 249.84, 'Juros': 169.89, 'Multa': 49.97, 'Total': '469.70', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 97.23, 'Juros': 66.12, 'Multa': 19.45, 'Total': '182.80', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 249.83, 'Juros': 77.45, 'Multa': 49.97, 'Total': '377.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 72.03, 'Juros': 22.33, 'Multa': 14.41, 'Total': '108.77', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 259.19, 'Juros': 51.84, 'Multa': 51.84, 'Total': '362.87', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 65.23, 'Juros': 13.05, 'Multa': 13.05, 'Total': '91.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 249.84, 'Juros': 139.91, 'Multa': 49.97, 'Total': '439.72', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 75.79, 'Juros': 42.44, 'Multa': 15.16, 'Total': '133.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 249.83, 'Juros': 109.93, 'Multa': 49.97, 'Total': '409.73', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 76.15, 'Juros': 33.51, 'Multa': 15.23, 'Total': '124.89', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4243.1900000000005}]</t>
         </is>
       </c>
     </row>
@@ -2632,20 +2363,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua ARAUCARIA         0 QD. 37 LT. 05B JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 05B107.539.0345.000 </t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
           <t>107.539.0345.000</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Rua ARAUCARIA         0 QD. 37 LT. 05B JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 05B</t>
-        </is>
-      </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Dívida Ativa Situação:
-2022 01 IPTU - DA 205,00 41,00 41,00 287,00 1 0
-2022 01 TSU - DA 50,67 10,14 10,14 70,95 1 0
-255,67 51,14 51,14 357,95 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 377.72, 'Juros': 28.33, 'Multa': 75.54, 'Total': '481.59', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 340.28, 'Juros': 105.49, 'Multa': 68.06, 'Total': '513.83', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 377.71, 'Juros': 75.54, 'Multa': 75.54, 'Total': '528.79', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1636.8300000000002}]</t>
         </is>
       </c>
     </row>
@@ -2662,28 +2390,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua ACACIA         0 QD. 45, LT. 15 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 15107.548.0027.000 </t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
           <t>107.548.0027.000</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Rua ACACIA         0 QD. 45, LT. 15 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 15</t>
-        </is>
-      </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 273.46, 'Juros': 20.51, 'Multa': 54.7, 'Total': '348.67', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 51.1, 'Juros': 4.09, 'Multa': 10.22, 'Total': '65.41', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 262.32, 'Juros': 81.32, 'Multa': 52.46, 'Total': '396.10', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 59.75, 'Juros': 18.52, 'Multa': 11.95, 'Total': '90.22', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 273.45, 'Juros': 54.69, 'Multa': 54.69, 'Total': '382.83', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 499.73, 'Juros': 350.98, 'Multa': 78.92, 'Total': '929.63', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 390.41, 'Juros': 181.05, 'Multa': 66.77, 'Total': '638.23', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 54.11, 'Juros': 10.82, 'Multa': 10.82, 'Total': '75.75', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2926.84}]</t>
         </is>
       </c>
     </row>
@@ -2700,28 +2417,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA 0 QD.45, LT.18 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 18107.548.0063.001 </t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
           <t>107.548.0063.001</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Avenida RAIMUNDO CARLOS SILVA 0 QD.45, LT.18 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 18</t>
-        </is>
-      </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 939.26, 'Juros': 46.96, 'Multa': 123.44, 'Total': '1109.66', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 156.76, 'Juros': 12.54, 'Multa': 31.35, 'Total': '200.65', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 288.65, 'Juros': 89.48, 'Multa': 57.73, 'Total': '435.86', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 98.23, 'Juros': 30.45, 'Multa': 19.65, 'Total': '148.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 939.24, 'Juros': 187.85, 'Multa': 187.85, 'Total': '1314.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 166.01, 'Juros': 33.2, 'Multa': 33.2, 'Total': '232.41', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3441.85}]</t>
         </is>
       </c>
     </row>
@@ -2738,28 +2444,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 19 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 19107.548.0077.001 </t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
           <t>107.548.0077.001</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 19 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 19</t>
-        </is>
-      </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 800.16, 'Juros': 44.01, 'Multa': 112.02, 'Total': '956.19', 'Vencidas': 6, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 164.23, 'Juros': 13.14, 'Multa': 32.85, 'Total': '210.22', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 320.85, 'Juros': 141.17, 'Multa': 64.17, 'Total': '526.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 90.0, 'Juros': 39.6, 'Multa': 18.0, 'Total': '147.60', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 666.79, 'Juros': 126.69, 'Multa': 133.36, 'Total': '926.84', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2767.04}]</t>
         </is>
       </c>
     </row>
@@ -2776,28 +2471,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA         0 QD. 45, LT. 21 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 21107.548.0109.000 </t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
           <t>107.548.0109.000</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Avenida RAIMUNDO CARLOS SILVA         0 QD. 45, LT. 21 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 21</t>
-        </is>
-      </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 273,46 20,51 54,70 348,67 2 0
-2023 01 TSU 51,10 4,09 10,22 65,41 1 0
-324,56 24,60 64,92 414,08 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 262,32 81,32 52,46 396,10 1 0
-2021 01 TSU - DA 59,75 18,52 11,95 90,22 1 0
-2022 01 IPTU - DA 273,45 54,69 54,69 382,83 1 0
-2022 03 Saldo Parc. D.A 499,73 350,98 78,92 929,63 1 0
-2022 03 Saldo Parc. D.A 390,41 181,05 66,77 638,23 1 0
-2022 01 TSU - DA 54,11 10,82 10,82 75,75 1 0
-1.539,77 697,38 275,61 2.512,76 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 193.19, 'Juros': 15.46, 'Multa': 38.64, 'Total': '247.29', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 69.3, 'Juros': 5.54, 'Multa': 13.86, 'Total': '88.70', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 335.99}]</t>
         </is>
       </c>
     </row>
@@ -2814,25 +2498,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 02 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 02107.548.0157.001 </t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
           <t>107.548.0157.001</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 02 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 02</t>
-        </is>
-      </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 578.72, 'Juros': 37.61, 'Multa': 98.39, 'Total': '714.72', 'Vencidas': 4, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 139.82, 'Juros': 11.19, 'Multa': 27.97, 'Total': '178.98', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 578.72, 'Juros': 115.74, 'Multa': 115.74, 'Total': '810.20', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 640.44, 'Juros': 372.02, 'Multa': 109.54, 'Total': '1122.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 148.07, 'Juros': 29.61, 'Multa': 29.61, 'Total': '207.29', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3033.19}]</t>
         </is>
       </c>
     </row>
@@ -2849,25 +2525,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RA 26         0 QD. 45, LT. 12 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 12107.548.0470.000 </t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
           <t>107.548.0470.000</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Rua RA 26         0 QD. 45, LT. 12 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 12</t>
-        </is>
-      </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 343.6, 'Juros': 25.77, 'Multa': 68.72, 'Total': '438.09', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 63.7, 'Juros': 5.1, 'Multa': 12.74, 'Total': '81.54', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 332.47, 'Juros': 226.08, 'Multa': 66.49, 'Total': '625.04', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 100.55, 'Juros': 68.37, 'Multa': 20.11, 'Total': '189.03', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 332.46, 'Juros': 186.18, 'Multa': 66.49, 'Total': '585.13', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 78.37, 'Juros': 43.89, 'Multa': 15.67, 'Total': '137.93', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 332.47, 'Juros': 146.29, 'Multa': 66.49, 'Total': '545.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 78.75, 'Juros': 34.65, 'Multa': 15.75, 'Total': '129.15', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 332.47, 'Juros': 103.07, 'Multa': 66.49, 'Total': '502.03', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 74.49, 'Juros': 23.09, 'Multa': 14.9, 'Total': '112.48', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 343.6, 'Juros': 68.72, 'Multa': 68.72, 'Total': '481.04', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 67.46, 'Juros': 13.49, 'Multa': 13.49, 'Total': '94.44', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3921.1499999999996}]</t>
         </is>
       </c>
     </row>
@@ -2884,25 +2552,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida PERIMETRAL 0 ANT.AREA PUBL. PARQUE RESIDENCIAL DAS FLORES, Qt.Qd.Lt.SubLt. 30A 04107.552.0235.001 </t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
           <t>107.552.0235.001</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Avenida PERIMETRAL 0 ANT.AREA PUBL. PARQUE RESIDENCIAL DAS FLORES, Qt.Qd.Lt.SubLt. 30A 04</t>
-        </is>
-      </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 396.99, 'Juros': 27.79, 'Multa': 79.41, 'Total': '504.19', 'Vencidas': 3, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 186.57, 'Juros': 14.93, 'Multa': 37.31, 'Total': '238.81', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 743.0}]</t>
         </is>
       </c>
     </row>
@@ -2919,25 +2579,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FLAMBOYANT 0 QD. 02 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 07107.587.0020.001 </t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
           <t>107.587.0020.001</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Rua FLAMBOYANT 0 QD. 02 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 07</t>
-        </is>
-      </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 578,72 37,61 98,39 714,72 4 0
-2023 01 TSU 139,82 11,19 27,97 178,98 1 0
-718,54 48,80 126,36 893,70 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 578,72 115,74 115,74 810,20 1 0
-2022 01 Saldo Parc. D.A 640,44 372,02 109,54 1.122,00 1 0
-2022 01 TSU - DA 148,07 29,61 29,61 207,29 1 0
-1.367,23 517,37 254,89 2.139,49 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 2676.4, 'Juros': 120.44, 'Multa': 314.46, 'Total': '3111.30', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 454.47, 'Juros': 31.81, 'Multa': 90.9, 'Total': '577.18', 'Vencidas': 3, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 1410.55, 'Juros': 437.27, 'Multa': 282.11, 'Total': '2129.93', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 215.28, 'Juros': 66.74, 'Multa': 43.06, 'Total': '325.08', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 2676.37, 'Juros': 535.27, 'Multa': 535.27, 'Total': '3746.91', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 481.27, 'Juros': 96.25, 'Multa': 96.25, 'Total': '673.77', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2016', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 1410.55, 'Juros': 1297.71, 'Multa': 282.11, 'Total': '2990.37', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2016', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 333.96, 'Juros': 307.25, 'Multa': 66.79, 'Total': '708.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 1410.55, 'Juros': 1128.44, 'Multa': 282.11, 'Total': '2821.10', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 591.08, 'Juros': 472.87, 'Multa': 118.22, 'Total': '1182.17', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 528.96, 'Juros': 333.24, 'Multa': 105.79, 'Total': '967.99', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 1410.55, 'Juros': 789.91, 'Multa': 282.11, 'Total': '2482.57', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 226.49, 'Juros': 126.84, 'Multa': 45.3, 'Total': '398.63', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 1410.55, 'Juros': 620.64, 'Multa': 282.11, 'Total': '2313.30', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 227.59, 'Juros': 100.14, 'Multa': 45.52, 'Total': '373.25', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 24801.55}]</t>
         </is>
       </c>
     </row>
@@ -2954,30 +2606,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FLAMBOYANT         0 QD. 02 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 06107.587.0062.000 </t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
           <t>107.587.0062.000</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Rua FLAMBOYANT         0 QD. 02 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 06</t>
-        </is>
-      </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 TOTAL:
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 TOTAL:
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1356.88, 'Juros': 61.06, 'Multa': 159.43, 'Total': '1577.37', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1222.4, 'Juros': 378.94, 'Multa': 244.48, 'Total': '1845.82', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1356.86, 'Juros': 271.37, 'Multa': 271.37, 'Total': '1899.60', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1222.41, 'Juros': 537.86, 'Multa': 244.48, 'Total': '2004.75', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 7493.41}]</t>
         </is>
       </c>
     </row>
@@ -2994,30 +2633,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua PAINEIRA         0 QD. 03 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 15107.588.0234.000 </t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
           <t>107.588.0234.000</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Rua PAINEIRA         0 QD. 03 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 15</t>
-        </is>
-      </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 TOTAL:
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 TOTAL:
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 974.68, 'Juros': 48.73, 'Multa': 128.11, 'Total': '1151.52', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 122.5, 'Juros': 9.8, 'Multa': 24.5, 'Total': '156.80', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '08', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': 1926.83, 'Juros': 0.0, 'Multa': 0.0, 'Total': '1926.83', 'Vencidas': 0, 'A Vencer': 13}, {'Ano': '2023', 'Mês': '08', 'Tributo': 'Parcelamento DA', 'Valor Atual': 1875.76, 'Juros': 0.0, 'Multa': 0.0, 'Total': '1875.76', 'Vencidas': 0, 'A Vencer': 13}], 'Total Origem': 5110.91}]</t>
         </is>
       </c>
     </row>
@@ -3034,30 +2660,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua FLAMBOYANT         0 QD. 03 LT. 22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 22107.588.0385.000 </t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
           <t>107.588.0385.000</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Rua FLAMBOYANT         0 QD. 03 LT. 22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 22</t>
-        </is>
-      </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.356,88 61,06 159,43 1.577,37 8 0
-1.383,40 63,18 164,73 1.611,31 TOTAL:
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.222,40 378,94 244,48 1.845,82 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.356,86 271,37 271,37 1.899,60 1 0
-2.633,14 664,34 526,62 3.824,10 TOTAL:
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.222,41 537,86 244,48 2.004,75 1 0
-1.254,88 552,15 250,97 2.058,00 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2020', 'Mês': '02', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 1220.61, 'Juros': 912.28, 'Multa': 192.76, 'Total': '2325.65', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2325.65}]</t>
         </is>
       </c>
     </row>
@@ -3074,20 +2687,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua AROEIRA         0 QD. 04A LT. 12 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 12107.589.0343.000 </t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
           <t>107.589.0343.000</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Rua AROEIRA         0 QD. 04A LT. 12 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 12</t>
-        </is>
-      </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': 254.32, 'Juros': 10.17, 'Multa': 20.35, 'Total': '284.84', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 254.32, 'Juros': 17.8, 'Multa': 50.86, 'Total': '322.98', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 607.8199999999999}]</t>
         </is>
       </c>
     </row>
@@ -3104,20 +2714,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JACARANDA         0 QD. 04A LT. 17 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 17107.589.0412.000 </t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
           <t>107.589.0412.000</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Rua JACARANDA         0 QD. 04A LT. 17 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 17</t>
-        </is>
-      </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 664.15, 'Juros': 39.85, 'Multa': 100.97, 'Total': '804.97', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 89.25, 'Juros': 7.14, 'Multa': 17.85, 'Total': '114.24', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 664.14, 'Juros': 132.83, 'Multa': 132.83, 'Total': '929.80', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 94.52, 'Juros': 18.9, 'Multa': 18.9, 'Total': '132.32', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1981.33}]</t>
         </is>
       </c>
     </row>
@@ -3134,20 +2741,17 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21107.589.0460.001 </t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
           <t>107.589.0460.001</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21</t>
-        </is>
-      </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 368.16, 'Juros': 27.62, 'Multa': 73.64, 'Total': '469.42', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 66.97, 'Juros': 5.36, 'Multa': 13.39, 'Total': '85.72', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': 836.4, 'Juros': 0.0, 'Multa': 0.0, 'Total': '836.40', 'Vencidas': 0, 'A Vencer': 6}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': 1146.61, 'Juros': 0.0, 'Multa': 0.0, 'Total': '1146.61', 'Vencidas': 0, 'A Vencer': 8}], 'Total Origem': 2538.1499999999996}]</t>
         </is>
       </c>
     </row>
@@ -3164,20 +2768,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21107.589.0460.002 </t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
           <t>107.589.0460.002</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21</t>
-        </is>
-      </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 434.34, 'Juros': 30.4, 'Multa': 86.88, 'Total': '551.62', 'Vencidas': 3, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 86.52, 'Juros': 6.92, 'Multa': 17.3, 'Total': '110.74', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 157.03, 'Juros': 29.84, 'Multa': 31.41, 'Total': '218.28', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 880.64}]</t>
         </is>
       </c>
     </row>
@@ -3194,20 +2795,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JACARANDA 0 Qd. 04A        Lt.22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 22107.589.0472.001 </t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
           <t>107.589.0472.001</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Rua JACARANDA 0 Qd. 04A        Lt.22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 22</t>
-        </is>
-      </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 254,32 10,17 20,35 284,84 1 0
-2023 02 Capinação e Roç 254,32 17,80 50,86 322,98 1 0
-508,64 27,97 71,21 607,82 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 969.43, 'Juros': 48.46, 'Multa': 127.42, 'Total': '1145.31', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 149.69, 'Juros': 11.98, 'Multa': 29.94, 'Total': '191.61', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': 1250.78, 'Juros': 0.0, 'Multa': 0.0, 'Total': '1250.78', 'Vencidas': 0, 'A Vencer': 9}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': 2285.47, 'Juros': 0.0, 'Multa': 0.0, 'Total': '2285.47', 'Vencidas': 0, 'A Vencer': 11}], 'Total Origem': 4873.17}]</t>
         </is>
       </c>
     </row>
@@ -3224,19 +2822,17 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MANGUEIRA         0 Qd. 05         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 07107.590.0107.000 </t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
           <t>107.590.0107.000</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Rua MANGUEIRA         0 Qd. 05         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 07</t>
-        </is>
-      </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Divida': [{'Ano': '2023', 'Mês': '09', 'Tributo': 'Parcelamento DA', 'Valor Atual': 170.92, 'Juros': 0.0, 'Multa': 0.0, 'Total': '170.92', 'Vencidas': 0, 'A Vencer': 1}], 'Total Origem': 170.92}]</t>
         </is>
       </c>
     </row>
@@ -3253,19 +2849,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua CAJU 0 QD. 05 LT. 18 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 18107.590.0267.001 </t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
           <t>107.590.0267.001</t>
         </is>
       </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Rua CAJU 0 QD. 05 LT. 18 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 18</t>
-        </is>
-      </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 50.19, 'Juros': 22.08, 'Multa': 10.04, 'Total': '82.31', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 82.31}]</t>
         </is>
       </c>
     </row>
@@ -3282,19 +2876,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JOAO FLORENTINO       361 Qd. 05 Lt. 19 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 19107.590.0305.000 </t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
           <t>107.590.0305.000</t>
         </is>
       </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>Rua JOAO FLORENTINO       361 Qd. 05 Lt. 19 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 19</t>
-        </is>
-      </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 50.19, 'Juros': 22.08, 'Multa': 10.04, 'Total': '82.31', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 82.31}]</t>
         </is>
       </c>
     </row>
@@ -3311,19 +2903,17 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA 0 Qd. 06         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 07107.591.0107.001 </t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
           <t>107.591.0107.001</t>
         </is>
       </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA 0 Qd. 06         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 07</t>
-        </is>
-      </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 817.44, 'Juros': 44.96, 'Multa': 114.45, 'Total': '976.85', 'Vencidas': 6, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 121.62, 'Juros': 9.73, 'Multa': 24.32, 'Total': '155.67', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 393.47, 'Juros': 173.13, 'Multa': 78.69, 'Total': '645.29', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '02', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 154.91, 'Juros': 113.24, 'Multa': 23.56, 'Total': '291.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '02', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 176.56, 'Juros': 113.38, 'Multa': 27.88, 'Total': '317.82', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 60.57, 'Juros': 26.65, 'Multa': 12.11, 'Total': '99.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 393.47, 'Juros': 121.98, 'Multa': 78.69, 'Total': '594.14', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 57.3, 'Juros': 17.76, 'Multa': 11.46, 'Total': '86.52', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 817.46, 'Juros': 163.49, 'Multa': 163.49, 'Total': '1144.44', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 128.8, 'Juros': 25.76, 'Multa': 25.76, 'Total': '180.32', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4492.09}]</t>
         </is>
       </c>
     </row>
@@ -3340,19 +2930,17 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA         0 QD. 06 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 10107.591.0143.000 </t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
           <t>107.591.0143.000</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA         0 QD. 06 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 10</t>
-        </is>
-      </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 336.12, 'Juros': 25.2, 'Multa': 67.22, 'Total': '428.54', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 42.7, 'Juros': 3.42, 'Multa': 8.54, 'Total': '54.66', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 483.20000000000005}]</t>
         </is>
       </c>
     </row>
@@ -3369,19 +2957,17 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua JACARANDA         0 QD. 07 LT. 02 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 02107.592.0047.000 </t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
           <t>107.592.0047.000</t>
         </is>
       </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Rua JACARANDA         0 QD. 07 LT. 02 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 02</t>
-        </is>
-      </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Dívida Parcelada Situação:
-2023 09 Parcelamento DA 170,92 0,00 0,00 170,92 0 1
-170,92 0,00 0,00 170,92 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 995.61, 'Juros': 49.78, 'Multa': 130.87, 'Total': '1176.26', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 995.61, 'Juros': 199.12, 'Multa': 199.12, 'Total': '1393.85', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcel. D. Corr', 'Valor Atual': 5533.53, 'Juros': 0.0, 'Multa': 0.0, 'Total': '5533.53', 'Vencidas': 0, 'A Vencer': 35}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcel. D. Corr', 'Valor Atual': 2216.33, 'Juros': 0.0, 'Multa': 0.0, 'Total': '2216.33', 'Vencidas': 0, 'A Vencer': 15}], 'Total Origem': 10387.88}]</t>
         </is>
       </c>
     </row>
@@ -3398,25 +2984,17 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua AROEIRA 0 QD. 07 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 07107.592.0107.001 </t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
           <t>107.592.0107.001</t>
         </is>
       </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Rua AROEIRA 0 QD. 07 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 07</t>
-        </is>
-      </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
-2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
-2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
-2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 962.71, 'Juros': 48.14, 'Multa': 126.53, 'Total': '1137.38', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 142.63, 'Juros': 11.41, 'Multa': 28.53, 'Total': '182.57', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 962.68, 'Juros': 192.54, 'Multa': 192.54, 'Total': '1347.76', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 392.2, 'Juros': 112.41, 'Multa': 23.38, 'Total': '527.99', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 151.04, 'Juros': 30.21, 'Multa': 30.21, 'Total': '211.46', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3407.16}]</t>
         </is>
       </c>
     </row>
@@ -3433,25 +3011,17 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA         0 QD. 08 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 07107.594.0075.000 </t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
           <t>107.594.0075.000</t>
         </is>
       </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA         0 QD. 08 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 07</t>
-        </is>
-      </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
-2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
-2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
-2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Divida': [{'Ano': '2023', 'Mês': '10', 'Tributo': 'Parcel. D. Corr', 'Valor Atual': 195.09, 'Juros': 0.0, 'Multa': 0.0, 'Total': '195.09', 'Vencidas': 0, 'A Vencer': 1}], 'Total Origem': 195.09}]</t>
         </is>
       </c>
     </row>
@@ -3468,25 +3038,17 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA 0 QD. 08 LT. 08 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 08107.594.0087.001 </t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
           <t>107.594.0087.001</t>
         </is>
       </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA 0 QD. 08 LT. 08 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 08</t>
-        </is>
-      </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 962,71 48,14 126,53 1.137,38 7 0
-2023 01 TSU 142,63 11,41 28,53 182,57 1 0
-1.105,34 59,55 155,06 1.319,95 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 962,68 192,54 192,54 1.347,76 1 0
-2022 04 Saldo Parc. D.A 392,20 112,41 23,38 527,99 1 0
-2022 01 TSU - DA 151,04 30,21 30,21 211,46 1 0
-1.505,92 335,16 246,13 2.087,21 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 754.5, 'Juros': 45.27, 'Multa': 114.68, 'Total': '914.45', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 131.75, 'Juros': 10.54, 'Multa': 26.35, 'Total': '168.64', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 404.97, 'Juros': 275.38, 'Multa': 80.99, 'Total': '761.34', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 81.76, 'Juros': 55.6, 'Multa': 16.35, 'Total': '153.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 404.97, 'Juros': 125.54, 'Multa': 80.99, 'Total': '611.50', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 60.57, 'Juros': 18.78, 'Multa': 12.11, 'Total': '91.46', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 754.51, 'Juros': 150.9, 'Multa': 150.9, 'Total': '1056.31', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 139.52, 'Juros': 27.9, 'Multa': 27.9, 'Total': '195.32', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 404.98, 'Juros': 323.98, 'Multa': 81.0, 'Total': '809.96', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '05', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 249.47, 'Juros': 222.34, 'Multa': 35.59, 'Total': '507.40', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 166.31, 'Juros': 133.05, 'Multa': 33.26, 'Total': '332.62', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 404.98, 'Juros': 226.79, 'Multa': 81.0, 'Total': '712.77', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 63.73, 'Juros': 35.69, 'Multa': 12.75, 'Total': '112.17', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 404.97, 'Juros': 178.19, 'Multa': 80.99, 'Total': '664.15', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 64.04, 'Juros': 28.18, 'Multa': 12.81, 'Total': '105.03', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 7196.829999999999}]</t>
         </is>
       </c>
     </row>
@@ -3503,20 +3065,17 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA         0 QD. 08 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 13107.594.0147.000 </t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
           <t>107.594.0147.000</t>
         </is>
       </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA         0 QD. 08 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 13</t>
-        </is>
-      </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 853.38, 'Juros': 46.94, 'Multa': 119.49, 'Total': '1019.81', 'Vencidas': 6, 'A Vencer': 0}], 'Total Origem': 1053.75}]</t>
         </is>
       </c>
     </row>
@@ -3533,20 +3092,17 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua IPE         0 QD. 08 LT. 14 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 14107.594.0183.000 </t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
           <t>107.594.0183.000</t>
         </is>
       </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Rua IPE         0 QD. 08 LT. 14 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 14</t>
-        </is>
-      </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': 238.0, 'Juros': 9.52, 'Multa': 19.04, 'Total': '266.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1194.72, 'Juros': 53.76, 'Multa': 140.4, 'Total': '1388.88', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '08', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 348.11, 'Juros': 107.91, 'Multa': 69.62, 'Total': '525.64', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '09', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 224.0, 'Juros': 24.64, 'Multa': 44.8, 'Total': '293.44', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1194.73, 'Juros': 238.95, 'Multa': 238.95, 'Total': '1672.63', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4215.0599999999995}]</t>
         </is>
       </c>
     </row>
@@ -3563,20 +3119,17 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua IPE         0 QD. 08 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 15107.594.0198.000 </t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
           <t>107.594.0198.000</t>
         </is>
       </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Rua IPE         0 QD. 08 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 15</t>
-        </is>
-      </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 682.0, 'Juros': 40.92, 'Multa': 103.66, 'Total': '826.58', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 79.17, 'Juros': 6.33, 'Multa': 15.83, 'Total': '101.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '12', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 196.44, 'Juros': 128.2, 'Multa': 31.02, 'Total': '355.66', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 660.79, 'Juros': 290.75, 'Multa': 132.16, 'Total': '1083.70', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 97.87, 'Juros': 43.06, 'Multa': 19.57, 'Total': '160.50', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2527.7700000000004}]</t>
         </is>
       </c>
     </row>
@@ -3593,20 +3146,17 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MANGUEIRA 0 QD. 08 LT. 24 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 24107.594.0329.001 </t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
           <t>107.594.0329.001</t>
         </is>
       </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>Rua MANGUEIRA 0 QD. 08 LT. 24 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 24</t>
-        </is>
-      </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 853,38 46,94 119,49 1.019,81 6 0
-879,90 49,06 124,79 1.053,75 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 1118.16, 'Juros': 50.32, 'Multa': 131.37, 'Total': '1299.85', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 135.79, 'Juros': 10.86, 'Multa': 27.16, 'Total': '173.81', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 633.06, 'Juros': 196.25, 'Multa': 126.61, 'Total': '955.92', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 92.25, 'Juros': 28.6, 'Multa': 18.45, 'Total': '139.30', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 1118.12, 'Juros': 223.62, 'Multa': 223.62, 'Total': '1565.36', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '08', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 337.57, 'Juros': 204.95, 'Multa': 57.74, 'Total': '600.26', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 143.8, 'Juros': 28.76, 'Multa': 28.76, 'Total': '201.32', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4935.82}]</t>
         </is>
       </c>
     </row>
@@ -3623,19 +3173,17 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MANGUEIRA         0 QD.9A  LT.01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 9A 01107.595.0163.000 </t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
           <t>107.595.0163.000</t>
         </is>
       </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Rua MANGUEIRA         0 QD.9A  LT.01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 9A 01</t>
-        </is>
-      </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 8.16, 'Multa': 16.32, 'Total': '228.48', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 228.48}]</t>
         </is>
       </c>
     </row>
@@ -3652,19 +3200,17 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA 0 QD. 11 LT. 04 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 04107.597.0039.001 </t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
           <t>107.597.0039.001</t>
         </is>
       </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA 0 QD. 11 LT. 04 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 04</t>
-        </is>
-      </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 703.7, 'Juros': 42.22, 'Multa': 106.97, 'Total': '852.89', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '11', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 2291.6, 'Juros': 1073.36, 'Multa': 458.31, 'Total': '3823.27', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 109.22, 'Juros': 8.74, 'Multa': 21.84, 'Total': '139.80', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2016', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 76.19, 'Juros': 70.09, 'Multa': 15.24, 'Total': '161.52', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4977.4800000000005}]</t>
         </is>
       </c>
     </row>
@@ -3681,19 +3227,17 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SIBIPIRUNA 0 Qd. 11         Lt.06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 06107.597.0063.001 </t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
           <t>107.597.0063.001</t>
         </is>
       </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Rua SIBIPIRUNA 0 Qd. 11         Lt.06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 06</t>
-        </is>
-      </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 603.8, 'Juros': 39.26, 'Multa': 102.65, 'Total': '745.71', 'Vencidas': 4, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 141.56, 'Juros': 11.32, 'Multa': 28.31, 'Total': '181.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 603.81, 'Juros': 120.76, 'Multa': 120.76, 'Total': '845.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 149.91, 'Juros': 29.98, 'Multa': 29.98, 'Total': '209.87', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1982.1}]</t>
         </is>
       </c>
     </row>
@@ -3710,19 +3254,17 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua LARANJEIRA         0 QD. 11 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 15107.597.0187.000 </t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
           <t>107.597.0187.000</t>
         </is>
       </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Rua LARANJEIRA         0 QD. 11 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 15</t>
-        </is>
-      </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 07 Capinação e Roç 204,00 8,16 16,32 228,48 1 0
-204,00 8,16 16,32 228,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1222.08, 'Juros': 55.0, 'Multa': 143.59, 'Total': '1420.67', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1100.93, 'Juros': 341.29, 'Multa': 220.19, 'Total': '1662.41', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1222.03, 'Juros': 244.41, 'Multa': 244.41, 'Total': '1710.85', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '08', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 882.91, 'Juros': 413.4, 'Multa': 151.01, 'Total': '1447.32', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '08', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 1232.22, 'Juros': 939.33, 'Multa': 191.88, 'Total': '2363.43', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 8717.3}]</t>
         </is>
       </c>
     </row>
@@ -3739,25 +3281,17 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MANGUEIRA 0 QD. 11 LT. 20 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 20107.597.0267.001 </t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
           <t>107.597.0267.001</t>
         </is>
       </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Rua MANGUEIRA 0 QD. 11 LT. 20 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 20</t>
-        </is>
-      </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 686.8, 'Juros': 41.2, 'Multa': 104.39, 'Total': '832.39', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 105.45, 'Juros': 8.44, 'Multa': 21.09, 'Total': '134.98', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 686.77, 'Juros': 137.35, 'Multa': 137.35, 'Total': '961.47', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '03', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 1125.88, 'Juros': 584.62, 'Multa': 192.56, 'Total': '1903.06', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 111.67, 'Juros': 22.33, 'Multa': 22.33, 'Total': '156.33', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3988.23}]</t>
         </is>
       </c>
     </row>
@@ -3774,25 +3308,17 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MANGUEIRA         0 Qd. 11         Lt.23 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 23107.597.0303.000 </t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
           <t>107.597.0303.000</t>
         </is>
       </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Rua MANGUEIRA         0 Qd. 11         Lt.23 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 23</t>
-        </is>
-      </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 640.04, 'Juros': 41.6, 'Multa': 108.8, 'Total': '790.44', 'Vencidas': 4, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 640.03, 'Juros': 128.01, 'Multa': 128.01, 'Total': '896.05', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1754.4}]</t>
         </is>
       </c>
     </row>
@@ -3809,25 +3335,17 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua EUCALYPTO         0 QD. 12 LT. 01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 01107.598.0013.000 </t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
           <t>107.598.0013.000</t>
         </is>
       </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Rua EUCALYPTO         0 QD. 12 LT. 01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 01</t>
-        </is>
-      </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 14.28, 'Multa': 40.8, 'Total': '259.08', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 8.16, 'Multa': 16.32, 'Total': '228.48', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 853.38, 'Juros': 46.94, 'Multa': 119.49, 'Total': '1019.81', 'Vencidas': 6, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '09', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.0, 'Juros': 21.12, 'Multa': 38.4, 'Total': '251.52', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '04', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 203.33, 'Juros': 26.43, 'Multa': 40.67, 'Total': '270.43', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.0, 'Juros': 21.12, 'Multa': 38.4, 'Total': '251.52', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 853.37, 'Juros': 170.67, 'Multa': 170.67, 'Total': '1194.71', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3543.4599999999996}]</t>
         </is>
       </c>
     </row>
@@ -3844,25 +3362,17 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua EUCALYPTO 0 QD. 12 LT. 03 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 03107.598.0037.001 </t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
           <t>107.598.0037.001</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Rua EUCALYPTO 0 QD. 12 LT. 03 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 03</t>
-        </is>
-      </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 686,80 41,20 104,39 832,39 5 0
-2023 01 TSU 105,45 8,44 21,09 134,98 1 0
-792,25 49,64 125,48 967,37 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 686,77 137,35 137,35 961,47 1 0
-2022 03 Saldo Parc. D.A 1.125,88 584,62 192,56 1.903,06 1 0
-2022 01 TSU - DA 111,67 22,33 22,33 156,33 1 0
-1.924,32 744,30 352,24 3.020,86 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 477.59, 'Juros': 210.14, 'Multa': 95.52, 'Total': '783.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 111.08, 'Juros': 48.87, 'Multa': 22.22, 'Total': '182.17', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 477.59, 'Juros': 148.05, 'Multa': 95.52, 'Total': '721.16', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 105.07, 'Juros': 32.57, 'Multa': 21.01, 'Total': '158.65', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 698.29, 'Juros': 139.66, 'Multa': 139.66, 'Total': '977.61', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 125.03, 'Juros': 25.01, 'Multa': 25.01, 'Total': '175.05', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2997.8900000000003}]</t>
         </is>
       </c>
     </row>
@@ -3879,24 +3389,17 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06107.598.0096.001 </t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
           <t>107.598.0096.001</t>
         </is>
       </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06</t>
-        </is>
-      </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 857.58, 'Juros': 47.17, 'Multa': 120.06, 'Total': '1024.81', 'Vencidas': 6, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 84.86, 'Juros': 6.79, 'Multa': 16.97, 'Total': '108.62', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 599.87, 'Juros': 119.97, 'Multa': 119.97, 'Total': '839.81', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 128.38, 'Juros': 25.68, 'Multa': 25.68, 'Total': '179.74', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2152.9799999999996}]</t>
         </is>
       </c>
     </row>
@@ -3913,24 +3416,17 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06107.598.0096.002 </t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
           <t>107.598.0096.002</t>
         </is>
       </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06</t>
-        </is>
-      </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 110.32, 'Juros': 8.83, 'Multa': 22.06, 'Total': '141.21', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 13.78, 'Juros': 1.1, 'Multa': 2.76, 'Total': '17.64', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 367.99, 'Juros': 73.6, 'Multa': 73.6, 'Total': '515.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 14.59, 'Juros': 2.92, 'Multa': 2.92, 'Total': '20.43', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 694.47}]</t>
         </is>
       </c>
     </row>
@@ -3947,24 +3443,17 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua LIMOEIRO         0 QD. 12 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 10107.598.0183.000 </t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
           <t>107.598.0183.000</t>
         </is>
       </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Rua LIMOEIRO         0 QD. 12 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 10</t>
-        </is>
-      </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '02', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 14.28, 'Multa': 40.8, 'Total': '259.08', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '09', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.0, 'Juros': 21.12, 'Multa': 38.4, 'Total': '251.52', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 192.0, 'Juros': 21.12, 'Multa': 38.4, 'Total': '251.52', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 762.12}]</t>
         </is>
       </c>
     </row>
@@ -3981,24 +3470,17 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua LARANJEIRA         0 QD. 13 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 13 15107.599.0262.000 </t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
           <t>107.599.0262.000</t>
         </is>
       </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Rua LARANJEIRA         0 QD. 13 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 13 15</t>
-        </is>
-      </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 857,58 47,17 120,06 1.024,81 6 0
-2023 01 TSU 84,86 6,79 16,97 108,62 1 0
-942,44 53,96 137,03 1.133,43 TOTAL:
-Dívida Ativa Situação:
-2022 01 IPTU - DA 599,87 119,97 119,97 839,81 1 0
-2022 01 TSU - DA 128,38 25,68 25,68 179,74 1 0
-728,25 145,65 145,65 1.019,55 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 715.2, 'Juros': 42.9, 'Multa': 108.71, 'Total': '866.81', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 89.95, 'Juros': 7.2, 'Multa': 17.99, 'Total': '115.14', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 685.51, 'Juros': 301.62, 'Multa': 137.1, 'Total': '1124.23', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 111.2, 'Juros': 48.93, 'Multa': 22.24, 'Total': '182.37', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 685.52, 'Juros': 212.51, 'Multa': 137.1, 'Total': '1035.13', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 105.18, 'Juros': 32.61, 'Multa': 21.04, 'Total': '158.83', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 715.2, 'Juros': 143.04, 'Multa': 143.04, 'Total': '1001.28', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 95.26, 'Juros': 19.05, 'Multa': 19.05, 'Total': '133.36', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4617.15}]</t>
         </is>
       </c>
     </row>
@@ -4015,34 +3497,17 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua LARANJEIRA 0 QD. 14 LT. 05 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 05107.600.0069.001 </t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
           <t>107.600.0069.001</t>
         </is>
       </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Rua LARANJEIRA 0 QD. 14 LT. 05 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 05</t>
-        </is>
-      </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 988.05, 'Juros': 49.4, 'Multa': 129.85, 'Total': '1167.30', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 172.55, 'Juros': 13.8, 'Multa': 34.51, 'Total': '220.86', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 293.93, 'Juros': 235.14, 'Multa': 58.79, 'Total': '587.86', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 155.07, 'Juros': 124.06, 'Multa': 31.01, 'Total': '310.14', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 293.93, 'Juros': 199.87, 'Multa': 58.79, 'Total': '552.59', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 76.24, 'Juros': 51.84, 'Multa': 15.25, 'Total': '143.33', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 293.93, 'Juros': 164.6, 'Multa': 58.79, 'Total': '517.32', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 59.42, 'Juros': 33.28, 'Multa': 11.88, 'Total': '104.58', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 293.93, 'Juros': 129.33, 'Multa': 58.79, 'Total': '482.05', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 59.71, 'Juros': 26.27, 'Multa': 11.94, 'Total': '97.92', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 293.94, 'Juros': 91.12, 'Multa': 58.79, 'Total': '443.85', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 56.48, 'Juros': 17.51, 'Multa': 11.3, 'Total': '85.29', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 988.04, 'Juros': 197.61, 'Multa': 197.61, 'Total': '1383.26', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 182.73, 'Juros': 36.55, 'Multa': 36.55, 'Total': '255.83', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 6352.18}]</t>
         </is>
       </c>
     </row>
@@ -4059,34 +3524,17 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua LARANJEIRA 0 QD. 14 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 13107.600.0184.003 </t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
           <t>107.600.0184.003</t>
         </is>
       </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Rua LARANJEIRA 0 QD. 14 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 13</t>
-        </is>
-      </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 377.06, 'Juros': 28.28, 'Multa': 75.42, 'Total': '480.76', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 56.37, 'Juros': 4.51, 'Multa': 11.27, 'Total': '72.15', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 296.16, 'Juros': 59.23, 'Multa': 59.23, 'Total': '414.62', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 85.28, 'Juros': 17.06, 'Multa': 17.06, 'Total': '119.40', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1086.93}]</t>
         </is>
       </c>
     </row>
@@ -4103,34 +3551,17 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua MANGUEIRA         0 QD.14  LT.28 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 28107.600.0422.000 </t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
           <t>107.600.0422.000</t>
         </is>
       </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Rua MANGUEIRA         0 QD.14  LT.28 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 28</t>
-        </is>
-      </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Parcelada', 'Divida': [{'Ano': '2023', 'Mês': '11', 'Tributo': 'Parcelamento DA', 'Valor Atual': 616.43, 'Juros': 0.0, 'Multa': 0.0, 'Total': '616.43', 'Vencidas': 0, 'A Vencer': 4}], 'Total Origem': 616.43}]</t>
         </is>
       </c>
     </row>
@@ -4147,34 +3578,17 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua 25         0 QD. 47 LT. 33 RESIDENCIAL VALE DO SOL 1º E 2º ETAPA, Qt.Qd.Lt.SubLt. 47 33107.663.0091.000 </t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
           <t>107.663.0091.000</t>
         </is>
       </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>Rua 25         0 QD. 47 LT. 33 RESIDENCIAL VALE DO SOL 1º E 2º ETAPA, Qt.Qd.Lt.SubLt. 47 33</t>
-        </is>
-      </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 988,05 49,40 129,85 1.167,30 7 0
-2023 01 TSU 172,55 13,80 34,51 220,86 1 0
-1.160,60 63,20 164,36 1.388,16 TOTAL:
-Dívida Ativa Situação:
-2017 01 IPTU - DA 293,93 235,14 58,79 587,86 1 0
-2017 01 TSU - DA 155,07 124,06 31,01 310,14 1 0
-2018 01 IPTU - DA 293,93 199,87 58,79 552,59 1 0
-2018 01 TSU - DA 76,24 51,84 15,25 143,33 1 0
-2019 01 IPTU - DA 293,93 164,60 58,79 517,32 1 0
-2019 01 TSU - DA 59,42 33,28 11,88 104,58 1 0
-2020 01 IPTU - DA 293,93 129,33 58,79 482,05 1 0
-2020 01 TSU - DA 59,71 26,27 11,94 97,92 1 0
-2021 01 IPTU - DA 293,94 91,12 58,79 443,85 1 0
-2021 01 TSU - DA 56,48 17,51 11,30 85,29 1 0
-2022 01 IPTU - DA 988,04 197,61 197,61 1.383,26 1 0
-2022 01 TSU - DA 182,73 36,55 36,55 255,83 1 0
-3.047,35 1.307,18 609,49 4.964,02 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 146.67, 'Juros': 5.87, 'Multa': 11.73, 'Total': '164.27', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 707.96, 'Juros': 219.47, 'Multa': 141.59, 'Total': '1069.02', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 83.77, 'Juros': 25.97, 'Multa': 16.75, 'Total': '126.49', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1359.78}]</t>
         </is>
       </c>
     </row>
@@ -4191,33 +3605,17 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
+          <t xml:space="preserve">Alameda RIO DE JANEIRO         0 QD. J LT. 1J SETOR INDUSTRIAL AEROPORTO, Qt.Qd.Lt.SubLt. J 1J201.224.0213.000 </t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
           <t>201.224.0213.000</t>
         </is>
       </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>Alameda RIO DE JANEIRO         0 QD. J LT. 1J SETOR INDUSTRIAL AEROPORTO, Qt.Qd.Lt.SubLt. J 1J</t>
-        </is>
-      </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
-2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 TOTAL:
-Dívida Ativa Situação:
-2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
-2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
-2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
-2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
-2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 TOTAL:
-Ajuizada Situação:
-2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
-2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
-2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
-2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 756.15, 'Juros': 45.37, 'Multa': 114.95, 'Total': '916.47', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 106.4, 'Juros': 8.51, 'Multa': 21.28, 'Total': '136.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '04', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 324.41, 'Juros': 228.77, 'Multa': 51.23, 'Total': '604.41', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 751.45, 'Juros': 232.95, 'Multa': 150.29, 'Total': '1134.69', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 124.42, 'Juros': 38.57, 'Multa': 24.88, 'Total': '187.87', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 756.13, 'Juros': 151.23, 'Multa': 151.23, 'Total': '1058.59', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 112.68, 'Juros': 22.54, 'Multa': 22.54, 'Total': '157.76', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 751.45, 'Juros': 420.81, 'Multa': 150.29, 'Total': '1322.55', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 130.9, 'Juros': 73.31, 'Multa': 26.18, 'Total': '230.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 751.45, 'Juros': 330.64, 'Multa': 150.29, 'Total': '1232.38', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 131.53, 'Juros': 57.88, 'Multa': 26.31, 'Total': '215.72', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 7197.020000000001}]</t>
         </is>
       </c>
     </row>
@@ -4234,33 +3632,17 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SC 9 S/N QD. 12 LT. 23 SETOR SANTA CLARA, Qt.Qd.Lt.SubLt. 12 23202.107.0243.001 </t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
           <t>202.107.0243.001</t>
         </is>
       </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>Rua SC 9 S/N QD. 12 LT. 23 SETOR SANTA CLARA, Qt.Qd.Lt.SubLt. 12 23</t>
-        </is>
-      </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
-2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 TOTAL:
-Dívida Ativa Situação:
-2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
-2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
-2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
-2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
-2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 TOTAL:
-Ajuizada Situação:
-2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
-2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
-2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
-2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 487.11, 'Juros': 34.1, 'Multa': 97.41, 'Total': '618.62', 'Vencidas': 3, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 112.64, 'Juros': 9.01, 'Multa': 22.53, 'Total': '144.18', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 167.63, 'Juros': 112.31, 'Multa': 33.53, 'Total': '313.47', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 335.26, 'Juros': 187.75, 'Multa': 67.05, 'Total': '590.06', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 94.73, 'Juros': 53.05, 'Multa': 18.95, 'Total': '166.73', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 335.26, 'Juros': 147.51, 'Multa': 67.05, 'Total': '549.82', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 95.19, 'Juros': 41.88, 'Multa': 19.04, 'Total': '156.11', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 335.26, 'Juros': 103.93, 'Multa': 67.05, 'Total': '506.24', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 90.04, 'Juros': 27.91, 'Multa': 18.01, 'Total': '135.96', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 487.11, 'Juros': 97.42, 'Multa': 97.42, 'Total': '681.95', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 119.29, 'Juros': 23.86, 'Multa': 23.86, 'Total': '167.01', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4030.1500000000005}]</t>
         </is>
       </c>
     </row>
@@ -4277,33 +3659,17 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RF-05         0 Qd. 07         Lt.07 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 07 07301.675.0112.000 </t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
           <t>301.675.0112.000</t>
         </is>
       </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>Rua RF-05         0 Qd. 07         Lt.07 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 07 07</t>
-        </is>
-      </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 756,15 45,37 114,95 916,47 5 0
-2023 01 TSU 106,40 8,51 21,28 136,19 1 0
-862,55 53,88 136,23 1.052,66 TOTAL:
-Dívida Ativa Situação:
-2020 04 Saldo Parc. D.A 324,41 228,77 51,23 604,41 1 0
-2021 01 IPTU - DA 751,45 232,95 150,29 1.134,69 1 0
-2021 01 TSU - DA 124,42 38,57 24,88 187,87 1 0
-2022 01 IPTU - DA 756,13 151,23 151,23 1.058,59 1 0
-2022 01 TSU - DA 112,68 22,54 22,54 157,76 1 0
-2.069,09 674,06 400,17 3.143,32 TOTAL:
-Ajuizada Situação:
-2019 01 IPTU - DA 751,45 420,81 150,29 1.322,55 1 0
-2019 01 TSU - DA 130,90 73,31 26,18 230,39 1 0
-2020 01 IPTU - DA 751,45 330,64 150,29 1.232,38 1 0
-2020 01 TSU - DA 131,53 57,88 26,31 215,72 1 0
-1.765,33 882,64 353,07 3.001,04 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '06', 'Tributo': 'Capinação e Roç', 'Valor Atual': 484.84, 'Juros': 19.39, 'Multa': 38.79, 'Total': '543.02', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': 484.84, 'Juros': 33.94, 'Multa': 96.97, 'Total': '615.75', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 483.24, 'Juros': 62.82, 'Multa': 96.65, 'Total': '642.71', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1801.48}]</t>
         </is>
       </c>
     </row>
@@ -4320,30 +3686,17 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RF-05         0 QD. 08 LT. 09 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 08 09301.676.0121.000 </t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
           <t>301.676.0121.000</t>
         </is>
       </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>Rua RF-05         0 QD. 08 LT. 09 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 08 09</t>
-        </is>
-      </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 TOTAL:
-Dívida Ativa Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 611,92 189,70 122,38 924,00 1 0
-2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 14.28, 'Multa': 40.8, 'Total': '259.08', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 679.25, 'Juros': 40.75, 'Multa': 103.25, 'Total': '823.25', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 611.92, 'Juros': 269.24, 'Multa': 122.38, 'Total': '1003.54', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 611.92, 'Juros': 189.7, 'Multa': 122.38, 'Total': '924.00', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 203.33, 'Juros': 26.43, 'Multa': 40.67, 'Total': '270.43', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 679.23, 'Juros': 135.85, 'Multa': 135.85, 'Total': '950.93', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4397.099999999999}]</t>
         </is>
       </c>
     </row>
@@ -4360,30 +3713,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida CONTORNO         0 QD.05 LT.22 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 22302.419.0219.000 </t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
           <t>302.419.0219.000</t>
         </is>
       </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>Avenida CONTORNO         0 QD.05 LT.22 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 22</t>
-        </is>
-      </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 TOTAL:
-Dívida Ativa Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 611,92 189,70 122,38 924,00 1 0
-2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 741.65, 'Juros': 44.5, 'Multa': 112.75, 'Total': '898.90', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 124.6, 'Juros': 9.97, 'Multa': 24.92, 'Total': '159.49', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 741.64, 'Juros': 148.33, 'Multa': 148.33, 'Total': '1038.30', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 131.95, 'Juros': 26.39, 'Multa': 26.39, 'Total': '184.73', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2281.4199999999996}]</t>
         </is>
       </c>
     </row>
@@ -4400,30 +3740,17 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua SAO PEDRO         0 QD.05 LT.24 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 24302.419.0243.000 </t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
           <t>302.419.0243.000</t>
         </is>
       </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>Rua SAO PEDRO         0 QD.05 LT.24 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 24</t>
-        </is>
-      </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 679,25 40,75 103,25 823,25 5 0
-909,77 57,15 149,35 1.116,27 TOTAL:
-Dívida Ativa Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 611,92 269,24 122,38 1.003,54 1 0
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 611,92 189,70 122,38 924,00 1 0
-2022 02 Capin. RoçaD.A 203,33 26,43 40,67 270,43 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 679,23 135,85 135,85 950,93 1 0
-2.192,75 649,54 438,54 3.280,83 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 224.5, 'Juros': 17.96, 'Multa': 44.9, 'Total': '287.36', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 46.2, 'Juros': 3.7, 'Multa': 9.24, 'Total': '59.14', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 216.69, 'Juros': 147.35, 'Multa': 43.34, 'Total': '407.38', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '05', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 468.49, 'Juros': 428.67, 'Multa': 71.23, 'Total': '968.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '05', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 236.42, 'Juros': 184.03, 'Multa': 35.95, 'Total': '456.40', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 72.92, 'Juros': 49.59, 'Multa': 14.58, 'Total': '137.09', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 216.68, 'Juros': 121.34, 'Multa': 43.34, 'Total': '381.36', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 56.84, 'Juros': 31.83, 'Multa': 11.37, 'Total': '100.04', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 216.68, 'Juros': 95.34, 'Multa': 43.34, 'Total': '355.36', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 57.11, 'Juros': 25.13, 'Multa': 11.42, 'Total': '93.66', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 216.68, 'Juros': 67.17, 'Multa': 43.34, 'Total': '327.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 54.02, 'Juros': 16.75, 'Multa': 10.8, 'Total': '81.57', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 224.5, 'Juros': 44.9, 'Multa': 44.9, 'Total': '314.30', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 48.93, 'Juros': 9.79, 'Multa': 9.79, 'Total': '68.51', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2009', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 44.0, 'Juros': 78.32, 'Multa': 8.8, 'Total': '131.12', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2009', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 168.92, 'Juros': 299.84, 'Multa': 33.78, 'Total': '502.54', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2010', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 42.75, 'Juros': 70.54, 'Multa': 8.55, 'Total': '121.84', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2010', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 100.85, 'Juros': 166.4, 'Multa': 20.17, 'Total': '287.42', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2011', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 174.46, 'Juros': 264.29, 'Multa': 34.88, 'Total': '473.63', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2011', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 78.99, 'Juros': 120.07, 'Multa': 15.8, 'Total': '214.86', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2012', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 187.05, 'Juros': 260.0, 'Multa': 37.41, 'Total': '484.46', 'Vencidas': 3, 'A Vencer': 0}, {'Ano': '2012', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 78.99, 'Juros': 110.58, 'Multa': 15.8, 'Total': '205.37', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2014', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 192.23, 'Juros': 223.0, 'Multa': 38.45, 'Total': '453.68', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2014', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 75.21, 'Juros': 87.24, 'Multa': 15.04, 'Total': '177.49', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 7090.160000000001}]</t>
         </is>
       </c>
     </row>
@@ -4440,26 +3767,17 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua ABADIANIA          S/N QD: 9 LT: 8 PARQUE CALIXTOPOLIS E II ETAPA, Qt.Qd.Lt.SubLt. 9 8306.009.0082.001 </t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
           <t>306.009.0082.001</t>
         </is>
       </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>Rua ABADIANIA          S/N QD: 9 LT: 8 PARQUE CALIXTOPOLIS E II ETAPA, Qt.Qd.Lt.SubLt. 9 8</t>
-        </is>
-      </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
-2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
-2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
-2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
-2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 290.52, 'Juros': 21.79, 'Multa': 58.1, 'Total': '370.41', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 76.09, 'Juros': 6.09, 'Multa': 15.22, 'Total': '97.40', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 288.47, 'Juros': 89.42, 'Multa': 57.69, 'Total': '435.58', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 88.98, 'Juros': 27.58, 'Multa': 17.8, 'Total': '134.36', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 290.52, 'Juros': 58.1, 'Multa': 58.1, 'Total': '406.72', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 80.58, 'Juros': 16.12, 'Multa': 16.12, 'Total': '112.82', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1557.29}]</t>
         </is>
       </c>
     </row>
@@ -4476,26 +3794,17 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-02         0 QD. 02 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 02 10401.527.0142.000 </t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
           <t>401.527.0142.000</t>
         </is>
       </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>Rua RJ-02         0 QD. 02 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 02 10</t>
-        </is>
-      </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
-2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
-2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
-2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
-2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 211.38, 'Juros': 29.59, 'Multa': 42.28, 'Total': '283.25', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 283.25}]</t>
         </is>
       </c>
     </row>
@@ -4512,26 +3821,17 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-14         0 QD- 04 LT- 05 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 04 05401.529.0058.000 </t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
           <t>401.529.0058.000</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>Rua RJ-14         0 QD- 04 LT- 05 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 04 05</t>
-        </is>
-      </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 IPTU 290,52 21,79 58,10 370,41 2 0
-2023 01 TSU 76,09 6,09 15,22 97,40 1 0
-366,61 27,88 73,32 467,81 TOTAL:
-Dívida Ativa Situação:
-2021 01 IPTU - DA 288,47 89,42 57,69 435,58 1 0
-2021 01 TSU - DA 88,98 27,58 17,80 134,36 1 0
-2022 01 IPTU - DA 290,52 58,10 58,10 406,72 1 0
-2022 01 TSU - DA 80,58 16,12 16,12 112,82 1 0
-748,55 191,22 149,71 1.089,48 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '04', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.59, 'Juros': 10.23, 'Multa': 16.37, 'Total': '231.19', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.59, 'Juros': 14.32, 'Multa': 40.92, 'Total': '259.83', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1024.38, 'Juros': 51.22, 'Multa': 134.65, 'Total': '1210.25', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 922.84, 'Juros': 286.08, 'Multa': 184.57, 'Total': '1393.49', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 203.92, 'Juros': 28.55, 'Multa': 40.78, 'Total': '273.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1024.35, 'Juros': 204.87, 'Multa': 204.87, 'Total': '1434.09', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 65.64, 'Juros': 52.51, 'Multa': 13.13, 'Total': '131.28', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 922.84, 'Juros': 738.27, 'Multa': 184.57, 'Total': '1845.68', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 50.83, 'Juros': 34.56, 'Multa': 10.17, 'Total': '95.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 922.84, 'Juros': 627.53, 'Multa': 184.57, 'Total': '1734.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '04', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 205.75, 'Juros': 113.16, 'Multa': 41.15, 'Total': '360.06', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 36.02, 'Juros': 20.17, 'Multa': 7.2, 'Total': '63.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 922.84, 'Juros': 516.79, 'Multa': 184.57, 'Total': '1624.20', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 922.84, 'Juros': 406.05, 'Multa': 184.57, 'Total': '1513.46', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 12336.54}]</t>
         </is>
       </c>
     </row>
@@ -4548,26 +3848,17 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-02         0 QD.08 LT. 09 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 09401.533.0191.000 </t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
           <t>401.533.0191.000</t>
         </is>
       </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>Rua RJ-02         0 QD.08 LT. 09 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 09</t>
-        </is>
-      </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': 204.0, 'Juros': 14.28, 'Multa': 40.8, 'Total': '259.08', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1021.37, 'Juros': 51.07, 'Multa': 134.22, 'Total': '1206.66', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 203.33, 'Juros': 28.47, 'Multa': 40.67, 'Total': '272.47', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1021.38, 'Juros': 204.28, 'Multa': 204.28, 'Total': '1429.94', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 3236.0600000000004}]</t>
         </is>
       </c>
     </row>
@@ -4584,26 +3875,17 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
+          <t xml:space="preserve">Avenida FRANCISCO FONTES         0 QD.08 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 10401.533.0236.000 </t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
           <t>401.533.0236.000</t>
         </is>
       </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>Avenida FRANCISCO FONTES         0 QD.08 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 10</t>
-        </is>
-      </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': 267.8, 'Juros': 18.75, 'Multa': 53.56, 'Total': '340.11', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1608.96, 'Juros': 72.4, 'Multa': 189.04, 'Total': '1870.40', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelam/Div/Aj', 'Valor Atual': 1312.75, 'Juros': 0.0, 'Multa': 0.0, 'Total': '1312.75', 'Vencidas': 0, 'A Vencer': 5}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': 3160.92, 'Juros': 0.0, 'Multa': 0.0, 'Total': '3160.92', 'Vencidas': 0, 'A Vencer': 11}], 'Total Origem': 6718.120000000001}]</t>
         </is>
       </c>
     </row>
@@ -4620,26 +3902,17 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-02          S/N QD: 09 LT: 04 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 04401.534.0128.001 </t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
           <t>401.534.0128.001</t>
         </is>
       </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>Rua RJ-02          S/N QD: 09 LT: 04 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 04</t>
-        </is>
-      </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 1362.16, 'Juros': 61.3, 'Multa': 160.04, 'Total': '1583.50', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 120.15, 'Juros': 9.61, 'Multa': 24.03, 'Total': '153.79', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1737.29}]</t>
         </is>
       </c>
     </row>
@@ -4656,26 +3929,17 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-02         0 QD- 09 LT- 03 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 03401.534.0140.000 </t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
           <t>401.534.0140.000</t>
         </is>
       </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>Rua RJ-02         0 QD- 09 LT- 03 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 03</t>
-        </is>
-      </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '04', 'Tributo': 'Capinação e Roç', 'Valor Atual': 221.46, 'Juros': 11.07, 'Multa': 17.72, 'Total': '250.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1108.8, 'Juros': 49.9, 'Multa': 130.29, 'Total': '1288.99', 'Vencidas': 8, 'A Vencer': 0}], 'Total Origem': 1573.18}]</t>
         </is>
       </c>
     </row>
@@ -4692,26 +3956,17 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-07         0 QD14 LT02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 02401.537.0018.000 </t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
           <t>401.537.0018.000</t>
         </is>
       </c>
-      <c r="D131" t="inlineStr">
-        <is>
-          <t>Rua RJ-07         0 QD14 LT02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 02</t>
-        </is>
-      </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 204,00 14,28 40,80 259,08 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-1.251,89 67,47 180,32 1.499,68 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.021,38 204,28 204,28 1.429,94 1 0
-1.248,98 237,60 249,80 1.736,38 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 735.4, 'Juros': 44.12, 'Multa': 111.8, 'Total': '891.32', 'Vencidas': 5, 'A Vencer': 0}], 'Total Origem': 925.26}]</t>
         </is>
       </c>
     </row>
@@ -4728,23 +3983,17 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-09         0 QD14 LT19 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 19401.537.0274.000 </t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
           <t>401.537.0274.000</t>
         </is>
       </c>
-      <c r="D132" t="inlineStr">
-        <is>
-          <t>Rua RJ-09         0 QD14 LT19 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 19</t>
-        </is>
-      </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 898.8, 'Juros': 49.43, 'Multa': 125.82, 'Total': '1074.05', 'Vencidas': 6, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 203.33, 'Juros': 28.47, 'Multa': 40.67, 'Total': '272.47', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 1380.46}]</t>
         </is>
       </c>
     </row>
@@ -4761,23 +4010,17 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-09          S/N QD: 13 LT: 01 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 01401.538.0006.001 </t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
           <t>401.538.0006.001</t>
         </is>
       </c>
-      <c r="D133" t="inlineStr">
-        <is>
-          <t>Rua RJ-09          S/N QD: 13 LT: 01 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 01</t>
-        </is>
-      </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 687.65, 'Juros': 41.26, 'Multa': 104.53, 'Total': '833.44', 'Vencidas': 5, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 63.74, 'Juros': 5.1, 'Multa': 12.75, 'Total': '81.59', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 65.64, 'Juros': 52.51, 'Multa': 13.13, 'Total': '131.28', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 668.38, 'Juros': 207.2, 'Multa': 133.68, 'Total': '1009.26', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 74.53, 'Juros': 23.11, 'Multa': 14.91, 'Total': '112.55', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 687.64, 'Juros': 137.53, 'Multa': 137.53, 'Total': '962.70', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 67.5, 'Juros': 13.5, 'Multa': 13.5, 'Total': '94.50', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 50.83, 'Juros': 34.56, 'Multa': 10.17, 'Total': '95.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 950.29, 'Juros': 646.2, 'Multa': 190.06, 'Total': '1786.55', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 36.02, 'Juros': 20.17, 'Multa': 7.2, 'Total': '63.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 950.29, 'Juros': 532.16, 'Multa': 190.06, 'Total': '1672.51', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 950.29, 'Juros': 418.13, 'Multa': 190.06, 'Total': '1558.48', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 8455.060000000001}]</t>
         </is>
       </c>
     </row>
@@ -4794,23 +4037,17 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-09          S/N QD: 13 LT: 02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 02401.538.0018.001 </t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
           <t>401.538.0018.001</t>
         </is>
       </c>
-      <c r="D134" t="inlineStr">
-        <is>
-          <t>Rua RJ-09          S/N QD: 13 LT: 02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 02</t>
-        </is>
-      </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 898,80 49,43 125,82 1.074,05 6 0
-925,32 51,55 131,12 1.107,99 TOTAL:
-Dívida Ativa Situação:
-2022 02 Capin. RoçaD.A 203,33 28,47 40,67 272,47 1 0
-203,33 28,47 40,67 272,47 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 266.6, 'Juros': 19.99, 'Multa': 53.32, 'Total': '339.91', 'Vencidas': 2, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 14.0, 'Juros': 1.12, 'Multa': 2.8, 'Total': '17.92', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 248.38, 'Juros': 77.0, 'Multa': 49.68, 'Total': '375.06', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 16.37, 'Juros': 5.07, 'Multa': 3.27, 'Total': '24.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 266.59, 'Juros': 53.32, 'Multa': 53.32, 'Total': '373.23', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 14.83, 'Juros': 2.97, 'Multa': 2.97, 'Total': '20.77', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 65.64, 'Juros': 52.51, 'Multa': 13.13, 'Total': '131.28', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2017', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 662.51, 'Juros': 530.01, 'Multa': 132.5, 'Total': '1325.02', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 50.83, 'Juros': 34.56, 'Multa': 10.17, 'Total': '95.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 662.52, 'Juros': 450.51, 'Multa': 132.5, 'Total': '1245.53', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 36.02, 'Juros': 20.17, 'Multa': 7.2, 'Total': '63.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 662.51, 'Juros': 371.01, 'Multa': 132.5, 'Total': '1166.02', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 662.52, 'Juros': 291.51, 'Multa': 132.5, 'Total': '1086.53', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 6318.179999999999}]</t>
         </is>
       </c>
     </row>
@@ -4827,21 +4064,17 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-12         0 QD- 16 LT- 23 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 16 23401.541.0319.000 </t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
           <t>401.541.0319.000</t>
         </is>
       </c>
-      <c r="D135" t="inlineStr">
-        <is>
-          <t>Rua RJ-12         0 QD- 16 LT- 23 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 16 23</t>
-        </is>
-      </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1021.37, 'Juros': 51.07, 'Multa': 134.22, 'Total': '1206.66', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '12', 'Tributo': 'Parcelamento DA', 'Valor Atual': 897.02, 'Juros': 0.0, 'Multa': 0.0, 'Total': '897.02', 'Vencidas': 0, 'A Vencer': 2}], 'Total Origem': 2137.62}]</t>
         </is>
       </c>
     </row>
@@ -4858,21 +4091,17 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua RJ-14         0 QD.17 LT. 25 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 17 25401.542.0348.000 </t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
           <t>401.542.0348.000</t>
         </is>
       </c>
-      <c r="D136" t="inlineStr">
-        <is>
-          <t>Rua RJ-14         0 QD.17 LT. 25 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 17 25</t>
-        </is>
-      </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1021.37, 'Juros': 51.07, 'Multa': 134.22, 'Total': '1206.66', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '05', 'Tributo': 'Saldo Parc. DCC', 'Valor Atual': 813.27, 'Juros': 138.82, 'Multa': 121.78, 'Total': '1073.87', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2314.4700000000003}]</t>
         </is>
       </c>
     </row>
@@ -4889,21 +4118,17 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua ANTONIO DE SOUZA FRANÇA         0 QD.01 LT- 04 RESIDENCIAL PARIS, Qt.Qd.Lt.SubLt. 01 04403.316.0153.000 </t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
           <t>403.316.0153.000</t>
         </is>
       </c>
-      <c r="D137" t="inlineStr">
-        <is>
-          <t>Rua ANTONIO DE SOUZA FRANÇA         0 QD.01 LT- 04 RESIDENCIAL PARIS, Qt.Qd.Lt.SubLt. 01 04</t>
-        </is>
-      </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 588.6, 'Juros': 38.26, 'Multa': 100.06, 'Total': '726.92', 'Vencidas': 4, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 67.34, 'Juros': 5.39, 'Multa': 13.47, 'Total': '86.20', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 813.12}]</t>
         </is>
       </c>
     </row>
@@ -4920,21 +4145,17 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua 02 S/N QD. 01 LT.08 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 01 08404.002.0152.001 </t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
           <t>404.002.0152.001</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr">
-        <is>
-          <t>Rua 02 S/N QD. 01 LT.08 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 01 08</t>
-        </is>
-      </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.021,37 51,07 134,22 1.206,66 7 0
-2023 12 Parcelamento DA 897,02 0,00 0,00 897,02 0 2
-1.944,91 53,19 139,52 2.137,62 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1171.73, 'Juros': 363.24, 'Multa': 234.35, 'Total': '1769.32', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 681.63, 'Juros': 136.33, 'Multa': 136.33, 'Total': '954.29', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 156.2, 'Juros': 31.24, 'Multa': 31.24, 'Total': '218.68', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 50.83, 'Juros': 34.56, 'Multa': 10.17, 'Total': '95.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2018', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1171.74, 'Juros': 796.78, 'Multa': 234.35, 'Total': '2202.87', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2019', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 36.02, 'Juros': 20.17, 'Multa': 7.2, 'Total': '63.39', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1171.74, 'Juros': 515.57, 'Multa': 234.35, 'Total': '1921.66', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 7323.73}]</t>
         </is>
       </c>
     </row>
@@ -4951,26 +4172,17 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua 01         0 QD. 02 LT.03 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 02 03404.003.0106.000 </t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
           <t>404.003.0106.000</t>
         </is>
       </c>
-      <c r="D139" t="inlineStr">
-        <is>
-          <t>Rua 01         0 QD. 02 LT.03 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 02 03</t>
-        </is>
-      </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'Capinação e Roç', 'Valor Atual': 220.32, 'Juros': 15.42, 'Multa': 44.06, 'Total': '279.80', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '07', 'Tributo': 'Capinação e Roç', 'Valor Atual': 220.32, 'Juros': 6.61, 'Multa': 17.63, 'Total': '244.56', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1003.38, 'Juros': 50.17, 'Multa': 131.89, 'Total': '1185.44', 'Vencidas': 7, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '08', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 219.59, 'Juros': 26.35, 'Multa': 43.92, 'Total': '289.86', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 219.59, 'Juros': 30.74, 'Multa': 43.92, 'Total': '294.25', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2327.85}]</t>
         </is>
       </c>
     </row>
@@ -4987,26 +4199,17 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua 03         0 QD. 03 LT.04 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 03 04404.004.0116.000 </t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
           <t>404.004.0116.000</t>
         </is>
       </c>
-      <c r="D140" t="inlineStr">
-        <is>
-          <t>Rua 03         0 QD. 03 LT.04 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 03 04</t>
-        </is>
-      </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'IPTU', 'Valor Atual': 917.04, 'Juros': 50.44, 'Multa': 128.4, 'Total': '1095.88', 'Vencidas': 6, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'TSU', 'Valor Atual': 119.21, 'Juros': 9.54, 'Multa': 23.84, 'Total': '152.59', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 892.15, 'Juros': 276.57, 'Multa': 178.43, 'Total': '1347.15', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 139.4, 'Juros': 43.21, 'Multa': 27.88, 'Total': '210.49', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 917.01, 'Juros': 183.4, 'Multa': 183.4, 'Total': '1283.81', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 126.24, 'Juros': 25.25, 'Multa': 25.25, 'Total': '176.74', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 4266.66}]</t>
         </is>
       </c>
     </row>
@@ -5023,26 +4226,17 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua 01         0 A. NÃO EDIFICANTE RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 00 A. NÃO EDI404.007.0450.000 </t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
           <t>404.007.0450.000</t>
         </is>
       </c>
-      <c r="D141" t="inlineStr">
-        <is>
-          <t>Rua 01         0 A. NÃO EDIFICANTE RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 00 A. NÃO EDI</t>
-        </is>
-      </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 33.94}]</t>
         </is>
       </c>
     </row>
@@ -5059,26 +4253,17 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua ELIAS PAVLIKOFF         0 Qd. 01         Lt.14 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 01 14406.746.0243.000 </t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
           <t>406.746.0243.000</t>
         </is>
       </c>
-      <c r="D142" t="inlineStr">
-        <is>
-          <t>Rua ELIAS PAVLIKOFF         0 Qd. 01         Lt.14 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 01 14</t>
-        </is>
-      </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Ativa', 'Divida': [{'Ano': '2021', 'Mês': '01', 'Tributo': 'IPTU - DA', 'Valor Atual': 770.78, 'Juros': 238.94, 'Multa': 154.16, 'Total': '1163.88', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'TSU - DA', 'Valor Atual': 93.31, 'Juros': 28.93, 'Multa': 18.66, 'Total': '140.90', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '02', 'Tributo': 'Saldo Parc. D.A', 'Valor Atual': 444.29, 'Juros': 226.2, 'Multa': 75.99, 'Total': '746.48', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 2051.26}]</t>
         </is>
       </c>
     </row>
@@ -5095,26 +4280,17 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua HAGI         0 QD. 11 LT.05 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 11 05406.752.0076.000 </t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
           <t>406.752.0076.000</t>
         </is>
       </c>
-      <c r="D143" t="inlineStr">
-        <is>
-          <t>Rua HAGI         0 QD. 11 LT.05 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 11 05</t>
-        </is>
-      </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 Capinação e Roç 220,32 15,42 44,06 279,80 1 0
-2023 07 Capinação e Roç 220,32 6,61 17,63 244,56 1 0
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.003,38 50,17 131,89 1.185,44 7 0
-1.470,54 74,32 198,88 1.743,74 TOTAL:
-Dívida Ativa Situação:
-2022 08 Capin. RoçaD.A 219,59 26,35 43,92 289,86 1 0
-2022 01 Capin. RoçaD.A 219,59 30,74 43,92 294,25 1 0
-439,18 57,09 87,84 584,11 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1479.6, 'Juros': 66.6, 'Multa': 173.87, 'Total': '1720.07', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1333.0, 'Juros': 413.23, 'Multa': 266.6, 'Total': '2012.83', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1479.62, 'Juros': 295.92, 'Multa': 295.92, 'Total': '2071.46', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 5916.98}]</t>
         </is>
       </c>
     </row>
@@ -5131,31 +4307,17 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
+          <t xml:space="preserve">Rua TOMAS EDISON         0 Qd. 13         Lt.32 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 13 32406.753.0510.000 </t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
           <t>406.753.0510.000</t>
         </is>
       </c>
-      <c r="D144" t="inlineStr">
-        <is>
-          <t>Rua TOMAS EDISON         0 Qd. 13         Lt.32 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 13 32</t>
-        </is>
-      </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Dívida Corrente Situação:
-2023 01 CIP 26,52 2,12 5,30 33,94 1 0
-2023 01 ITU 1.683,92 75,76 197,87 1.957,55 8 0
-1.710,44 77,88 203,17 1.991,49 TOTAL:
-Dívida Ativa Situação:
-2021 01 CIP - DA 29,61 9,18 5,92 44,71 1 0
-2021 01 ITU - DA 1.517,01 470,27 303,40 2.290,68 1 0
-2022 07 Capin. RoçaD.A 216,32 23,80 43,26 283,38 1 0
-2022 01 CIP - DA 24,27 4,85 4,85 33,97 1 0
-2022 01 ITU - DA 1.683,88 336,78 336,78 2.357,44 1 0
-3.471,09 844,88 694,21 5.010,18 TOTAL:
-Ajuizada Situação:
-2020 01 CIP - DA 32,47 14,29 6,49 53,25 1 0
-2020 01 ITU - DA 1.517,01 667,48 303,40 2.487,89 1 0
-1.549,48 681,77 309,89 2.541,14 TOTAL:</t>
+          <t>[{'Situação': 'Dívida Corrente', 'Divida': [{'Ano': '2023', 'Mês': '01', 'Tributo': 'CIP', 'Valor Atual': 26.52, 'Juros': 2.12, 'Multa': 5.3, 'Total': '33.94', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2023', 'Mês': '01', 'Tributo': 'ITU', 'Valor Atual': 1683.92, 'Juros': 75.76, 'Multa': 197.87, 'Total': '1957.55', 'Vencidas': 8, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 29.61, 'Juros': 9.18, 'Multa': 5.92, 'Total': '44.71', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2021', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1517.01, 'Juros': 470.27, 'Multa': 303.4, 'Total': '2290.68', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '07', 'Tributo': 'Capin. RoçaD.A', 'Valor Atual': 216.32, 'Juros': 23.8, 'Multa': 43.26, 'Total': '283.38', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 24.27, 'Juros': 4.85, 'Multa': 4.85, 'Total': '33.97', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2022', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1683.88, 'Juros': 336.78, 'Multa': 336.78, 'Total': '2357.44', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'CIP - DA', 'Valor Atual': 32.47, 'Juros': 14.29, 'Multa': 6.49, 'Total': '53.25', 'Vencidas': 1, 'A Vencer': 0}, {'Ano': '2020', 'Mês': '01', 'Tributo': 'ITU - DA', 'Valor Atual': 1517.01, 'Juros': 667.48, 'Multa': 303.4, 'Total': '2487.89', 'Vencidas': 1, 'A Vencer': 0}], 'Total Origem': 9542.81}]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Regex de padrão de endereço
</commit_message>
<xml_diff>
--- a/prototipos/DataInput/Relatório.xlsx
+++ b/prototipos/DataInput/Relatório.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JOSE NETO PARANHOS         0 QD. 41 LT. 62 BAIRRO JUNDIAI, Qt.Qd.Lt.SubLt. 41 62101.165.0706.000 </t>
+          <t>Rua JOSE NETO PARANHOS         0 QD. 41 LT. 62 BAIRRO JUNDIAI, Qt.Qd.Lt.SubLt. 41 62</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida PB 1          S/N QD: 30 LT: 14 PARQUE BRASILIA I E II ETAPA, Qt.Qd.Lt.SubLt. 30 14104.063.0283.001 </t>
+          <t>Avenida PB 1          S/N QD: 30 LT: 14 PARQUE BRASILIA I E II ETAPA, Qt.Qd.Lt.SubLt. 30 14</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CEREJEIRAS         0 QD- 19 LT- 13 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 13104.433.0025.000 </t>
+          <t>Avenida CEREJEIRAS         0 QD- 19 LT- 13 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 13</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -554,7 +554,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CEREJEIRAS         0 QD- 19 LT- 12 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 12104.433.0041.000 </t>
+          <t>Avenida CEREJEIRAS         0 QD- 19 LT- 12 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 12</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CEREJEIRAS         0 QD- 19 LT- 11 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 11104.433.0057.000 </t>
+          <t>Avenida CEREJEIRAS         0 QD- 19 LT- 11 RESIDENCIAL CEREJEIRAS, Qt.Qd.Lt.SubLt. 19 11</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida UNIVERSITARIA      2045 SALA: 02 RESIDENCIAL ARAUJOVILLE, Qt.Qd.Lt.SubLt. 01 14/17105.279.0351.002 </t>
+          <t>Avenida UNIVERSITARIA      2045 SALA: 02 RESIDENCIAL ARAUJOVILLE, Qt.Qd.Lt.SubLt. 01 14/17</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -635,7 +635,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua TARSILA DO AMARAL         0 QD.13  LT.17 CONDOMÍNO RESIDENCIAL  BELAS ARTES, Qt.Qd.Lt.SubLt. 13 17105.322.0262.000 </t>
+          <t>Rua TARSILA DO AMARAL         0 QD.13  LT.17 CONDOMÍNO RESIDENCIAL  BELAS ARTES, Qt.Qd.Lt.SubLt. 13 17</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua GT 16         0 QD. 23 LT. 19 CONDOMÍNIO RESIDENCIAL GRAND TRIANON, Qt.Qd.Lt.SubLt. 23 19105.350.0307.000 </t>
+          <t>Rua GT 16         0 QD. 23 LT. 19 CONDOMÍNIO RESIDENCIAL GRAND TRIANON, Qt.Qd.Lt.SubLt. 23 19</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.02 LT. 14 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 14105.373.0166.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.02 LT. 14 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 14</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-18         0 QD.02 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 23105.373.0334.000 </t>
+          <t>Rua CJ-18         0 QD.02 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 23</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-18         0 QD.02 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 25105.373.0358.000 </t>
+          <t>Rua CJ-18         0 QD.02 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 02 25</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -770,7 +770,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CJ-02         0 QD.03 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 07105.374.0090.000 </t>
+          <t>Avenida CJ-02         0 QD.03 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 07</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-18         0 QD.03 LT. 24 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 24105.374.0330.000 </t>
+          <t>Rua CJ-18         0 QD.03 LT. 24 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 03 24</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida AV. CJ-01         0 QD.06 LT. 13 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 13105.377.0199.000 </t>
+          <t>Avenida AV. CJ-01         0 QD.06 LT. 13 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 13</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida AV. CJ-01         0 QD.06 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 16105.377.0235.000 </t>
+          <t>Avenida AV. CJ-01         0 QD.06 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 06 16</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -878,7 +878,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-06         0 QD.11 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 04105.382.0049.000 </t>
+          <t>Rua CJ-06         0 QD.11 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 04</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-06         0 QD.11 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 09105.382.0109.000 </t>
+          <t>Rua CJ-06         0 QD.11 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 09</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -932,7 +932,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-05         0 QD.11 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 16105.382.0235.000 </t>
+          <t>Rua CJ-05         0 QD.11 LT. 16 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 16</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -959,7 +959,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-05         0 QD.11 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 17105.382.0247.000 </t>
+          <t>Rua CJ-05         0 QD.11 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 11 17</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-06         0 QD.12 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 12 18105.383.0259.000 </t>
+          <t>Rua CJ-06         0 QD.12 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 12 18</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-11         0 QD.13 LT. 11 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 13 11105.384.0133.000 </t>
+          <t>Rua CJ-11         0 QD.13 LT. 11 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 13 11</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-14         0 QD.16 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 16 05105.387.0061.000 </t>
+          <t>Rua CJ-14         0 QD.16 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 16 05</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-15         0 QD.17 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 17 04105.388.0049.000 </t>
+          <t>Rua CJ-15         0 QD.17 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 17 04</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-15         0 QD.18 LT. 21 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 18 21105.389.0295.000 </t>
+          <t>Rua CJ-15         0 QD.18 LT. 21 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 18 21</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-17         0 QD.20 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 20 23105.391.0328.000 </t>
+          <t>Rua CJ-17         0 QD.20 LT. 23 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 20 23</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1148,7 +1148,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-22         0 QD.21 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 04105.392.0209.000 </t>
+          <t>Rua CJ-22         0 QD.21 LT. 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 04</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-22         0 QD.21 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 05105.392.0222.000 </t>
+          <t>Rua CJ-22         0 QD.21 LT. 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 05</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-22         0 QD.21 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 06105.392.0235.000 </t>
+          <t>Rua CJ-22         0 QD.21 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 21 06</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-24         0 QD.22 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 22 17105.393.0274.000 </t>
+          <t>Rua CJ-24         0 QD.22 LT. 17 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 22 17</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-24         0 QD.23 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 01105.394.0013.000 </t>
+          <t>Rua CJ-24         0 QD.23 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 01</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-25         0 QD.23 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 19105.394.0306.000 </t>
+          <t>Rua CJ-25         0 QD.23 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 23 19</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1310,7 +1310,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-14         0 QD. 25 LT. 15 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 25 15105.396.0223.000 </t>
+          <t>Rua CJ-14         0 QD. 25 LT. 15 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 25 15</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-13         0 QD.27 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 27 03105.398.0066.000 </t>
+          <t>Rua CJ-13         0 QD.27 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 27 03</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CJ-02         0 QD.34 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 34 09105.405.0165.000 </t>
+          <t>Avenida CJ-02         0 QD.34 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 34 09</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 18105.407.0274.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 18 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 18</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 19105.407.0289.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.36 LT. 19 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 36 19</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-25         0 QD.37 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 37 09105.408.0116.000 </t>
+          <t>Rua CJ-25         0 QD.37 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 37 09</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-25         0 QD.38 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 07105.409.0090.000 </t>
+          <t>Rua CJ-25         0 QD.38 LT. 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 07</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.38 LT. 33 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 33105.409.0458.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.38 LT. 33 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 38 33</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.40 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 40 25105.411.0358.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.40 LT. 25 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 40 25</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-25         0 QD.41 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 41 09105.412.0117.000 </t>
+          <t>Rua CJ-25         0 QD.41 LT. 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 41 09</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-26         0 QD.43 LT. 20 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 43 20105.414.0298.000 </t>
+          <t>Rua CJ-26         0 QD.43 LT. 20 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 43 20</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.47 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 47 01105.418.0015.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.47 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 47 01</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 QD.48 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 48 01105.419.0025.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 QD.48 LT. 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 48 01</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-29         0 QD.49 LT. 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 49 02105.420.0059.000 </t>
+          <t>Rua CJ-29         0 QD.49 LT. 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 49 02</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1688,7 +1688,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-30         0 QD.50 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 50 06105.421.0148.000 </t>
+          <t>Rua CJ-30         0 QD.50 LT. 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 50 06</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-35         0 QD.55 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 55 03105.426.0070.000 </t>
+          <t>Rua CJ-35         0 QD.55 LT. 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 55 03</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 APM 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 01105.427.0077.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 APM 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 01</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ - 08         0 APM 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 02105.428.0040.000 </t>
+          <t>Rua CJ - 08         0 APM 02 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 02</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ- 07         0 APM 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 03105.429.0040.000 </t>
+          <t>Rua CJ- 07         0 APM 03 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 03</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ - 08         0 APM 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 04105.430.0040.000 </t>
+          <t>Rua CJ - 08         0 APM 04 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 04</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ- 07         0 AREA APM 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 05105.431.0040.000 </t>
+          <t>Rua CJ- 07         0 AREA APM 05 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 05</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ-16         0 APM 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 06105.432.0109.000 </t>
+          <t>Rua CJ-16         0 APM 06 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 06</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1904,7 +1904,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ- 28         0 APM 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 07105.433.0073.000 </t>
+          <t>Rua CJ- 28         0 APM 07 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 07</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CJ- 20         0 AREA APM 08 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM08105.434.0030.000 </t>
+          <t>Rua CJ- 20         0 AREA APM 08 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM08</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1958,7 +1958,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 01         0 AREA APM 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 09105.435.0040.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 01         0 AREA APM 09 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 09</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 02         0 APP 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 AREA APP01105.435.0205.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 02         0 APP 01 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 AREA APP01</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CAMPOS DO JORDAO 02         0 APM 10 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 10105.435.0399.000 </t>
+          <t>Avenida CAMPOS DO JORDAO 02         0 APM 10 RESIDENCIAL CAMPOS DO JORDAO, Qt.Qd.Lt.SubLt. 00 APM 10</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 01 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 01106.027.0012.000 </t>
+          <t>Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 01 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 01</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 27 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 27106.027.0407.000 </t>
+          <t>Avenida AGLAIA DE ARAUJO         0 QD. 02 LT. 27 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 02 27</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida AGLAIA DE ARAUJO         0 QD.04  LT.25 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 25106.029.0109.000 </t>
+          <t>Avenida AGLAIA DE ARAUJO         0 QD.04  LT.25 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 25</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2120,7 +2120,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FC-07         0 QD.04  LT.03 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 03106.029.0244.000 </t>
+          <t>Rua FC-07         0 QD.04  LT.03 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 03</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FC-07         0 QD.04  LT.04 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 04106.029.0256.000 </t>
+          <t>Rua FC-07         0 QD.04  LT.04 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 04 04</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FC-07         0 QD.05 LT. 26 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 05 26106.030.0393.000 </t>
+          <t>Rua FC-07         0 QD.05 LT. 26 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 05 26</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FC-15          S/N QD: 29 LT: 24 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 29 24106.054.0334.000 </t>
+          <t>Rua FC-15          S/N QD: 29 LT: 24 RESIDENCIAL FLOR DO CERRADO 1ª e 2ª ETAPA, Qt.Qd.Lt.SubLt. 29 24</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RA 02         0 QD. 04 LT. 21A RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21A107.488.0366.000 </t>
+          <t>Rua RA 02         0 QD. 04 LT. 21A RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21A</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RA 02          -777 QD. 04 LT. 21C RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21C107.488.0390.002 </t>
+          <t>Rua RA 02          -777 QD. 04 LT. 21C RESIDENCIAL ARAGUAIA, Qt.Qd.Lt.SubLt. 04 21C</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30107.533.0338.001 </t>
+          <t>Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30107.533.0338.002 </t>
+          <t>Rua MOGNO 0 QD.31 LT.30 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 31 30</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua ACACIA          S/N QD: 37 LT: 5-C JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 5-C107.539.0331.000 </t>
+          <t>Rua ACACIA          S/N QD: 37 LT: 5-C JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 5-C</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua ARAUCARIA         0 QD. 37 LT. 05B JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 05B107.539.0345.000 </t>
+          <t>Rua ARAUCARIA         0 QD. 37 LT. 05B JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 37 05B</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua ACACIA         0 QD. 45, LT. 15 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 15107.548.0027.000 </t>
+          <t>Rua ACACIA         0 QD. 45, LT. 15 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 15</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA 0 QD.45, LT.18 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 18107.548.0063.001 </t>
+          <t>Avenida RAIMUNDO CARLOS SILVA 0 QD.45, LT.18 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 18</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 19 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 19107.548.0077.001 </t>
+          <t>Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 19 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 19</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA         0 QD. 45, LT. 21 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 21107.548.0109.000 </t>
+          <t>Avenida RAIMUNDO CARLOS SILVA         0 QD. 45, LT. 21 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 21</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2498,7 +2498,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 02 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 02107.548.0157.001 </t>
+          <t>Avenida RAIMUNDO CARLOS SILVA 0 QD. 45, LT. 02 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 02</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2525,7 +2525,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RA 26         0 QD. 45, LT. 12 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 12107.548.0470.000 </t>
+          <t>Rua RA 26         0 QD. 45, LT. 12 JARDIM DOS IPES, Qt.Qd.Lt.SubLt. 45 12</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida PERIMETRAL 0 ANT.AREA PUBL. PARQUE RESIDENCIAL DAS FLORES, Qt.Qd.Lt.SubLt. 30A 04107.552.0235.001 </t>
+          <t>Avenida PERIMETRAL 0 ANT.AREA PUBL. PARQUE RESIDENCIAL DAS FLORES, Qt.Qd.Lt.SubLt. 30A 04</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FLAMBOYANT 0 QD. 02 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 07107.587.0020.001 </t>
+          <t>Rua FLAMBOYANT 0 QD. 02 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 07</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FLAMBOYANT         0 QD. 02 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 06107.587.0062.000 </t>
+          <t>Rua FLAMBOYANT         0 QD. 02 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 02 06</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua PAINEIRA         0 QD. 03 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 15107.588.0234.000 </t>
+          <t>Rua PAINEIRA         0 QD. 03 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 15</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2660,7 +2660,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua FLAMBOYANT         0 QD. 03 LT. 22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 22107.588.0385.000 </t>
+          <t>Rua FLAMBOYANT         0 QD. 03 LT. 22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 03 22</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua AROEIRA         0 QD. 04A LT. 12 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 12107.589.0343.000 </t>
+          <t>Rua AROEIRA         0 QD. 04A LT. 12 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 12</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JACARANDA         0 QD. 04A LT. 17 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 17107.589.0412.000 </t>
+          <t>Rua JACARANDA         0 QD. 04A LT. 17 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 17</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21107.589.0460.001 </t>
+          <t>Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21107.589.0460.002 </t>
+          <t>Rua JACARANDA         0 QD. 04A LT. 21 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 21</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2795,7 +2795,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JACARANDA 0 Qd. 04A        Lt.22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 22107.589.0472.001 </t>
+          <t>Rua JACARANDA 0 Qd. 04A        Lt.22 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 04A 22</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2822,7 +2822,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MANGUEIRA         0 Qd. 05         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 07107.590.0107.000 </t>
+          <t>Rua MANGUEIRA         0 Qd. 05         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 07</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua CAJU 0 QD. 05 LT. 18 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 18107.590.0267.001 </t>
+          <t>Rua CAJU 0 QD. 05 LT. 18 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 18</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JOAO FLORENTINO       361 Qd. 05 Lt. 19 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 19107.590.0305.000 </t>
+          <t>Rua JOAO FLORENTINO       361 Qd. 05 Lt. 19 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 05 19</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA 0 Qd. 06         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 07107.591.0107.001 </t>
+          <t>Rua SIBIPIRUNA 0 Qd. 06         Lt.07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 07</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2930,7 +2930,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA         0 QD. 06 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 10107.591.0143.000 </t>
+          <t>Rua SIBIPIRUNA         0 QD. 06 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 06 10</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua JACARANDA         0 QD. 07 LT. 02 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 02107.592.0047.000 </t>
+          <t>Rua JACARANDA         0 QD. 07 LT. 02 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 02</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2984,7 +2984,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua AROEIRA 0 QD. 07 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 07107.592.0107.001 </t>
+          <t>Rua AROEIRA 0 QD. 07 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 07 07</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA         0 QD. 08 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 07107.594.0075.000 </t>
+          <t>Rua SIBIPIRUNA         0 QD. 08 LT. 07 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 07</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA 0 QD. 08 LT. 08 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 08107.594.0087.001 </t>
+          <t>Rua SIBIPIRUNA 0 QD. 08 LT. 08 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 08</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3065,7 +3065,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA         0 QD. 08 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 13107.594.0147.000 </t>
+          <t>Rua SIBIPIRUNA         0 QD. 08 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 13</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3092,7 +3092,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua IPE         0 QD. 08 LT. 14 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 14107.594.0183.000 </t>
+          <t>Rua IPE         0 QD. 08 LT. 14 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 14</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua IPE         0 QD. 08 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 15107.594.0198.000 </t>
+          <t>Rua IPE         0 QD. 08 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 15</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MANGUEIRA 0 QD. 08 LT. 24 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 24107.594.0329.001 </t>
+          <t>Rua MANGUEIRA 0 QD. 08 LT. 24 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 08 24</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MANGUEIRA         0 QD.9A  LT.01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 9A 01107.595.0163.000 </t>
+          <t>Rua MANGUEIRA         0 QD.9A  LT.01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 9A 01</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA 0 QD. 11 LT. 04 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 04107.597.0039.001 </t>
+          <t>Rua SIBIPIRUNA 0 QD. 11 LT. 04 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 04</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3227,7 +3227,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SIBIPIRUNA 0 Qd. 11         Lt.06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 06107.597.0063.001 </t>
+          <t>Rua SIBIPIRUNA 0 Qd. 11         Lt.06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 06</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3254,7 +3254,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua LARANJEIRA         0 QD. 11 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 15107.597.0187.000 </t>
+          <t>Rua LARANJEIRA         0 QD. 11 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 15</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MANGUEIRA 0 QD. 11 LT. 20 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 20107.597.0267.001 </t>
+          <t>Rua MANGUEIRA 0 QD. 11 LT. 20 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 20</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3308,7 +3308,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MANGUEIRA         0 Qd. 11         Lt.23 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 23107.597.0303.000 </t>
+          <t>Rua MANGUEIRA         0 Qd. 11         Lt.23 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 11 23</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3335,7 +3335,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua EUCALYPTO         0 QD. 12 LT. 01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 01107.598.0013.000 </t>
+          <t>Rua EUCALYPTO         0 QD. 12 LT. 01 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 01</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua EUCALYPTO 0 QD. 12 LT. 03 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 03107.598.0037.001 </t>
+          <t>Rua EUCALYPTO 0 QD. 12 LT. 03 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 03</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06107.598.0096.001 </t>
+          <t>Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06107.598.0096.002 </t>
+          <t>Rua EUCALYPTO         0 QD. 12 LT. 06 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 06</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua LIMOEIRO         0 QD. 12 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 10107.598.0183.000 </t>
+          <t>Rua LIMOEIRO         0 QD. 12 LT. 10 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 12 10</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3470,7 +3470,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua LARANJEIRA         0 QD. 13 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 13 15107.599.0262.000 </t>
+          <t>Rua LARANJEIRA         0 QD. 13 LT. 15 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 13 15</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua LARANJEIRA 0 QD. 14 LT. 05 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 05107.600.0069.001 </t>
+          <t>Rua LARANJEIRA 0 QD. 14 LT. 05 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 05</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3524,7 +3524,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua LARANJEIRA 0 QD. 14 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 13107.600.0184.003 </t>
+          <t>Rua LARANJEIRA 0 QD. 14 LT. 13 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 13</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3551,7 +3551,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua MANGUEIRA         0 QD.14  LT.28 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 28107.600.0422.000 </t>
+          <t>Rua MANGUEIRA         0 QD.14  LT.28 RESIDENCIAL PORTAL DO CERRADO, Qt.Qd.Lt.SubLt. 14 28</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua 25         0 QD. 47 LT. 33 RESIDENCIAL VALE DO SOL 1º E 2º ETAPA, Qt.Qd.Lt.SubLt. 47 33107.663.0091.000 </t>
+          <t>Rua 25         0 QD. 47 LT. 33 RESIDENCIAL VALE DO SOL 1º E 2º ETAPA, Qt.Qd.Lt.SubLt. 47 33</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3605,7 +3605,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alameda RIO DE JANEIRO         0 QD. J LT. 1J SETOR INDUSTRIAL AEROPORTO, Qt.Qd.Lt.SubLt. J 1J201.224.0213.000 </t>
+          <t>Alameda RIO DE JANEIRO         0 QD. J LT. 1J SETOR INDUSTRIAL AEROPORTO, Qt.Qd.Lt.SubLt. J 1J</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3632,7 +3632,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SC 9 S/N QD. 12 LT. 23 SETOR SANTA CLARA, Qt.Qd.Lt.SubLt. 12 23202.107.0243.001 </t>
+          <t>Rua SC 9 S/N QD. 12 LT. 23 SETOR SANTA CLARA, Qt.Qd.Lt.SubLt. 12 23</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RF-05         0 Qd. 07         Lt.07 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 07 07301.675.0112.000 </t>
+          <t>Rua RF-05         0 Qd. 07         Lt.07 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 07 07</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3686,7 +3686,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RF-05         0 QD. 08 LT. 09 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 08 09301.676.0121.000 </t>
+          <t>Rua RF-05         0 QD. 08 LT. 09 RESIDENCIAL FLORENCA, Qt.Qd.Lt.SubLt. 08 09</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida CONTORNO         0 QD.05 LT.22 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 22302.419.0219.000 </t>
+          <t>Avenida CONTORNO         0 QD.05 LT.22 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 22</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua SAO PEDRO         0 QD.05 LT.24 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 24302.419.0243.000 </t>
+          <t>Rua SAO PEDRO         0 QD.05 LT.24 PRACA C. RESIDENCIAL BELA VISTA, Qt.Qd.Lt.SubLt. 05 24</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3767,7 +3767,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua ABADIANIA          S/N QD: 9 LT: 8 PARQUE CALIXTOPOLIS E II ETAPA, Qt.Qd.Lt.SubLt. 9 8306.009.0082.001 </t>
+          <t>Rua ABADIANIA          S/N QD: 9 LT: 8 PARQUE CALIXTOPOLIS E II ETAPA, Qt.Qd.Lt.SubLt. 9 8</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-02         0 QD. 02 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 02 10401.527.0142.000 </t>
+          <t>Rua RJ-02         0 QD. 02 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 02 10</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-14         0 QD- 04 LT- 05 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 04 05401.529.0058.000 </t>
+          <t>Rua RJ-14         0 QD- 04 LT- 05 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 04 05</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-02         0 QD.08 LT. 09 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 09401.533.0191.000 </t>
+          <t>Rua RJ-02         0 QD.08 LT. 09 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 09</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t xml:space="preserve">Avenida FRANCISCO FONTES         0 QD.08 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 10401.533.0236.000 </t>
+          <t>Avenida FRANCISCO FONTES         0 QD.08 LT. 10 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 08 10</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-02          S/N QD: 09 LT: 04 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 04401.534.0128.001 </t>
+          <t>Rua RJ-02          S/N QD: 09 LT: 04 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 04</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-02         0 QD- 09 LT- 03 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 03401.534.0140.000 </t>
+          <t>Rua RJ-02         0 QD- 09 LT- 03 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 09 03</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-07         0 QD14 LT02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 02401.537.0018.000 </t>
+          <t>Rua RJ-07         0 QD14 LT02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 02</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-09         0 QD14 LT19 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 19401.537.0274.000 </t>
+          <t>Rua RJ-09         0 QD14 LT19 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 14 19</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-09          S/N QD: 13 LT: 01 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 01401.538.0006.001 </t>
+          <t>Rua RJ-09          S/N QD: 13 LT: 01 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 01</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-09          S/N QD: 13 LT: 02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 02401.538.0018.001 </t>
+          <t>Rua RJ-09          S/N QD: 13 LT: 02 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 13 02</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -4064,7 +4064,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-12         0 QD- 16 LT- 23 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 16 23401.541.0319.000 </t>
+          <t>Rua RJ-12         0 QD- 16 LT- 23 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 16 23</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua RJ-14         0 QD.17 LT. 25 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 17 25401.542.0348.000 </t>
+          <t>Rua RJ-14         0 QD.17 LT. 25 RESIDENCIAL RIO JORDÃO, Qt.Qd.Lt.SubLt. 17 25</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4118,7 +4118,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua ANTONIO DE SOUZA FRANÇA         0 QD.01 LT- 04 RESIDENCIAL PARIS, Qt.Qd.Lt.SubLt. 01 04403.316.0153.000 </t>
+          <t>Rua ANTONIO DE SOUZA FRANÇA         0 QD.01 LT- 04 RESIDENCIAL PARIS, Qt.Qd.Lt.SubLt. 01 04</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4145,7 +4145,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua 02 S/N QD. 01 LT.08 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 01 08404.002.0152.001 </t>
+          <t>Rua 02 S/N QD. 01 LT.08 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 01 08</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4172,7 +4172,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua 01         0 QD. 02 LT.03 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 02 03404.003.0106.000 </t>
+          <t>Rua 01         0 QD. 02 LT.03 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 02 03</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua 03         0 QD. 03 LT.04 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 03 04404.004.0116.000 </t>
+          <t>Rua 03         0 QD. 03 LT.04 RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 03 04</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua 01         0 A. NÃO EDIFICANTE RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 00 A. NÃO EDI404.007.0450.000 </t>
+          <t>Rua 01         0 A. NÃO EDIFICANTE RESIDENCIAL VALENCIA, Qt.Qd.Lt.SubLt. 00 A. NÃO EDI</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua ELIAS PAVLIKOFF         0 Qd. 01         Lt.14 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 01 14406.746.0243.000 </t>
+          <t>Rua ELIAS PAVLIKOFF         0 Qd. 01         Lt.14 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 01 14</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua HAGI         0 QD. 11 LT.05 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 11 05406.752.0076.000 </t>
+          <t>Rua HAGI         0 QD. 11 LT.05 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 11 05</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4307,7 +4307,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t xml:space="preserve">Rua TOMAS EDISON         0 Qd. 13         Lt.32 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 13 32406.753.0510.000 </t>
+          <t>Rua TOMAS EDISON         0 Qd. 13         Lt.32 RESIDENCIAL VILLA BELLA, Qt.Qd.Lt.SubLt. 13 32</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">

</xml_diff>